<commit_message>
Redone testcase 3 and 4 and done testcase 5
</commit_message>
<xml_diff>
--- a/TESTCASES/TestCases.xlsx
+++ b/TESTCASES/TestCases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andra\OneDrive - University of Greenwich\PhD\Application\ObjectController\TESTCASES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uogcloud-my.sharepoint.com/personal/mj4126n_gre_ac_uk/Documents/PhD/Application/ObjectController/TESTCASES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18352CE1-B835-4F67-B7F2-89796C74D3C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="8" documentId="13_ncr:1_{18352CE1-B835-4F67-B7F2-89796C74D3C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1B02510E-44D4-430E-9EBB-650C5B086219}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="241" uniqueCount="155">
   <si>
     <t>Vertices and attachment points are correct relative to CoR</t>
   </si>
@@ -234,13 +234,7 @@
     <t>Place object at one end of test region (offset to allow for acceleration), add goal at other end. Play simulation at 1s/s. Length travelled / time taken.</t>
   </si>
   <si>
-    <t>Rectangle_W1L10.csv</t>
-  </si>
-  <si>
     <t>SingleNode.csv</t>
-  </si>
-  <si>
-    <t>Graph of holonomicity vs time taken</t>
   </si>
   <si>
     <t>Visual confirmation + graph of num occupied nodes vs frequency (+ avg + SD)</t>
@@ -284,16 +278,10 @@
 CorridorWithRooms.csv</t>
   </si>
   <si>
-    <t>Place long, thin object (front is long edge) at one end of thin corridor so it cannot rotate. Add goal at other end of corridor. Test for different holonomicities. Should be able to move if holonomic, unable to move if non-holonomic and speed reduction if in between.</t>
-  </si>
-  <si>
     <t>Calculate freespace, look at each layer of C-Space and check the validities match the Minkowski sum of the object and boundaries</t>
   </si>
   <si>
     <t>Visual confirmation with overlay of Minkowski sum</t>
-  </si>
-  <si>
-    <t>LShape_W3L20x2 .csv</t>
   </si>
   <si>
     <t>Paths are generated following holonomicity</t>
@@ -378,9 +366,6 @@
   </si>
   <si>
     <t>Set tasks for people to pick up, move, then drop off object.</t>
-  </si>
-  <si>
-    <t>Make 2 versions of a square object, one holonomic and one non-holonomic. The holonomic one should have a path that does not rotate when going to the goal, the non-holonomic one should rotate.</t>
   </si>
   <si>
     <t>Test a couple of geometries with objects, people and stairs. Check geometries etc. match up</t>
@@ -518,7 +503,13 @@
     <t>Distance time graph with line of best fit (speed). Table of speeds for each geometry and object</t>
   </si>
   <si>
-    <t>Redo this</t>
+    <t>Make 3 versions of an object, fully holonomic, fully non-holonomic, in between. Send object to point behind it and look at the path it takes</t>
+  </si>
+  <si>
+    <t>Make different versions of test object with 1 in different places of holonomicity. Make object move to left and right, see what angle object is at when moves.</t>
+  </si>
+  <si>
+    <t>Frequency table of angles when moved</t>
   </si>
 </sst>
 </file>
@@ -1437,6 +1428,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1446,25 +1446,16 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1826,7 +1817,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L5" sqref="L5"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1863,23 +1854,23 @@
         <v>34</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="H1" s="33" t="s">
         <v>35</v>
       </c>
       <c r="I1" s="70" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="J1" s="71" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="87" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="84" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="12">
@@ -1895,7 +1886,7 @@
         <v>36</v>
       </c>
       <c r="G2" s="26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H2" s="34" t="s">
         <v>63</v>
@@ -1906,8 +1897,8 @@
       <c r="J2" s="73"/>
     </row>
     <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="85"/>
-      <c r="B3" s="88"/>
+      <c r="A3" s="88"/>
+      <c r="B3" s="85"/>
       <c r="C3" s="6">
         <v>2</v>
       </c>
@@ -1921,29 +1912,29 @@
         <v>36</v>
       </c>
       <c r="G3" s="17" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H3" s="35" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="I3" s="74" t="s">
         <v>37</v>
       </c>
       <c r="J3" s="75"/>
       <c r="K3" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="85"/>
-      <c r="B4" s="88" t="s">
+      <c r="A4" s="88"/>
+      <c r="B4" s="85" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="E4" s="47" t="s">
         <v>65</v>
@@ -1952,19 +1943,19 @@
         <v>36</v>
       </c>
       <c r="G4" s="27" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="H4" s="36" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="I4" s="74" t="s">
-        <v>157</v>
+        <v>37</v>
       </c>
       <c r="J4" s="75"/>
     </row>
     <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="85"/>
-      <c r="B5" s="88"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="85"/>
       <c r="C5" s="6">
         <v>4</v>
       </c>
@@ -1978,19 +1969,19 @@
         <v>36</v>
       </c>
       <c r="G5" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H5" s="36" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="I5" s="74" t="s">
-        <v>157</v>
+        <v>37</v>
       </c>
       <c r="J5" s="75"/>
     </row>
-    <row r="6" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A6" s="85"/>
-      <c r="B6" s="88" t="s">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="88"/>
+      <c r="B6" s="85" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="6">
@@ -2000,23 +1991,25 @@
         <v>18</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>82</v>
+        <v>153</v>
       </c>
       <c r="F6" s="61" t="s">
         <v>36</v>
       </c>
       <c r="G6" s="29" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>68</v>
-      </c>
-      <c r="I6" s="74"/>
+        <v>154</v>
+      </c>
+      <c r="I6" s="74" t="s">
+        <v>37</v>
+      </c>
       <c r="J6" s="75"/>
     </row>
     <row r="7" spans="1:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="86"/>
-      <c r="B7" s="89"/>
+      <c r="A7" s="89"/>
+      <c r="B7" s="86"/>
       <c r="C7" s="13">
         <v>6</v>
       </c>
@@ -2024,16 +2017,16 @@
         <v>19</v>
       </c>
       <c r="E7" s="49" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F7" s="62" t="s">
         <v>36</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H7" s="38" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="I7" s="76"/>
       <c r="J7" s="77"/>
@@ -2042,57 +2035,57 @@
       <c r="A8" s="90" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="92" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="14">
         <v>7</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F8" s="63" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="19" t="s">
+        <v>73</v>
+      </c>
+      <c r="H8" s="39" t="s">
         <v>75</v>
-      </c>
-      <c r="H8" s="39" t="s">
-        <v>77</v>
       </c>
       <c r="I8" s="78"/>
       <c r="J8" s="79"/>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="85"/>
-      <c r="B9" s="88"/>
+      <c r="A9" s="88"/>
+      <c r="B9" s="85"/>
       <c r="C9" s="6">
         <v>8</v>
       </c>
       <c r="D9" s="17" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E9" s="46" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F9" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G9" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="H9" s="35" t="s">
         <v>75</v>
-      </c>
-      <c r="H9" s="35" t="s">
-        <v>77</v>
       </c>
       <c r="I9" s="74"/>
       <c r="J9" s="75"/>
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="85"/>
-      <c r="B10" s="88"/>
+      <c r="A10" s="88"/>
+      <c r="B10" s="85"/>
       <c r="C10" s="6">
         <v>9</v>
       </c>
@@ -2100,49 +2093,49 @@
         <v>9</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="F10" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="17" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="35" t="s">
         <v>81</v>
-      </c>
-      <c r="H10" s="35" t="s">
-        <v>84</v>
       </c>
       <c r="I10" s="74"/>
       <c r="J10" s="75"/>
     </row>
-    <row r="11" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="85"/>
-      <c r="B11" s="88" t="s">
+    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="88"/>
+      <c r="B11" s="85" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E11" s="48" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="F11" s="61" t="s">
         <v>36</v>
       </c>
       <c r="G11" s="29" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="I11" s="74"/>
       <c r="J11" s="75"/>
     </row>
     <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="85"/>
-      <c r="B12" s="88"/>
+      <c r="A12" s="88"/>
+      <c r="B12" s="85"/>
       <c r="C12" s="6">
         <v>11</v>
       </c>
@@ -2150,23 +2143,23 @@
         <v>51</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F12" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I12" s="74"/>
       <c r="J12" s="75"/>
     </row>
     <row r="13" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="91"/>
-      <c r="B13" s="92"/>
+      <c r="B13" s="93"/>
       <c r="C13" s="9">
         <v>12</v>
       </c>
@@ -2174,75 +2167,75 @@
         <v>10</v>
       </c>
       <c r="E13" s="51" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="F13" s="64" t="s">
         <v>36</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="I13" s="80"/>
       <c r="J13" s="81"/>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="84" t="s">
+      <c r="A14" s="87" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="84" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="12">
         <v>13</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E14" s="45" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F14" s="58" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I14" s="72"/>
       <c r="J14" s="73"/>
     </row>
     <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="85"/>
-      <c r="B15" s="88"/>
+      <c r="A15" s="88"/>
+      <c r="B15" s="85"/>
       <c r="C15" s="6">
         <v>14</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E15" s="47" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="F15" s="60" t="s">
         <v>37</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H15" s="36" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I15" s="74"/>
       <c r="J15" s="75"/>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="85"/>
-      <c r="B16" s="88" t="s">
+      <c r="A16" s="88"/>
+      <c r="B16" s="85" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="6">
@@ -2252,23 +2245,23 @@
         <v>15</v>
       </c>
       <c r="E16" s="48" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="F16" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G16" s="29" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H16" s="37" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I16" s="74"/>
       <c r="J16" s="75"/>
     </row>
     <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="85"/>
-      <c r="B17" s="88"/>
+      <c r="A17" s="88"/>
+      <c r="B17" s="85"/>
       <c r="C17" s="6">
         <v>16</v>
       </c>
@@ -2276,23 +2269,23 @@
         <v>16</v>
       </c>
       <c r="E17" s="47" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="F17" s="60" t="s">
         <v>37</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H17" s="36" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="I17" s="74"/>
       <c r="J17" s="75"/>
     </row>
     <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="85"/>
-      <c r="B18" s="88" t="s">
+      <c r="A18" s="88"/>
+      <c r="B18" s="85" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="6">
@@ -2302,23 +2295,23 @@
         <v>17</v>
       </c>
       <c r="E18" s="48" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F18" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I18" s="74"/>
       <c r="J18" s="75"/>
     </row>
     <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="85"/>
-      <c r="B19" s="88"/>
+      <c r="A19" s="88"/>
+      <c r="B19" s="85"/>
       <c r="C19" s="6">
         <v>18</v>
       </c>
@@ -2326,23 +2319,23 @@
         <v>20</v>
       </c>
       <c r="E19" s="48" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="F19" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I19" s="74"/>
       <c r="J19" s="75"/>
     </row>
     <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="85"/>
-      <c r="B20" s="88"/>
+      <c r="A20" s="88"/>
+      <c r="B20" s="85"/>
       <c r="C20" s="6">
         <v>19</v>
       </c>
@@ -2350,23 +2343,23 @@
         <v>21</v>
       </c>
       <c r="E20" s="48" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="F20" s="61" t="s">
         <v>36</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I20" s="74"/>
       <c r="J20" s="75"/>
     </row>
     <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="85"/>
-      <c r="B21" s="88"/>
+      <c r="A21" s="88"/>
+      <c r="B21" s="85"/>
       <c r="C21" s="6">
         <v>20</v>
       </c>
@@ -2374,23 +2367,23 @@
         <v>22</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F21" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H21" s="35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I21" s="74"/>
       <c r="J21" s="75"/>
     </row>
     <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="85"/>
-      <c r="B22" s="88"/>
+      <c r="A22" s="88"/>
+      <c r="B22" s="85"/>
       <c r="C22" s="6">
         <v>21</v>
       </c>
@@ -2398,23 +2391,23 @@
         <v>23</v>
       </c>
       <c r="E22" s="46" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="F22" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="H22" s="35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I22" s="74"/>
       <c r="J22" s="75"/>
     </row>
     <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="85"/>
-      <c r="B23" s="88"/>
+      <c r="A23" s="88"/>
+      <c r="B23" s="85"/>
       <c r="C23" s="6">
         <v>22</v>
       </c>
@@ -2422,49 +2415,49 @@
         <v>24</v>
       </c>
       <c r="E23" s="48" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="F23" s="61" t="s">
         <v>36</v>
       </c>
       <c r="G23" s="29" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H23" s="37" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I23" s="74"/>
       <c r="J23" s="75"/>
     </row>
     <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="85"/>
-      <c r="B24" s="88" t="s">
+      <c r="A24" s="88"/>
+      <c r="B24" s="85" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="6">
         <v>23</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="E24" s="46" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="F24" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H24" s="35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I24" s="74"/>
       <c r="J24" s="75"/>
     </row>
     <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="85"/>
-      <c r="B25" s="88"/>
+      <c r="A25" s="88"/>
+      <c r="B25" s="85"/>
       <c r="C25" s="6">
         <v>24</v>
       </c>
@@ -2472,23 +2465,23 @@
         <v>28</v>
       </c>
       <c r="E25" s="46" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="F25" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="H25" s="35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I25" s="74"/>
       <c r="J25" s="75"/>
     </row>
     <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="85"/>
-      <c r="B26" s="88"/>
+      <c r="A26" s="88"/>
+      <c r="B26" s="85"/>
       <c r="C26" s="6">
         <v>25</v>
       </c>
@@ -2496,23 +2489,23 @@
         <v>30</v>
       </c>
       <c r="E26" s="46" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="F26" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H26" s="35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I26" s="74"/>
       <c r="J26" s="75"/>
     </row>
     <row r="27" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="86"/>
-      <c r="B27" s="89"/>
+      <c r="A27" s="89"/>
+      <c r="B27" s="86"/>
       <c r="C27" s="13">
         <v>26</v>
       </c>
@@ -2520,16 +2513,16 @@
         <v>31</v>
       </c>
       <c r="E27" s="52" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="F27" s="65" t="s">
         <v>37</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="H27" s="41" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I27" s="76"/>
       <c r="J27" s="77"/>
@@ -2538,33 +2531,33 @@
       <c r="A28" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="93" t="s">
+      <c r="B28" s="92" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="14">
         <v>27</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="E28" s="53" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="F28" s="66" t="s">
         <v>37</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="H28" s="42" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="I28" s="78"/>
       <c r="J28" s="79"/>
     </row>
     <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="85"/>
-      <c r="B29" s="88"/>
+      <c r="A29" s="88"/>
+      <c r="B29" s="85"/>
       <c r="C29" s="6">
         <v>28</v>
       </c>
@@ -2572,23 +2565,23 @@
         <v>40</v>
       </c>
       <c r="E29" s="48" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F29" s="61" t="s">
         <v>36</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I29" s="74"/>
       <c r="J29" s="75"/>
     </row>
     <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="85"/>
-      <c r="B30" s="88"/>
+      <c r="A30" s="88"/>
+      <c r="B30" s="85"/>
       <c r="C30" s="6">
         <v>29</v>
       </c>
@@ -2596,23 +2589,23 @@
         <v>41</v>
       </c>
       <c r="E30" s="48" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="F30" s="61" t="s">
         <v>36</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="H30" s="37" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I30" s="74"/>
       <c r="J30" s="75"/>
     </row>
     <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="85"/>
-      <c r="B31" s="88" t="s">
+      <c r="A31" s="88"/>
+      <c r="B31" s="85" t="s">
         <v>39</v>
       </c>
       <c r="C31" s="6">
@@ -2622,23 +2615,23 @@
         <v>53</v>
       </c>
       <c r="E31" s="46" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="F31" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="H31" s="35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I31" s="74"/>
       <c r="J31" s="75"/>
     </row>
     <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="85"/>
-      <c r="B32" s="88"/>
+      <c r="A32" s="88"/>
+      <c r="B32" s="85"/>
       <c r="C32" s="6">
         <v>31</v>
       </c>
@@ -2646,23 +2639,23 @@
         <v>54</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="F32" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="H32" s="35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I32" s="74"/>
       <c r="J32" s="75"/>
     </row>
     <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="85"/>
-      <c r="B33" s="88"/>
+      <c r="A33" s="88"/>
+      <c r="B33" s="85"/>
       <c r="C33" s="6">
         <v>32</v>
       </c>
@@ -2670,23 +2663,23 @@
         <v>42</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="F33" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H33" s="35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I33" s="74"/>
       <c r="J33" s="75"/>
     </row>
     <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="85"/>
-      <c r="B34" s="88"/>
+      <c r="A34" s="88"/>
+      <c r="B34" s="85"/>
       <c r="C34" s="6">
         <v>33</v>
       </c>
@@ -2694,23 +2687,23 @@
         <v>43</v>
       </c>
       <c r="E34" s="46" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="F34" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H34" s="35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I34" s="74"/>
       <c r="J34" s="75"/>
     </row>
     <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="85"/>
-      <c r="B35" s="88"/>
+      <c r="A35" s="88"/>
+      <c r="B35" s="85"/>
       <c r="C35" s="6">
         <v>34</v>
       </c>
@@ -2718,23 +2711,23 @@
         <v>55</v>
       </c>
       <c r="E35" s="46" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="F35" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="H35" s="35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I35" s="74"/>
       <c r="J35" s="75"/>
     </row>
     <row r="36" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="91"/>
-      <c r="B36" s="92"/>
+      <c r="B36" s="93"/>
       <c r="C36" s="9">
         <v>35</v>
       </c>
@@ -2742,25 +2735,25 @@
         <v>56</v>
       </c>
       <c r="E36" s="54" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="F36" s="67" t="s">
         <v>37</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H36" s="35" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="I36" s="80"/>
       <c r="J36" s="81"/>
     </row>
     <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="84" t="s">
-        <v>100</v>
-      </c>
-      <c r="B37" s="87" t="s">
+      <c r="A37" s="87" t="s">
+        <v>96</v>
+      </c>
+      <c r="B37" s="84" t="s">
         <v>46</v>
       </c>
       <c r="C37" s="12">
@@ -2770,23 +2763,23 @@
         <v>47</v>
       </c>
       <c r="E37" s="55" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F37" s="68" t="s">
         <v>37</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="H37" s="43" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="I37" s="72"/>
       <c r="J37" s="73"/>
     </row>
     <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="85"/>
-      <c r="B38" s="88"/>
+      <c r="A38" s="88"/>
+      <c r="B38" s="85"/>
       <c r="C38" s="6">
         <v>37</v>
       </c>
@@ -2794,23 +2787,23 @@
         <v>52</v>
       </c>
       <c r="E38" s="46" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F38" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H38" s="35" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="I38" s="74"/>
       <c r="J38" s="75"/>
     </row>
     <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="85"/>
-      <c r="B39" s="88" t="s">
+      <c r="A39" s="88"/>
+      <c r="B39" s="85" t="s">
         <v>48</v>
       </c>
       <c r="C39" s="6">
@@ -2820,23 +2813,23 @@
         <v>49</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F39" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="H39" s="35" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="I39" s="74"/>
       <c r="J39" s="75"/>
     </row>
     <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="85"/>
-      <c r="B40" s="88"/>
+      <c r="A40" s="88"/>
+      <c r="B40" s="85"/>
       <c r="C40" s="6">
         <v>39</v>
       </c>
@@ -2844,23 +2837,23 @@
         <v>50</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F40" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="H40" s="35" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="I40" s="74"/>
       <c r="J40" s="75"/>
     </row>
     <row r="41" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="86"/>
-      <c r="B41" s="89"/>
+      <c r="A41" s="89"/>
+      <c r="B41" s="86"/>
       <c r="C41" s="13">
         <v>40</v>
       </c>
@@ -2868,16 +2861,16 @@
         <v>60</v>
       </c>
       <c r="E41" s="52" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="F41" s="65" t="s">
         <v>37</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="H41" s="41" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="I41" s="76"/>
       <c r="J41" s="77"/>
@@ -2896,22 +2889,29 @@
         <v>59</v>
       </c>
       <c r="E42" s="56" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="F42" s="69" t="s">
         <v>37</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H42" s="44" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="I42" s="82"/>
       <c r="J42" s="83"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="A37:A41"/>
@@ -2923,13 +2923,6 @@
     <mergeCell ref="A28:A36"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B36"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Y">

</xml_diff>

<commit_message>
Completed more test cases
</commit_message>
<xml_diff>
--- a/TESTCASES/TestCases.xlsx
+++ b/TESTCASES/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uogcloud-my.sharepoint.com/personal/mj4126n_gre_ac_uk/Documents/PhD/Application/ObjectController/TESTCASES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="13_ncr:1_{18352CE1-B835-4F67-B7F2-89796C74D3C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B8638761-7A36-44F0-8DCA-3AD217927AC7}"/>
+  <xr:revisionPtr revIDLastSave="33" documentId="13_ncr:1_{18352CE1-B835-4F67-B7F2-89796C74D3C6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{1BF10B6F-0765-4773-9E30-65CF4308D0F8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="158">
   <si>
     <t>Vertices and attachment points are correct relative to CoR</t>
   </si>
@@ -253,10 +253,6 @@
   </si>
   <si>
     <t>Rectangle_W3L40.csv</t>
-  </si>
-  <si>
-    <t>Rectangle_W2L2.csv
-Rectangle_W5L5.csv</t>
   </si>
   <si>
     <t>Generate TSBS (no layers). Take screenshot of T-Space and C-Space. Get degree of each of the nodes</t>
@@ -510,6 +506,20 @@
   </si>
   <si>
     <t>Frequency table of angles when moved</t>
+  </si>
+  <si>
+    <t>Rectangle_W2L2.csv
+Rectangle_W5L5.csv
+Irregular_W5L10.csv</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Results are together with 7</t>
+  </si>
+  <si>
+    <t>Get Rhino exports. Screenshots for corridor.</t>
   </si>
 </sst>
 </file>
@@ -1164,9 +1174,7 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -1177,7 +1185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="99">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1389,74 +1397,89 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1816,8 +1839,8 @@
   <dimension ref="A1:K42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I8" sqref="I8"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1831,7 +1854,8 @@
     <col min="8" max="8" width="28.28515625" style="24" customWidth="1"/>
     <col min="9" max="9" width="9.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.140625" style="2"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="17.7109375" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -1854,23 +1878,26 @@
         <v>34</v>
       </c>
       <c r="G1" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H1" s="33" t="s">
         <v>35</v>
       </c>
       <c r="I1" s="70" t="s">
+        <v>145</v>
+      </c>
+      <c r="J1" s="88" t="s">
         <v>146</v>
       </c>
-      <c r="J1" s="71" t="s">
-        <v>147</v>
+      <c r="K1" s="87" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="84" t="s">
+      <c r="A2" s="80" t="s">
         <v>44</v>
       </c>
-      <c r="B2" s="87" t="s">
+      <c r="B2" s="77" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="12">
@@ -1891,14 +1918,15 @@
       <c r="H2" s="34" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="72" t="s">
+      <c r="I2" s="71" t="s">
         <v>37</v>
       </c>
-      <c r="J2" s="73"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="96"/>
     </row>
     <row r="3" spans="1:11" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="85"/>
-      <c r="B3" s="88"/>
+      <c r="A3" s="81"/>
+      <c r="B3" s="78"/>
       <c r="C3" s="6">
         <v>2</v>
       </c>
@@ -1917,24 +1945,24 @@
       <c r="H3" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="74" t="s">
+      <c r="I3" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="75"/>
-      <c r="K3" s="1" t="s">
-        <v>148</v>
+      <c r="J3" s="90"/>
+      <c r="K3" s="97" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="85"/>
-      <c r="B4" s="88" t="s">
+      <c r="A4" s="81"/>
+      <c r="B4" s="78" t="s">
         <v>25</v>
       </c>
       <c r="C4" s="6">
         <v>3</v>
       </c>
       <c r="D4" s="27" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E4" s="47" t="s">
         <v>65</v>
@@ -1943,19 +1971,20 @@
         <v>36</v>
       </c>
       <c r="G4" s="27" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" s="36" t="s">
         <v>150</v>
       </c>
-      <c r="H4" s="36" t="s">
-        <v>151</v>
-      </c>
-      <c r="I4" s="74" t="s">
+      <c r="I4" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="75"/>
+      <c r="J4" s="90"/>
+      <c r="K4" s="97"/>
     </row>
     <row r="5" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="85"/>
-      <c r="B5" s="88"/>
+      <c r="A5" s="81"/>
+      <c r="B5" s="78"/>
       <c r="C5" s="6">
         <v>4</v>
       </c>
@@ -1974,14 +2003,15 @@
       <c r="H5" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="I5" s="74" t="s">
+      <c r="I5" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="J5" s="75"/>
+      <c r="J5" s="90"/>
+      <c r="K5" s="97"/>
     </row>
     <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="85"/>
-      <c r="B6" s="88" t="s">
+      <c r="A6" s="81"/>
+      <c r="B6" s="78" t="s">
         <v>26</v>
       </c>
       <c r="C6" s="6">
@@ -1991,7 +2021,7 @@
         <v>18</v>
       </c>
       <c r="E6" s="48" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F6" s="61" t="s">
         <v>36</v>
@@ -2000,16 +2030,17 @@
         <v>71</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>154</v>
-      </c>
-      <c r="I6" s="74" t="s">
+        <v>153</v>
+      </c>
+      <c r="I6" s="72" t="s">
         <v>37</v>
       </c>
-      <c r="J6" s="75"/>
+      <c r="J6" s="90"/>
+      <c r="K6" s="97"/>
     </row>
     <row r="7" spans="1:11" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="86"/>
-      <c r="B7" s="89"/>
+      <c r="A7" s="82"/>
+      <c r="B7" s="79"/>
       <c r="C7" s="13">
         <v>6</v>
       </c>
@@ -2023,71 +2054,80 @@
         <v>36</v>
       </c>
       <c r="G7" s="30" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H7" s="38" t="s">
         <v>69</v>
       </c>
-      <c r="I7" s="76" t="s">
+      <c r="I7" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="J7" s="77"/>
+      <c r="J7" s="91"/>
+      <c r="K7" s="98"/>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="90" t="s">
+      <c r="A8" s="83" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="93" t="s">
+      <c r="B8" s="85" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="14">
         <v>7</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E8" s="50" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" s="63" t="s">
         <v>36</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>73</v>
+        <v>154</v>
       </c>
       <c r="H8" s="39" t="s">
-        <v>75</v>
-      </c>
-      <c r="I8" s="78"/>
-      <c r="J8" s="79"/>
+        <v>74</v>
+      </c>
+      <c r="I8" s="74" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="92"/>
+      <c r="K8" s="96"/>
     </row>
     <row r="9" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="85"/>
-      <c r="B9" s="88"/>
+      <c r="A9" s="81"/>
+      <c r="B9" s="78"/>
       <c r="C9" s="6">
         <v>8</v>
       </c>
       <c r="D9" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="46" t="s">
         <v>77</v>
-      </c>
-      <c r="E9" s="46" t="s">
-        <v>78</v>
       </c>
       <c r="F9" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G9" s="17" t="s">
-        <v>73</v>
+        <v>154</v>
       </c>
       <c r="H9" s="35" t="s">
-        <v>75</v>
-      </c>
-      <c r="I9" s="74"/>
-      <c r="J9" s="75"/>
+        <v>74</v>
+      </c>
+      <c r="I9" s="72" t="s">
+        <v>37</v>
+      </c>
+      <c r="J9" s="90"/>
+      <c r="K9" s="97" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="85"/>
-      <c r="B10" s="88"/>
+      <c r="A10" s="81"/>
+      <c r="B10" s="78"/>
       <c r="C10" s="6">
         <v>9</v>
       </c>
@@ -2095,33 +2135,36 @@
         <v>9</v>
       </c>
       <c r="E10" s="46" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F10" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G10" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="H10" s="35" t="s">
-        <v>81</v>
-      </c>
-      <c r="I10" s="74"/>
-      <c r="J10" s="75"/>
+        <v>80</v>
+      </c>
+      <c r="I10" s="72"/>
+      <c r="J10" s="90"/>
+      <c r="K10" s="97" t="s">
+        <v>157</v>
+      </c>
     </row>
     <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="85"/>
-      <c r="B11" s="88" t="s">
+      <c r="A11" s="81"/>
+      <c r="B11" s="78" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="6">
         <v>10</v>
       </c>
       <c r="D11" s="29" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E11" s="48" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F11" s="61" t="s">
         <v>36</v>
@@ -2130,14 +2173,15 @@
         <v>71</v>
       </c>
       <c r="H11" s="37" t="s">
-        <v>88</v>
-      </c>
-      <c r="I11" s="74"/>
-      <c r="J11" s="75"/>
+        <v>87</v>
+      </c>
+      <c r="I11" s="72"/>
+      <c r="J11" s="90"/>
+      <c r="K11" s="97"/>
     </row>
     <row r="12" spans="1:11" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12" s="85"/>
-      <c r="B12" s="88"/>
+      <c r="A12" s="81"/>
+      <c r="B12" s="78"/>
       <c r="C12" s="6">
         <v>11</v>
       </c>
@@ -2145,23 +2189,24 @@
         <v>51</v>
       </c>
       <c r="E12" s="46" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F12" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G12" s="17" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="H12" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="I12" s="74"/>
-      <c r="J12" s="75"/>
+        <v>88</v>
+      </c>
+      <c r="I12" s="72"/>
+      <c r="J12" s="90"/>
+      <c r="K12" s="97"/>
     </row>
     <row r="13" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="91"/>
-      <c r="B13" s="92"/>
+      <c r="A13" s="84"/>
+      <c r="B13" s="86"/>
       <c r="C13" s="9">
         <v>12</v>
       </c>
@@ -2169,75 +2214,78 @@
         <v>10</v>
       </c>
       <c r="E13" s="51" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F13" s="64" t="s">
         <v>36</v>
       </c>
       <c r="G13" s="31" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="H13" s="40" t="s">
-        <v>92</v>
-      </c>
-      <c r="I13" s="80"/>
-      <c r="J13" s="81"/>
+        <v>91</v>
+      </c>
+      <c r="I13" s="75"/>
+      <c r="J13" s="93"/>
+      <c r="K13" s="98"/>
     </row>
     <row r="14" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="84" t="s">
+      <c r="A14" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="87" t="s">
+      <c r="B14" s="77" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="12">
         <v>13</v>
       </c>
       <c r="D14" s="26" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E14" s="45" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F14" s="58" t="s">
         <v>37</v>
       </c>
       <c r="G14" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H14" s="34" t="s">
-        <v>95</v>
-      </c>
-      <c r="I14" s="72"/>
-      <c r="J14" s="73"/>
+        <v>94</v>
+      </c>
+      <c r="I14" s="71"/>
+      <c r="J14" s="89"/>
+      <c r="K14" s="96"/>
     </row>
     <row r="15" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="85"/>
-      <c r="B15" s="88"/>
+      <c r="A15" s="81"/>
+      <c r="B15" s="78"/>
       <c r="C15" s="6">
         <v>14</v>
       </c>
       <c r="D15" s="27" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E15" s="47" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="F15" s="60" t="s">
         <v>37</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H15" s="36" t="s">
-        <v>95</v>
-      </c>
-      <c r="I15" s="74"/>
-      <c r="J15" s="75"/>
+        <v>94</v>
+      </c>
+      <c r="I15" s="72"/>
+      <c r="J15" s="90"/>
+      <c r="K15" s="97"/>
     </row>
     <row r="16" spans="1:11" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="85"/>
-      <c r="B16" s="88" t="s">
+      <c r="A16" s="81"/>
+      <c r="B16" s="78" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="6">
@@ -2247,23 +2295,24 @@
         <v>15</v>
       </c>
       <c r="E16" s="48" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F16" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G16" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="H16" s="37" t="s">
         <v>105</v>
       </c>
-      <c r="H16" s="37" t="s">
-        <v>106</v>
-      </c>
-      <c r="I16" s="74"/>
-      <c r="J16" s="75"/>
-    </row>
-    <row r="17" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="85"/>
-      <c r="B17" s="88"/>
+      <c r="I16" s="72"/>
+      <c r="J16" s="90"/>
+      <c r="K16" s="97"/>
+    </row>
+    <row r="17" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="81"/>
+      <c r="B17" s="78"/>
       <c r="C17" s="6">
         <v>16</v>
       </c>
@@ -2271,23 +2320,24 @@
         <v>16</v>
       </c>
       <c r="E17" s="47" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="F17" s="60" t="s">
         <v>37</v>
       </c>
       <c r="G17" s="27" t="s">
+        <v>104</v>
+      </c>
+      <c r="H17" s="36" t="s">
         <v>105</v>
       </c>
-      <c r="H17" s="36" t="s">
-        <v>106</v>
-      </c>
-      <c r="I17" s="74"/>
-      <c r="J17" s="75"/>
-    </row>
-    <row r="18" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A18" s="85"/>
-      <c r="B18" s="88" t="s">
+      <c r="I17" s="72"/>
+      <c r="J17" s="90"/>
+      <c r="K17" s="97"/>
+    </row>
+    <row r="18" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A18" s="81"/>
+      <c r="B18" s="78" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="6">
@@ -2297,23 +2347,24 @@
         <v>17</v>
       </c>
       <c r="E18" s="48" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F18" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G18" s="29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H18" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="I18" s="74"/>
-      <c r="J18" s="75"/>
-    </row>
-    <row r="19" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="85"/>
-      <c r="B19" s="88"/>
+        <v>112</v>
+      </c>
+      <c r="I18" s="72"/>
+      <c r="J18" s="90"/>
+      <c r="K18" s="97"/>
+    </row>
+    <row r="19" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="81"/>
+      <c r="B19" s="78"/>
       <c r="C19" s="6">
         <v>18</v>
       </c>
@@ -2321,23 +2372,24 @@
         <v>20</v>
       </c>
       <c r="E19" s="48" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="F19" s="61" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H19" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="I19" s="74"/>
-      <c r="J19" s="75"/>
-    </row>
-    <row r="20" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="85"/>
-      <c r="B20" s="88"/>
+        <v>112</v>
+      </c>
+      <c r="I19" s="72"/>
+      <c r="J19" s="90"/>
+      <c r="K19" s="97"/>
+    </row>
+    <row r="20" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="81"/>
+      <c r="B20" s="78"/>
       <c r="C20" s="6">
         <v>19</v>
       </c>
@@ -2345,23 +2397,24 @@
         <v>21</v>
       </c>
       <c r="E20" s="48" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F20" s="61" t="s">
         <v>36</v>
       </c>
       <c r="G20" s="29" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H20" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="I20" s="74"/>
-      <c r="J20" s="75"/>
-    </row>
-    <row r="21" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="85"/>
-      <c r="B21" s="88"/>
+        <v>112</v>
+      </c>
+      <c r="I20" s="72"/>
+      <c r="J20" s="90"/>
+      <c r="K20" s="97"/>
+    </row>
+    <row r="21" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="81"/>
+      <c r="B21" s="78"/>
       <c r="C21" s="6">
         <v>20</v>
       </c>
@@ -2369,23 +2422,24 @@
         <v>22</v>
       </c>
       <c r="E21" s="46" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F21" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G21" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H21" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I21" s="74"/>
-      <c r="J21" s="75"/>
-    </row>
-    <row r="22" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="85"/>
-      <c r="B22" s="88"/>
+        <v>112</v>
+      </c>
+      <c r="I21" s="72"/>
+      <c r="J21" s="90"/>
+      <c r="K21" s="97"/>
+    </row>
+    <row r="22" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="81"/>
+      <c r="B22" s="78"/>
       <c r="C22" s="6">
         <v>21</v>
       </c>
@@ -2393,23 +2447,24 @@
         <v>23</v>
       </c>
       <c r="E22" s="46" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F22" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G22" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="H22" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I22" s="74"/>
-      <c r="J22" s="75"/>
-    </row>
-    <row r="23" spans="1:10" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="85"/>
-      <c r="B23" s="88"/>
+        <v>112</v>
+      </c>
+      <c r="I22" s="72"/>
+      <c r="J22" s="90"/>
+      <c r="K22" s="97"/>
+    </row>
+    <row r="23" spans="1:11" ht="60" x14ac:dyDescent="0.25">
+      <c r="A23" s="81"/>
+      <c r="B23" s="78"/>
       <c r="C23" s="6">
         <v>22</v>
       </c>
@@ -2417,7 +2472,7 @@
         <v>24</v>
       </c>
       <c r="E23" s="48" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F23" s="61" t="s">
         <v>36</v>
@@ -2426,40 +2481,42 @@
         <v>71</v>
       </c>
       <c r="H23" s="37" t="s">
-        <v>119</v>
-      </c>
-      <c r="I23" s="74"/>
-      <c r="J23" s="75"/>
-    </row>
-    <row r="24" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="85"/>
-      <c r="B24" s="88" t="s">
+        <v>118</v>
+      </c>
+      <c r="I23" s="72"/>
+      <c r="J23" s="90"/>
+      <c r="K23" s="97"/>
+    </row>
+    <row r="24" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="81"/>
+      <c r="B24" s="78" t="s">
         <v>29</v>
       </c>
       <c r="C24" s="6">
         <v>23</v>
       </c>
       <c r="D24" s="17" t="s">
+        <v>120</v>
+      </c>
+      <c r="E24" s="46" t="s">
         <v>121</v>
-      </c>
-      <c r="E24" s="46" t="s">
-        <v>122</v>
       </c>
       <c r="F24" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G24" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H24" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I24" s="74"/>
-      <c r="J24" s="75"/>
-    </row>
-    <row r="25" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="85"/>
-      <c r="B25" s="88"/>
+        <v>112</v>
+      </c>
+      <c r="I24" s="72"/>
+      <c r="J24" s="90"/>
+      <c r="K24" s="97"/>
+    </row>
+    <row r="25" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="81"/>
+      <c r="B25" s="78"/>
       <c r="C25" s="6">
         <v>24</v>
       </c>
@@ -2467,23 +2524,24 @@
         <v>28</v>
       </c>
       <c r="E25" s="46" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F25" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G25" s="17" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="H25" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I25" s="74"/>
-      <c r="J25" s="75"/>
-    </row>
-    <row r="26" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="85"/>
-      <c r="B26" s="88"/>
+        <v>112</v>
+      </c>
+      <c r="I25" s="72"/>
+      <c r="J25" s="90"/>
+      <c r="K25" s="97"/>
+    </row>
+    <row r="26" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26" s="81"/>
+      <c r="B26" s="78"/>
       <c r="C26" s="6">
         <v>25</v>
       </c>
@@ -2491,23 +2549,24 @@
         <v>30</v>
       </c>
       <c r="E26" s="46" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F26" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G26" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H26" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I26" s="74"/>
-      <c r="J26" s="75"/>
-    </row>
-    <row r="27" spans="1:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="86"/>
-      <c r="B27" s="89"/>
+        <v>112</v>
+      </c>
+      <c r="I26" s="72"/>
+      <c r="J26" s="90"/>
+      <c r="K26" s="97"/>
+    </row>
+    <row r="27" spans="1:11" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="82"/>
+      <c r="B27" s="79"/>
       <c r="C27" s="13">
         <v>26</v>
       </c>
@@ -2515,51 +2574,53 @@
         <v>31</v>
       </c>
       <c r="E27" s="52" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F27" s="65" t="s">
         <v>37</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="H27" s="41" t="s">
-        <v>113</v>
-      </c>
-      <c r="I27" s="76"/>
-      <c r="J27" s="77"/>
-    </row>
-    <row r="28" spans="1:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="90" t="s">
+        <v>112</v>
+      </c>
+      <c r="I27" s="73"/>
+      <c r="J27" s="91"/>
+      <c r="K27" s="98"/>
+    </row>
+    <row r="28" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="93" t="s">
+      <c r="B28" s="85" t="s">
         <v>38</v>
       </c>
       <c r="C28" s="14">
         <v>27</v>
       </c>
       <c r="D28" s="28" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E28" s="53" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F28" s="66" t="s">
         <v>37</v>
       </c>
       <c r="G28" s="28" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H28" s="42" t="s">
-        <v>86</v>
-      </c>
-      <c r="I28" s="78"/>
-      <c r="J28" s="79"/>
-    </row>
-    <row r="29" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="85"/>
-      <c r="B29" s="88"/>
+        <v>85</v>
+      </c>
+      <c r="I28" s="74"/>
+      <c r="J28" s="92"/>
+      <c r="K28" s="96"/>
+    </row>
+    <row r="29" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="81"/>
+      <c r="B29" s="78"/>
       <c r="C29" s="6">
         <v>28</v>
       </c>
@@ -2567,23 +2628,24 @@
         <v>40</v>
       </c>
       <c r="E29" s="48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F29" s="61" t="s">
         <v>36</v>
       </c>
       <c r="G29" s="29" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="H29" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="I29" s="74"/>
-      <c r="J29" s="75"/>
-    </row>
-    <row r="30" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="85"/>
-      <c r="B30" s="88"/>
+        <v>112</v>
+      </c>
+      <c r="I29" s="72"/>
+      <c r="J29" s="90"/>
+      <c r="K29" s="97"/>
+    </row>
+    <row r="30" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="81"/>
+      <c r="B30" s="78"/>
       <c r="C30" s="6">
         <v>29</v>
       </c>
@@ -2591,23 +2653,24 @@
         <v>41</v>
       </c>
       <c r="E30" s="48" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F30" s="61" t="s">
         <v>36</v>
       </c>
       <c r="G30" s="29" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="H30" s="37" t="s">
-        <v>113</v>
-      </c>
-      <c r="I30" s="74"/>
-      <c r="J30" s="75"/>
-    </row>
-    <row r="31" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="85"/>
-      <c r="B31" s="88" t="s">
+        <v>112</v>
+      </c>
+      <c r="I30" s="72"/>
+      <c r="J30" s="90"/>
+      <c r="K30" s="97"/>
+    </row>
+    <row r="31" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="81"/>
+      <c r="B31" s="78" t="s">
         <v>39</v>
       </c>
       <c r="C31" s="6">
@@ -2617,23 +2680,24 @@
         <v>53</v>
       </c>
       <c r="E31" s="46" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F31" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G31" s="17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="H31" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I31" s="74"/>
-      <c r="J31" s="75"/>
-    </row>
-    <row r="32" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="85"/>
-      <c r="B32" s="88"/>
+        <v>112</v>
+      </c>
+      <c r="I31" s="72"/>
+      <c r="J31" s="90"/>
+      <c r="K31" s="97"/>
+    </row>
+    <row r="32" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="81"/>
+      <c r="B32" s="78"/>
       <c r="C32" s="6">
         <v>31</v>
       </c>
@@ -2641,23 +2705,24 @@
         <v>54</v>
       </c>
       <c r="E32" s="46" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="F32" s="59" t="s">
         <v>36</v>
       </c>
       <c r="G32" s="17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="H32" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I32" s="74"/>
-      <c r="J32" s="75"/>
-    </row>
-    <row r="33" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="85"/>
-      <c r="B33" s="88"/>
+        <v>112</v>
+      </c>
+      <c r="I32" s="72"/>
+      <c r="J32" s="90"/>
+      <c r="K32" s="97"/>
+    </row>
+    <row r="33" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="81"/>
+      <c r="B33" s="78"/>
       <c r="C33" s="6">
         <v>32</v>
       </c>
@@ -2665,23 +2730,24 @@
         <v>42</v>
       </c>
       <c r="E33" s="46" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F33" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G33" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H33" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I33" s="74"/>
-      <c r="J33" s="75"/>
-    </row>
-    <row r="34" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="85"/>
-      <c r="B34" s="88"/>
+        <v>112</v>
+      </c>
+      <c r="I33" s="72"/>
+      <c r="J33" s="90"/>
+      <c r="K33" s="97"/>
+    </row>
+    <row r="34" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="81"/>
+      <c r="B34" s="78"/>
       <c r="C34" s="6">
         <v>33</v>
       </c>
@@ -2689,23 +2755,24 @@
         <v>43</v>
       </c>
       <c r="E34" s="46" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F34" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G34" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H34" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I34" s="74"/>
-      <c r="J34" s="75"/>
-    </row>
-    <row r="35" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="85"/>
-      <c r="B35" s="88"/>
+        <v>112</v>
+      </c>
+      <c r="I34" s="72"/>
+      <c r="J34" s="90"/>
+      <c r="K34" s="97"/>
+    </row>
+    <row r="35" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="81"/>
+      <c r="B35" s="78"/>
       <c r="C35" s="6">
         <v>34</v>
       </c>
@@ -2713,23 +2780,24 @@
         <v>55</v>
       </c>
       <c r="E35" s="46" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="F35" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G35" s="17" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H35" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I35" s="74"/>
-      <c r="J35" s="75"/>
-    </row>
-    <row r="36" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="91"/>
-      <c r="B36" s="92"/>
+        <v>112</v>
+      </c>
+      <c r="I35" s="72"/>
+      <c r="J35" s="90"/>
+      <c r="K35" s="97"/>
+    </row>
+    <row r="36" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="84"/>
+      <c r="B36" s="86"/>
       <c r="C36" s="9">
         <v>35</v>
       </c>
@@ -2737,25 +2805,26 @@
         <v>56</v>
       </c>
       <c r="E36" s="54" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F36" s="67" t="s">
         <v>37</v>
       </c>
       <c r="G36" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="H36" s="35" t="s">
-        <v>113</v>
-      </c>
-      <c r="I36" s="80"/>
-      <c r="J36" s="81"/>
-    </row>
-    <row r="37" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="84" t="s">
-        <v>96</v>
-      </c>
-      <c r="B37" s="87" t="s">
+        <v>112</v>
+      </c>
+      <c r="I36" s="75"/>
+      <c r="J36" s="93"/>
+      <c r="K36" s="98"/>
+    </row>
+    <row r="37" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="80" t="s">
+        <v>95</v>
+      </c>
+      <c r="B37" s="77" t="s">
         <v>46</v>
       </c>
       <c r="C37" s="12">
@@ -2765,23 +2834,24 @@
         <v>47</v>
       </c>
       <c r="E37" s="55" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F37" s="68" t="s">
         <v>37</v>
       </c>
       <c r="G37" s="16" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H37" s="43" t="s">
-        <v>143</v>
-      </c>
-      <c r="I37" s="72"/>
-      <c r="J37" s="73"/>
-    </row>
-    <row r="38" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="85"/>
-      <c r="B38" s="88"/>
+        <v>142</v>
+      </c>
+      <c r="I37" s="71"/>
+      <c r="J37" s="89"/>
+      <c r="K37" s="96"/>
+    </row>
+    <row r="38" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="81"/>
+      <c r="B38" s="78"/>
       <c r="C38" s="6">
         <v>37</v>
       </c>
@@ -2789,23 +2859,24 @@
         <v>52</v>
       </c>
       <c r="E38" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F38" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G38" s="17" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H38" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="I38" s="74"/>
-      <c r="J38" s="75"/>
-    </row>
-    <row r="39" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="85"/>
-      <c r="B39" s="88" t="s">
+        <v>142</v>
+      </c>
+      <c r="I38" s="72"/>
+      <c r="J38" s="90"/>
+      <c r="K38" s="97"/>
+    </row>
+    <row r="39" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="81"/>
+      <c r="B39" s="78" t="s">
         <v>48</v>
       </c>
       <c r="C39" s="6">
@@ -2815,23 +2886,24 @@
         <v>49</v>
       </c>
       <c r="E39" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F39" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G39" s="17" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="H39" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="I39" s="74"/>
-      <c r="J39" s="75"/>
-    </row>
-    <row r="40" spans="1:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="85"/>
-      <c r="B40" s="88"/>
+        <v>142</v>
+      </c>
+      <c r="I39" s="72"/>
+      <c r="J39" s="90"/>
+      <c r="K39" s="97"/>
+    </row>
+    <row r="40" spans="1:11" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="81"/>
+      <c r="B40" s="78"/>
       <c r="C40" s="6">
         <v>39</v>
       </c>
@@ -2839,23 +2911,24 @@
         <v>50</v>
       </c>
       <c r="E40" s="46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F40" s="59" t="s">
         <v>37</v>
       </c>
       <c r="G40" s="17" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="H40" s="35" t="s">
-        <v>143</v>
-      </c>
-      <c r="I40" s="74"/>
-      <c r="J40" s="75"/>
-    </row>
-    <row r="41" spans="1:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="86"/>
-      <c r="B41" s="89"/>
+        <v>142</v>
+      </c>
+      <c r="I40" s="72"/>
+      <c r="J40" s="90"/>
+      <c r="K40" s="97"/>
+    </row>
+    <row r="41" spans="1:11" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="82"/>
+      <c r="B41" s="79"/>
       <c r="C41" s="13">
         <v>40</v>
       </c>
@@ -2863,21 +2936,22 @@
         <v>60</v>
       </c>
       <c r="E41" s="52" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F41" s="65" t="s">
         <v>37</v>
       </c>
       <c r="G41" s="18" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="H41" s="41" t="s">
-        <v>143</v>
-      </c>
-      <c r="I41" s="76"/>
-      <c r="J41" s="77"/>
-    </row>
-    <row r="42" spans="1:10" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>142</v>
+      </c>
+      <c r="I41" s="73"/>
+      <c r="J41" s="91"/>
+      <c r="K41" s="98"/>
+    </row>
+    <row r="42" spans="1:11" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="7" t="s">
         <v>45</v>
       </c>
@@ -2891,22 +2965,30 @@
         <v>59</v>
       </c>
       <c r="E42" s="56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="F42" s="69" t="s">
         <v>37</v>
       </c>
       <c r="G42" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="H42" s="44" t="s">
-        <v>145</v>
-      </c>
-      <c r="I42" s="82"/>
-      <c r="J42" s="83"/>
+        <v>144</v>
+      </c>
+      <c r="I42" s="76"/>
+      <c r="J42" s="94"/>
+      <c r="K42" s="95"/>
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="A37:A41"/>
@@ -2918,13 +3000,6 @@
     <mergeCell ref="A28:A36"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B36"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="F2:F1048576">
     <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Y">

</xml_diff>

<commit_message>
Combined some test cases together
</commit_message>
<xml_diff>
--- a/TESTCASES/TestCases.xlsx
+++ b/TESTCASES/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andra\OneDrive - University of Greenwich\PhD\Application\ObjectController\TESTCASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{979D7A01-467E-48CC-B807-BFCC2766DE32}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2C8C6F-BD8D-4938-B8C7-3CDB1E1397C4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="272" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="171">
   <si>
     <t>Vertices and attachment points are correct relative to CoR</t>
   </si>
@@ -122,9 +122,6 @@
     <t>Complex Movement</t>
   </si>
   <si>
-    <t>Object waits at entrance of thin corridor/doorway for another object with higher drive to pass in contra-flow</t>
-  </si>
-  <si>
     <t>Person waits at entrance of thin corridor/doorway for object with high drive to pass in contra-flow</t>
   </si>
   <si>
@@ -186,12 +183,6 @@
   </si>
   <si>
     <t>The OC can simulate a full hospital evacuation</t>
-  </si>
-  <si>
-    <t>Many different objects can navigate around each other in an open space (cross-flow)</t>
-  </si>
-  <si>
-    <t>Many different objects can navigate around each other in a corridor (contra-flow)</t>
   </si>
   <si>
     <t>Many different objects can navigate around many people in an open space (cross-flow)</t>
@@ -366,19 +357,10 @@
     <t>Object1 (large) in one corner and Object2 at opposite corner. Both moving to oposite ends. Object1 has very high drive. Object2 must avoid and goes far enough away from path that has to recalc a route</t>
   </si>
   <si>
-    <t>Slow person going down stairs moves out of the way of an object (with high drive) going down</t>
-  </si>
-  <si>
-    <t>Person goes down middle of stair, followed by object. Person has low move on stair speed. Object moves past. See if person moves to one side.</t>
-  </si>
-  <si>
     <t>Person goes up middle of stair, object goes down. See if person moves to one side.</t>
   </si>
   <si>
     <t>ThinWideCor_W3W6.mta</t>
-  </si>
-  <si>
-    <t>Object1 starts on thin side, Object2 starts on wide side. Move counter. See if object2 waits for object1. Try with different drives</t>
   </si>
   <si>
     <t>Object starts on thin side, person starts on wide side. Move counter. See if person waits for object. Try with different drives</t>
@@ -404,13 +386,7 @@
     <t>XShape_W6L20x2.csv</t>
   </si>
   <si>
-    <t>A number of objects moving W to E and a number moving N to S</t>
-  </si>
-  <si>
     <t>Rectangle_W6L30.csv</t>
-  </si>
-  <si>
-    <t>A number of objects moving W to E and a number moving E to W</t>
   </si>
   <si>
     <t>A number of objects moving W to E and a number of people moving N to S</t>
@@ -553,6 +529,42 @@
   </si>
   <si>
     <t>Object1 at one end of corridor and Object2 at opposite end. Both moving to oposite ends. Test Object1 with higher drive and both with similar drive.</t>
+  </si>
+  <si>
+    <t>Objects and people can can navigate around each other in cross-flow. Many objects, one object many people, many objects many people.</t>
+  </si>
+  <si>
+    <t>A number of entities moving W to E and a number moving N to S all mixed together</t>
+  </si>
+  <si>
+    <t>Covered in TC 30</t>
+  </si>
+  <si>
+    <t>Objects and people can can navigate around each other in contra-flow. Many objects, one object many people, many objects many people.</t>
+  </si>
+  <si>
+    <t>A number of objects moving W to E and a number moving E to W in corridor all mixed together</t>
+  </si>
+  <si>
+    <t>Covered in TC 31</t>
+  </si>
+  <si>
+    <t>Person going up/down stairs moves out of the way of an object (with high drive) going down</t>
+  </si>
+  <si>
+    <t>Covered in TC 23</t>
+  </si>
+  <si>
+    <t>Person goes up/down middle of stair, object goes down. See if person moves to one side t let object past. If person going down, movement speed is low</t>
+  </si>
+  <si>
+    <t>Object/Person waits at entrance of thin corridor/doorway for object with higher drive to pass in contra-flow</t>
+  </si>
+  <si>
+    <t>Object1 starts on thin side, Object2/person starts on wide side. Move counter. See if object2/person waits for object1. Try with different drives</t>
+  </si>
+  <si>
+    <t>Covered in TC25</t>
   </si>
 </sst>
 </file>
@@ -1207,7 +1219,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1242,9 +1254,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1317,9 +1326,6 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1437,9 +1443,6 @@
     <xf numFmtId="49" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1482,6 +1485,15 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1491,15 +1503,6 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1511,6 +1514,27 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="5" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1891,7 +1915,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G21" sqref="G21"/>
+      <selection pane="bottomLeft" activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1899,10 +1923,10 @@
     <col min="1" max="1" width="10.140625" style="3" customWidth="1"/>
     <col min="2" max="2" width="12.7109375" style="3" customWidth="1"/>
     <col min="3" max="4" width="11.28515625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="44.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" style="16" customWidth="1"/>
+    <col min="5" max="6" width="44.85546875" style="13" customWidth="1"/>
+    <col min="7" max="7" width="12.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5703125" style="13" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="28.28515625" style="15" customWidth="1"/>
     <col min="10" max="10" width="13.85546875" style="2" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="35.5703125" style="1" bestFit="1" customWidth="1"/>
@@ -1916,1302 +1940,1313 @@
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="48" t="s">
-        <v>153</v>
+      <c r="C1" s="46" t="s">
+        <v>145</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="F1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="G1" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="G1" s="40" t="s">
+      <c r="H1" s="8" t="s">
+        <v>74</v>
+      </c>
+      <c r="I1" s="21" t="s">
         <v>32</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>77</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="41" t="s">
-        <v>134</v>
-      </c>
-      <c r="K1" s="43" t="s">
-        <v>135</v>
-      </c>
-      <c r="L1" s="42" t="s">
-        <v>144</v>
+      <c r="J1" s="39" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="41" t="s">
+        <v>127</v>
+      </c>
+      <c r="L1" s="40" t="s">
+        <v>136</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="92" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="95" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" s="89" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="57">
+      <c r="C2" s="55">
         <v>1</v>
       </c>
-      <c r="D2" s="58"/>
-      <c r="E2" s="17" t="s">
+      <c r="D2" s="56"/>
+      <c r="E2" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="30" t="s">
-        <v>57</v>
-      </c>
-      <c r="G2" s="69" t="s">
-        <v>34</v>
-      </c>
-      <c r="H2" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="49" t="s">
+      <c r="F2" s="29" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="J2" s="79" t="s">
-        <v>35</v>
-      </c>
-      <c r="K2" s="87"/>
-      <c r="L2" s="45" t="s">
-        <v>156</v>
+      <c r="I2" s="47" t="s">
+        <v>56</v>
+      </c>
+      <c r="J2" s="76" t="s">
+        <v>34</v>
+      </c>
+      <c r="K2" s="84"/>
+      <c r="L2" s="43" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="93"/>
-      <c r="B3" s="96"/>
-      <c r="C3" s="59">
+      <c r="B3" s="90"/>
+      <c r="C3" s="57">
         <v>2</v>
       </c>
-      <c r="D3" s="60">
+      <c r="D3" s="58">
         <v>1</v>
       </c>
       <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="31" t="s">
-        <v>58</v>
-      </c>
-      <c r="G3" s="70" t="s">
-        <v>34</v>
+      <c r="F3" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="68" t="s">
+        <v>33</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>67</v>
-      </c>
-      <c r="I3" s="50" t="s">
-        <v>63</v>
-      </c>
-      <c r="J3" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="K3" s="85"/>
-      <c r="L3" s="46" t="s">
-        <v>136</v>
+        <v>64</v>
+      </c>
+      <c r="I3" s="48" t="s">
+        <v>60</v>
+      </c>
+      <c r="J3" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="82"/>
+      <c r="L3" s="44" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="93"/>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="59">
+      <c r="C4" s="57">
         <v>3</v>
       </c>
-      <c r="D4" s="60"/>
-      <c r="E4" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="F4" s="32" t="s">
-        <v>61</v>
-      </c>
-      <c r="G4" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="H4" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="I4" s="51" t="s">
-        <v>139</v>
-      </c>
-      <c r="J4" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="K4" s="85"/>
-      <c r="L4" s="46" t="s">
-        <v>156</v>
+      <c r="D4" s="58"/>
+      <c r="E4" s="17" t="s">
+        <v>129</v>
+      </c>
+      <c r="F4" s="31" t="s">
+        <v>58</v>
+      </c>
+      <c r="G4" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="17" t="s">
+        <v>130</v>
+      </c>
+      <c r="I4" s="49" t="s">
+        <v>131</v>
+      </c>
+      <c r="J4" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="82"/>
+      <c r="L4" s="44" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="93"/>
-      <c r="B5" s="96"/>
-      <c r="C5" s="59">
+      <c r="B5" s="90"/>
+      <c r="C5" s="57">
         <v>4</v>
       </c>
-      <c r="D5" s="60"/>
-      <c r="E5" s="18" t="s">
+      <c r="D5" s="58"/>
+      <c r="E5" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="32" t="s">
-        <v>60</v>
-      </c>
-      <c r="G5" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="H5" s="18" t="s">
-        <v>68</v>
-      </c>
-      <c r="I5" s="51" t="s">
-        <v>66</v>
-      </c>
-      <c r="J5" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="85"/>
-      <c r="L5" s="46" t="s">
-        <v>156</v>
+      <c r="F5" s="31" t="s">
+        <v>57</v>
+      </c>
+      <c r="G5" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="I5" s="49" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="K5" s="82"/>
+      <c r="L5" s="44" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="93"/>
-      <c r="B6" s="96" t="s">
+      <c r="B6" s="90" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="59">
+      <c r="C6" s="57">
         <v>5</v>
       </c>
-      <c r="D6" s="60">
+      <c r="D6" s="58">
         <v>2</v>
       </c>
-      <c r="E6" s="20" t="s">
+      <c r="E6" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="33" t="s">
-        <v>141</v>
-      </c>
-      <c r="G6" s="72" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I6" s="52" t="s">
-        <v>142</v>
-      </c>
-      <c r="J6" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="K6" s="85"/>
-      <c r="L6" s="46"/>
+      <c r="F6" s="32" t="s">
+        <v>133</v>
+      </c>
+      <c r="G6" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="H6" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I6" s="50" t="s">
+        <v>134</v>
+      </c>
+      <c r="J6" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="82"/>
+      <c r="L6" s="44"/>
     </row>
     <row r="7" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="94"/>
-      <c r="B7" s="97"/>
-      <c r="C7" s="61">
+      <c r="B7" s="91"/>
+      <c r="C7" s="59">
         <v>6</v>
       </c>
-      <c r="D7" s="62">
+      <c r="D7" s="60">
         <f t="shared" ref="D7:D42" si="0">D6+1</f>
         <v>3</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="34" t="s">
-        <v>64</v>
-      </c>
-      <c r="G7" s="73" t="s">
-        <v>34</v>
-      </c>
-      <c r="H7" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="I7" s="53" t="s">
-        <v>65</v>
-      </c>
-      <c r="J7" s="81" t="s">
-        <v>35</v>
-      </c>
-      <c r="K7" s="88"/>
-      <c r="L7" s="47"/>
+      <c r="F7" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="H7" s="20" t="s">
+        <v>76</v>
+      </c>
+      <c r="I7" s="51" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" s="78" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="85"/>
+      <c r="L7" s="45"/>
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="92" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="95" t="s">
+      <c r="B8" s="89" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="57">
+      <c r="C8" s="55">
         <v>7</v>
       </c>
-      <c r="D8" s="58">
+      <c r="D8" s="56">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="E8" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F8" s="38" t="s">
-        <v>69</v>
-      </c>
-      <c r="G8" s="74" t="s">
-        <v>34</v>
+        <v>68</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>66</v>
+      </c>
+      <c r="G8" s="72" t="s">
+        <v>33</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="I8" s="54" t="s">
-        <v>70</v>
-      </c>
-      <c r="J8" s="82" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="89"/>
-      <c r="L8" s="45"/>
+        <v>135</v>
+      </c>
+      <c r="I8" s="52" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="79" t="s">
+        <v>34</v>
+      </c>
+      <c r="K8" s="86"/>
+      <c r="L8" s="43"/>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A9" s="93"/>
-      <c r="B9" s="96"/>
-      <c r="C9" s="59">
+      <c r="B9" s="90"/>
+      <c r="C9" s="57">
         <v>8</v>
       </c>
-      <c r="D9" s="60">
+      <c r="D9" s="58">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="F9" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="G9" s="70" t="s">
-        <v>34</v>
+        <v>69</v>
+      </c>
+      <c r="F9" s="30" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" s="68" t="s">
+        <v>33</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="I9" s="50" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="K9" s="85"/>
-      <c r="L9" s="46" t="s">
-        <v>145</v>
+        <v>135</v>
+      </c>
+      <c r="I9" s="48" t="s">
+        <v>67</v>
+      </c>
+      <c r="J9" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="K9" s="82"/>
+      <c r="L9" s="44" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="93"/>
-      <c r="B10" s="96"/>
-      <c r="C10" s="59">
+      <c r="B10" s="90"/>
+      <c r="C10" s="57">
         <v>9</v>
       </c>
-      <c r="D10" s="60">
+      <c r="D10" s="58">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="E10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="31" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" s="70" t="s">
-        <v>34</v>
+      <c r="F10" s="30" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="68" t="s">
+        <v>33</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>150</v>
-      </c>
-      <c r="I10" s="50" t="s">
-        <v>75</v>
-      </c>
-      <c r="J10" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="K10" s="85"/>
-      <c r="L10" s="46" t="s">
-        <v>146</v>
+        <v>142</v>
+      </c>
+      <c r="I10" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="J10" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="K10" s="82"/>
+      <c r="L10" s="44" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A11" s="93"/>
-      <c r="B11" s="96" t="s">
+      <c r="B11" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="59">
+      <c r="C11" s="57">
         <v>10</v>
       </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="18" t="s">
-        <v>76</v>
-      </c>
-      <c r="F11" s="32" t="s">
-        <v>140</v>
-      </c>
-      <c r="G11" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="H11" s="18" t="s">
-        <v>67</v>
-      </c>
-      <c r="I11" s="51" t="s">
-        <v>80</v>
-      </c>
-      <c r="J11" s="80" t="s">
-        <v>34</v>
-      </c>
-      <c r="K11" s="85" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" s="46" t="s">
-        <v>152</v>
+      <c r="D11" s="58"/>
+      <c r="E11" s="17" t="s">
+        <v>73</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>132</v>
+      </c>
+      <c r="G11" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="I11" s="49" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="K11" s="82" t="s">
+        <v>33</v>
+      </c>
+      <c r="L11" s="44" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="93"/>
-      <c r="B12" s="96"/>
-      <c r="C12" s="59">
+      <c r="B12" s="90"/>
+      <c r="C12" s="57">
         <v>11</v>
       </c>
-      <c r="D12" s="60">
+      <c r="D12" s="58">
         <v>7</v>
       </c>
       <c r="E12" s="10" t="s">
-        <v>147</v>
-      </c>
-      <c r="F12" s="31" t="s">
-        <v>149</v>
-      </c>
-      <c r="G12" s="70" t="s">
-        <v>34</v>
+        <v>139</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>141</v>
+      </c>
+      <c r="G12" s="68" t="s">
+        <v>33</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>148</v>
-      </c>
-      <c r="I12" s="50" t="s">
-        <v>81</v>
-      </c>
-      <c r="J12" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="K12" s="85"/>
-      <c r="L12" s="46"/>
+        <v>140</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>78</v>
+      </c>
+      <c r="J12" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="K12" s="82"/>
+      <c r="L12" s="44"/>
     </row>
     <row r="13" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="94"/>
-      <c r="B13" s="97"/>
-      <c r="C13" s="61">
+      <c r="B13" s="91"/>
+      <c r="C13" s="59">
         <v>12</v>
       </c>
-      <c r="D13" s="62">
+      <c r="D13" s="60">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="E13" s="21" t="s">
+      <c r="E13" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="34" t="s">
-        <v>82</v>
-      </c>
-      <c r="G13" s="73" t="s">
-        <v>34</v>
-      </c>
-      <c r="H13" s="21" t="s">
-        <v>155</v>
-      </c>
-      <c r="I13" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="J13" s="83" t="s">
-        <v>35</v>
-      </c>
-      <c r="K13" s="86"/>
-      <c r="L13" s="47"/>
+      <c r="F13" s="33" t="s">
+        <v>79</v>
+      </c>
+      <c r="G13" s="71" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="I13" s="51" t="s">
+        <v>80</v>
+      </c>
+      <c r="J13" s="80" t="s">
+        <v>34</v>
+      </c>
+      <c r="K13" s="83"/>
+      <c r="L13" s="45"/>
     </row>
     <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="92" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="95" t="s">
+      <c r="B14" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="57">
+      <c r="C14" s="55">
         <v>13</v>
       </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="F14" s="36" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>151</v>
-      </c>
-      <c r="I14" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="J14" s="79" t="s">
-        <v>34</v>
-      </c>
-      <c r="K14" s="87"/>
-      <c r="L14" s="45" t="s">
-        <v>156</v>
+      <c r="D14" s="56"/>
+      <c r="E14" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>143</v>
+      </c>
+      <c r="I14" s="26" t="s">
+        <v>83</v>
+      </c>
+      <c r="J14" s="76" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="84"/>
+      <c r="L14" s="43" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="93"/>
-      <c r="B15" s="96"/>
-      <c r="C15" s="59">
+      <c r="B15" s="90"/>
+      <c r="C15" s="57">
         <v>14</v>
       </c>
-      <c r="D15" s="60"/>
-      <c r="E15" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="F15" s="32" t="s">
-        <v>100</v>
-      </c>
-      <c r="G15" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="H15" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="I15" s="24" t="s">
-        <v>86</v>
-      </c>
-      <c r="J15" s="80" t="s">
-        <v>34</v>
-      </c>
-      <c r="K15" s="85"/>
-      <c r="L15" s="46" t="s">
-        <v>156</v>
+      <c r="D15" s="58"/>
+      <c r="E15" s="17" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="31" t="s">
+        <v>97</v>
+      </c>
+      <c r="G15" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="I15" s="23" t="s">
+        <v>83</v>
+      </c>
+      <c r="J15" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="82"/>
+      <c r="L15" s="44" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="93"/>
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="90" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="59">
+      <c r="C16" s="57">
         <v>15</v>
       </c>
-      <c r="D16" s="60">
+      <c r="D16" s="58">
         <v>9</v>
       </c>
-      <c r="E16" s="20" t="s">
+      <c r="E16" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="F16" s="33" t="s">
-        <v>97</v>
-      </c>
-      <c r="G16" s="72" t="s">
-        <v>35</v>
-      </c>
-      <c r="H16" s="20" t="s">
-        <v>95</v>
-      </c>
-      <c r="I16" s="25" t="s">
-        <v>96</v>
-      </c>
-      <c r="J16" s="80"/>
-      <c r="K16" s="85"/>
-      <c r="L16" s="46"/>
+      <c r="F16" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="G16" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="I16" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="J16" s="77"/>
+      <c r="K16" s="82"/>
+      <c r="L16" s="44"/>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="93"/>
-      <c r="B17" s="96"/>
-      <c r="C17" s="59">
+      <c r="B17" s="90"/>
+      <c r="C17" s="57">
         <v>16</v>
       </c>
-      <c r="D17" s="60"/>
-      <c r="E17" s="18" t="s">
+      <c r="D17" s="58"/>
+      <c r="E17" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="F17" s="32" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="H17" s="18" t="s">
+      <c r="F17" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="I17" s="24" t="s">
-        <v>96</v>
-      </c>
-      <c r="J17" s="80" t="s">
-        <v>34</v>
-      </c>
-      <c r="K17" s="85"/>
-      <c r="L17" s="46" t="s">
-        <v>156</v>
+      <c r="G17" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="17" t="s">
+        <v>92</v>
+      </c>
+      <c r="I17" s="23" t="s">
+        <v>93</v>
+      </c>
+      <c r="J17" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="82"/>
+      <c r="L17" s="44" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A18" s="93"/>
-      <c r="B18" s="96" t="s">
+      <c r="B18" s="90" t="s">
         <v>14</v>
       </c>
-      <c r="C18" s="59">
+      <c r="C18" s="57">
         <v>17</v>
       </c>
-      <c r="D18" s="60">
+      <c r="D18" s="58">
         <v>10</v>
       </c>
-      <c r="E18" s="20" t="s">
-        <v>158</v>
-      </c>
-      <c r="F18" s="33" t="s">
-        <v>159</v>
-      </c>
-      <c r="G18" s="72" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" s="20" t="s">
-        <v>157</v>
-      </c>
-      <c r="I18" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="J18" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="K18" s="85"/>
-      <c r="L18" s="46" t="s">
-        <v>163</v>
+      <c r="E18" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="F18" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="G18" s="70" t="s">
+        <v>34</v>
+      </c>
+      <c r="H18" s="19" t="s">
+        <v>149</v>
+      </c>
+      <c r="I18" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="J18" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="K18" s="82"/>
+      <c r="L18" s="44" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="93"/>
-      <c r="B19" s="96"/>
-      <c r="C19" s="59">
+      <c r="B19" s="90"/>
+      <c r="C19" s="57">
         <v>18</v>
       </c>
-      <c r="D19" s="60"/>
-      <c r="E19" s="91" t="s">
+      <c r="D19" s="58"/>
+      <c r="E19" s="88" t="s">
         <v>19</v>
       </c>
-      <c r="F19" s="32" t="s">
-        <v>103</v>
-      </c>
-      <c r="G19" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="I19" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="J19" s="80" t="s">
-        <v>34</v>
-      </c>
-      <c r="K19" s="85"/>
-      <c r="L19" s="46" t="s">
-        <v>160</v>
+      <c r="F19" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="G19" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="H19" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="I19" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J19" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="K19" s="82"/>
+      <c r="L19" s="44" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="93"/>
-      <c r="B20" s="96"/>
-      <c r="C20" s="59">
+      <c r="B20" s="90"/>
+      <c r="C20" s="57">
         <v>19</v>
       </c>
-      <c r="D20" s="60">
+      <c r="D20" s="58">
         <v>11</v>
       </c>
-      <c r="E20" s="20" t="s">
-        <v>162</v>
-      </c>
-      <c r="F20" s="33" t="s">
-        <v>166</v>
-      </c>
-      <c r="G20" s="72" t="s">
-        <v>34</v>
-      </c>
-      <c r="H20" s="20" t="s">
-        <v>165</v>
-      </c>
-      <c r="I20" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="J20" s="80" t="s">
-        <v>35</v>
-      </c>
-      <c r="K20" s="85"/>
-      <c r="L20" s="46"/>
+      <c r="E20" s="19" t="s">
+        <v>154</v>
+      </c>
+      <c r="F20" s="32" t="s">
+        <v>158</v>
+      </c>
+      <c r="G20" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="19" t="s">
+        <v>157</v>
+      </c>
+      <c r="I20" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="J20" s="77" t="s">
+        <v>34</v>
+      </c>
+      <c r="K20" s="82"/>
+      <c r="L20" s="44"/>
     </row>
     <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A21" s="93"/>
-      <c r="B21" s="96"/>
-      <c r="C21" s="59">
+      <c r="B21" s="90"/>
+      <c r="C21" s="57">
         <v>20</v>
       </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="18" t="s">
+      <c r="D21" s="58"/>
+      <c r="E21" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="32" t="s">
-        <v>105</v>
-      </c>
-      <c r="G21" s="71" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>161</v>
-      </c>
-      <c r="I21" s="24" t="s">
+      <c r="F21" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="J21" s="80" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" s="85"/>
-      <c r="L21" s="46" t="s">
-        <v>164</v>
+      <c r="G21" s="69" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="17" t="s">
+        <v>153</v>
+      </c>
+      <c r="I21" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J21" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="K21" s="82"/>
+      <c r="L21" s="44" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="93"/>
-      <c r="B22" s="96"/>
-      <c r="C22" s="59">
+      <c r="B22" s="90"/>
+      <c r="C22" s="57">
         <v>21</v>
       </c>
-      <c r="D22" s="60"/>
-      <c r="E22" s="18" t="s">
+      <c r="D22" s="58"/>
+      <c r="E22" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="32" t="s">
-        <v>106</v>
-      </c>
-      <c r="G22" s="71" t="s">
-        <v>35</v>
-      </c>
-      <c r="H22" s="18" t="s">
-        <v>104</v>
-      </c>
-      <c r="I22" s="24" t="s">
-        <v>102</v>
-      </c>
-      <c r="J22" s="80" t="s">
-        <v>34</v>
-      </c>
-      <c r="K22" s="85"/>
-      <c r="L22" s="46" t="s">
-        <v>160</v>
+      <c r="F22" s="31" t="s">
+        <v>103</v>
+      </c>
+      <c r="G22" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="17" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J22" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" s="82"/>
+      <c r="L22" s="44" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A23" s="93"/>
-      <c r="B23" s="96"/>
-      <c r="C23" s="59">
+      <c r="B23" s="90"/>
+      <c r="C23" s="57">
         <v>22</v>
       </c>
-      <c r="D23" s="60">
+      <c r="D23" s="58">
         <v>12</v>
       </c>
-      <c r="E23" s="20" t="s">
+      <c r="E23" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="F23" s="33" t="s">
-        <v>108</v>
-      </c>
-      <c r="G23" s="72" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="20" t="s">
-        <v>67</v>
-      </c>
-      <c r="I23" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="J23" s="80"/>
-      <c r="K23" s="85"/>
-      <c r="L23" s="46"/>
+      <c r="F23" s="32" t="s">
+        <v>105</v>
+      </c>
+      <c r="G23" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="H23" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="I23" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="J23" s="77"/>
+      <c r="K23" s="82"/>
+      <c r="L23" s="44"/>
     </row>
     <row r="24" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A24" s="93"/>
-      <c r="B24" s="96" t="s">
+      <c r="B24" s="90" t="s">
         <v>27</v>
       </c>
-      <c r="C24" s="59">
+      <c r="C24" s="57">
         <v>23</v>
       </c>
-      <c r="D24" s="60">
+      <c r="D24" s="58">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="E24" s="10" t="s">
-        <v>109</v>
-      </c>
-      <c r="F24" s="31" t="s">
-        <v>110</v>
-      </c>
-      <c r="G24" s="70" t="s">
-        <v>35</v>
+        <v>165</v>
+      </c>
+      <c r="F24" s="30" t="s">
+        <v>167</v>
+      </c>
+      <c r="G24" s="68" t="s">
+        <v>34</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="I24" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="J24" s="80"/>
-      <c r="K24" s="85"/>
-      <c r="L24" s="46"/>
+        <v>91</v>
+      </c>
+      <c r="I24" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="J24" s="77"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="44"/>
     </row>
     <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="93"/>
-      <c r="B25" s="96"/>
-      <c r="C25" s="59">
+      <c r="B25" s="90"/>
+      <c r="C25" s="57">
         <v>24</v>
       </c>
-      <c r="D25" s="60">
-        <f t="shared" si="0"/>
+      <c r="D25" s="58"/>
+      <c r="E25" s="17" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="31" t="s">
+        <v>106</v>
+      </c>
+      <c r="G25" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="H25" s="17" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J25" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="82"/>
+      <c r="L25" s="44" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A26" s="93"/>
+      <c r="B26" s="90"/>
+      <c r="C26" s="57">
+        <v>25</v>
+      </c>
+      <c r="D26" s="58">
         <v>14</v>
       </c>
-      <c r="E25" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="31" t="s">
-        <v>111</v>
-      </c>
-      <c r="G25" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="H25" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="I25" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="J25" s="80"/>
-      <c r="K25" s="85"/>
-      <c r="L25" s="46"/>
-    </row>
-    <row r="26" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A26" s="93"/>
-      <c r="B26" s="96"/>
-      <c r="C26" s="59">
-        <v>25</v>
-      </c>
-      <c r="D26" s="60">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
       <c r="E26" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="F26" s="31" t="s">
-        <v>113</v>
-      </c>
-      <c r="G26" s="70" t="s">
-        <v>34</v>
+        <v>168</v>
+      </c>
+      <c r="F26" s="30" t="s">
+        <v>169</v>
+      </c>
+      <c r="G26" s="68" t="s">
+        <v>33</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="I26" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="J26" s="80"/>
-      <c r="K26" s="85"/>
-      <c r="L26" s="46"/>
+        <v>107</v>
+      </c>
+      <c r="I26" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="J26" s="77"/>
+      <c r="K26" s="82"/>
+      <c r="L26" s="44"/>
     </row>
     <row r="27" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="94"/>
-      <c r="B27" s="97"/>
-      <c r="C27" s="61">
+      <c r="B27" s="91"/>
+      <c r="C27" s="59">
         <v>26</v>
       </c>
-      <c r="D27" s="62">
+      <c r="D27" s="60"/>
+      <c r="E27" s="102" t="s">
+        <v>28</v>
+      </c>
+      <c r="F27" s="103" t="s">
+        <v>108</v>
+      </c>
+      <c r="G27" s="104" t="s">
+        <v>34</v>
+      </c>
+      <c r="H27" s="102" t="s">
+        <v>107</v>
+      </c>
+      <c r="I27" s="105" t="s">
+        <v>99</v>
+      </c>
+      <c r="J27" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="K27" s="85"/>
+      <c r="L27" s="45" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A28" s="95" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" s="97" t="s">
+        <v>35</v>
+      </c>
+      <c r="C28" s="61">
+        <v>27</v>
+      </c>
+      <c r="D28" s="62"/>
+      <c r="E28" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F28" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="G28" s="73" t="s">
+        <v>34</v>
+      </c>
+      <c r="H28" s="18" t="s">
+        <v>109</v>
+      </c>
+      <c r="I28" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="J28" s="79" t="s">
+        <v>33</v>
+      </c>
+      <c r="K28" s="86"/>
+      <c r="L28" s="43" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="93"/>
+      <c r="B29" s="90"/>
+      <c r="C29" s="57">
+        <v>28</v>
+      </c>
+      <c r="D29" s="58">
+        <v>15</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="F29" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="G29" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="19" t="s">
+        <v>111</v>
+      </c>
+      <c r="I29" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="J29" s="77"/>
+      <c r="K29" s="82"/>
+      <c r="L29" s="44"/>
+    </row>
+    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="93"/>
+      <c r="B30" s="90"/>
+      <c r="C30" s="57">
+        <v>29</v>
+      </c>
+      <c r="D30" s="58">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="E27" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="F27" s="35" t="s">
-        <v>114</v>
-      </c>
-      <c r="G27" s="76" t="s">
-        <v>35</v>
-      </c>
-      <c r="H27" s="11" t="s">
+      <c r="E30" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="F30" s="32" t="s">
+        <v>113</v>
+      </c>
+      <c r="G30" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="I27" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="J27" s="81"/>
-      <c r="K27" s="88"/>
-      <c r="L27" s="47"/>
-    </row>
-    <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="98" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="100" t="s">
+      <c r="I30" s="24" t="s">
+        <v>99</v>
+      </c>
+      <c r="J30" s="77"/>
+      <c r="K30" s="82"/>
+      <c r="L30" s="44"/>
+    </row>
+    <row r="31" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="93"/>
+      <c r="B31" s="90" t="s">
         <v>36</v>
       </c>
-      <c r="C28" s="63">
-        <v>27</v>
-      </c>
-      <c r="D28" s="64">
+      <c r="C31" s="57">
+        <v>30</v>
+      </c>
+      <c r="D31" s="58">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="E28" s="19" t="s">
-        <v>116</v>
-      </c>
-      <c r="F28" s="36" t="s">
-        <v>101</v>
-      </c>
-      <c r="G28" s="75" t="s">
-        <v>35</v>
-      </c>
-      <c r="H28" s="19" t="s">
-        <v>115</v>
-      </c>
-      <c r="I28" s="27" t="s">
-        <v>78</v>
-      </c>
-      <c r="J28" s="82"/>
-      <c r="K28" s="89"/>
-      <c r="L28" s="45"/>
-    </row>
-    <row r="29" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="93"/>
-      <c r="B29" s="96"/>
-      <c r="C29" s="59">
-        <v>28</v>
-      </c>
-      <c r="D29" s="60">
+      <c r="E31" s="10" t="s">
+        <v>159</v>
+      </c>
+      <c r="F31" s="30" t="s">
+        <v>160</v>
+      </c>
+      <c r="G31" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="I31" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="J31" s="77"/>
+      <c r="K31" s="82"/>
+      <c r="L31" s="44"/>
+    </row>
+    <row r="32" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="93"/>
+      <c r="B32" s="90"/>
+      <c r="C32" s="57">
+        <v>31</v>
+      </c>
+      <c r="D32" s="58">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="E29" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="33" t="s">
+      <c r="E32" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>163</v>
+      </c>
+      <c r="G32" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="I32" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="J32" s="77"/>
+      <c r="K32" s="82"/>
+      <c r="L32" s="44"/>
+    </row>
+    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="93"/>
+      <c r="B33" s="90"/>
+      <c r="C33" s="57">
+        <v>32</v>
+      </c>
+      <c r="D33" s="58"/>
+      <c r="E33" s="17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F33" s="31" t="s">
+        <v>120</v>
+      </c>
+      <c r="G33" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="I33" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J33" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="K33" s="82"/>
+      <c r="L33" s="44" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="93"/>
+      <c r="B34" s="90"/>
+      <c r="C34" s="57">
+        <v>33</v>
+      </c>
+      <c r="D34" s="58"/>
+      <c r="E34" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="F34" s="31" t="s">
+        <v>121</v>
+      </c>
+      <c r="G34" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="17" t="s">
         <v>119</v>
       </c>
-      <c r="G29" s="72" t="s">
-        <v>34</v>
-      </c>
-      <c r="H29" s="20" t="s">
+      <c r="I34" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J34" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" s="82"/>
+      <c r="L34" s="44" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35" s="93"/>
+      <c r="B35" s="90"/>
+      <c r="C35" s="57">
+        <v>34</v>
+      </c>
+      <c r="D35" s="58"/>
+      <c r="E35" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F35" s="31" t="s">
+        <v>116</v>
+      </c>
+      <c r="G35" s="69" t="s">
+        <v>34</v>
+      </c>
+      <c r="H35" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="I35" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J35" s="77" t="s">
+        <v>33</v>
+      </c>
+      <c r="K35" s="82"/>
+      <c r="L35" s="44" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="96"/>
+      <c r="B36" s="98"/>
+      <c r="C36" s="63">
+        <v>35</v>
+      </c>
+      <c r="D36" s="64"/>
+      <c r="E36" s="99" t="s">
+        <v>50</v>
+      </c>
+      <c r="F36" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="I29" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="J29" s="80"/>
-      <c r="K29" s="85"/>
-      <c r="L29" s="46"/>
-    </row>
-    <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="93"/>
-      <c r="B30" s="96"/>
-      <c r="C30" s="59">
-        <v>29</v>
-      </c>
-      <c r="D30" s="60">
-        <f t="shared" si="0"/>
+      <c r="G36" s="101" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" s="17" t="s">
+        <v>119</v>
+      </c>
+      <c r="I36" s="23" t="s">
+        <v>99</v>
+      </c>
+      <c r="J36" s="80" t="s">
+        <v>33</v>
+      </c>
+      <c r="K36" s="83"/>
+      <c r="L36" s="45" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="92" t="s">
+        <v>84</v>
+      </c>
+      <c r="B37" s="89" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="55">
+        <v>36</v>
+      </c>
+      <c r="D37" s="56">
         <v>19</v>
       </c>
-      <c r="E30" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="F30" s="33" t="s">
-        <v>119</v>
-      </c>
-      <c r="G30" s="72" t="s">
-        <v>34</v>
-      </c>
-      <c r="H30" s="20" t="s">
-        <v>118</v>
-      </c>
-      <c r="I30" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="J30" s="80"/>
-      <c r="K30" s="85"/>
-      <c r="L30" s="46"/>
-    </row>
-    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="93"/>
-      <c r="B31" s="96" t="s">
+      <c r="E37" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="F37" s="36" t="s">
+        <v>122</v>
+      </c>
+      <c r="G37" s="72" t="s">
+        <v>34</v>
+      </c>
+      <c r="H37" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="I37" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="J37" s="76"/>
+      <c r="K37" s="84"/>
+      <c r="L37" s="43"/>
+    </row>
+    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="93"/>
+      <c r="B38" s="90"/>
+      <c r="C38" s="57">
         <v>37</v>
       </c>
-      <c r="C31" s="59">
-        <v>30</v>
-      </c>
-      <c r="D31" s="60">
+      <c r="D38" s="58">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="E31" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="F31" s="31" t="s">
-        <v>121</v>
-      </c>
-      <c r="G31" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="I31" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="J31" s="80"/>
-      <c r="K31" s="85"/>
-      <c r="L31" s="46"/>
-    </row>
-    <row r="32" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="93"/>
-      <c r="B32" s="96"/>
-      <c r="C32" s="59">
-        <v>31</v>
-      </c>
-      <c r="D32" s="60">
+      <c r="E38" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="F38" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G38" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="H38" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="I38" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="J38" s="77"/>
+      <c r="K38" s="82"/>
+      <c r="L38" s="44"/>
+    </row>
+    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="93"/>
+      <c r="B39" s="90" t="s">
+        <v>45</v>
+      </c>
+      <c r="C39" s="57">
+        <v>38</v>
+      </c>
+      <c r="D39" s="58">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="E32" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="F32" s="31" t="s">
+      <c r="E39" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="F39" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G39" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="I39" s="22" t="s">
         <v>123</v>
       </c>
-      <c r="G32" s="70" t="s">
-        <v>34</v>
-      </c>
-      <c r="H32" s="10" t="s">
-        <v>122</v>
-      </c>
-      <c r="I32" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="J32" s="80"/>
-      <c r="K32" s="85"/>
-      <c r="L32" s="46"/>
-    </row>
-    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="93"/>
-      <c r="B33" s="96"/>
-      <c r="C33" s="59">
-        <v>32</v>
-      </c>
-      <c r="D33" s="60">
+      <c r="J39" s="77"/>
+      <c r="K39" s="82"/>
+      <c r="L39" s="44"/>
+    </row>
+    <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="93"/>
+      <c r="B40" s="90"/>
+      <c r="C40" s="57">
+        <v>39</v>
+      </c>
+      <c r="D40" s="58">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="E33" s="10" t="s">
+      <c r="E40" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="F40" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="G40" s="68" t="s">
+        <v>34</v>
+      </c>
+      <c r="H40" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="I40" s="22" t="s">
+        <v>123</v>
+      </c>
+      <c r="J40" s="77"/>
+      <c r="K40" s="82"/>
+      <c r="L40" s="44"/>
+    </row>
+    <row r="41" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="94"/>
+      <c r="B41" s="91"/>
+      <c r="C41" s="59">
         <v>40</v>
       </c>
-      <c r="F33" s="31" t="s">
-        <v>128</v>
-      </c>
-      <c r="G33" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="I33" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="J33" s="80"/>
-      <c r="K33" s="85"/>
-      <c r="L33" s="46"/>
-    </row>
-    <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="93"/>
-      <c r="B34" s="96"/>
-      <c r="C34" s="59">
-        <v>33</v>
-      </c>
-      <c r="D34" s="60">
+      <c r="D41" s="60">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E41" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="F41" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="G41" s="74" t="s">
+        <v>34</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="I41" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="J41" s="78"/>
+      <c r="K41" s="85"/>
+      <c r="L41" s="45"/>
+    </row>
+    <row r="42" spans="1:12" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="53" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="C42" s="65">
         <v>41</v>
       </c>
-      <c r="F34" s="31" t="s">
-        <v>129</v>
-      </c>
-      <c r="G34" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="H34" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="I34" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="J34" s="80"/>
-      <c r="K34" s="85"/>
-      <c r="L34" s="46"/>
-    </row>
-    <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="93"/>
-      <c r="B35" s="96"/>
-      <c r="C35" s="59">
-        <v>34</v>
-      </c>
-      <c r="D35" s="60">
+      <c r="D42" s="66">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="E35" s="10" t="s">
+      <c r="E42" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="F35" s="31" t="s">
+      <c r="F42" s="37" t="s">
         <v>124</v>
       </c>
-      <c r="G35" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="H35" s="10" t="s">
-        <v>126</v>
-      </c>
-      <c r="I35" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="J35" s="80"/>
-      <c r="K35" s="85"/>
-      <c r="L35" s="46"/>
-    </row>
-    <row r="36" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="99"/>
-      <c r="B36" s="101"/>
-      <c r="C36" s="65">
-        <v>35</v>
-      </c>
-      <c r="D36" s="66">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="E36" s="12" t="s">
-        <v>53</v>
-      </c>
-      <c r="F36" s="37" t="s">
+      <c r="G42" s="75" t="s">
+        <v>34</v>
+      </c>
+      <c r="H42" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="I42" s="28" t="s">
         <v>125</v>
       </c>
-      <c r="G36" s="77" t="s">
-        <v>35</v>
-      </c>
-      <c r="H36" s="10" t="s">
-        <v>127</v>
-      </c>
-      <c r="I36" s="23" t="s">
-        <v>102</v>
-      </c>
-      <c r="J36" s="83"/>
-      <c r="K36" s="86"/>
-      <c r="L36" s="47"/>
-    </row>
-    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="92" t="s">
-        <v>87</v>
-      </c>
-      <c r="B37" s="95" t="s">
-        <v>44</v>
-      </c>
-      <c r="C37" s="57">
-        <v>36</v>
-      </c>
-      <c r="D37" s="58">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="E37" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="F37" s="38" t="s">
-        <v>130</v>
-      </c>
-      <c r="G37" s="74" t="s">
-        <v>35</v>
-      </c>
-      <c r="H37" s="9" t="s">
-        <v>88</v>
-      </c>
-      <c r="I37" s="28" t="s">
-        <v>131</v>
-      </c>
-      <c r="J37" s="79"/>
-      <c r="K37" s="87"/>
-      <c r="L37" s="45"/>
-    </row>
-    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="93"/>
-      <c r="B38" s="96"/>
-      <c r="C38" s="59">
-        <v>37</v>
-      </c>
-      <c r="D38" s="60">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="F38" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="G38" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>89</v>
-      </c>
-      <c r="I38" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="J38" s="80"/>
-      <c r="K38" s="85"/>
-      <c r="L38" s="46"/>
-    </row>
-    <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="93"/>
-      <c r="B39" s="96" t="s">
-        <v>46</v>
-      </c>
-      <c r="C39" s="59">
-        <v>38</v>
-      </c>
-      <c r="D39" s="60">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="E39" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F39" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="G39" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="H39" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="I39" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="J39" s="80"/>
-      <c r="K39" s="85"/>
-      <c r="L39" s="46"/>
-    </row>
-    <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="93"/>
-      <c r="B40" s="96"/>
-      <c r="C40" s="59">
-        <v>39</v>
-      </c>
-      <c r="D40" s="60">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="E40" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="F40" s="31" t="s">
-        <v>130</v>
-      </c>
-      <c r="G40" s="70" t="s">
-        <v>35</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I40" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="J40" s="80"/>
-      <c r="K40" s="85"/>
-      <c r="L40" s="46"/>
-    </row>
-    <row r="41" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="94"/>
-      <c r="B41" s="97"/>
-      <c r="C41" s="61">
-        <v>40</v>
-      </c>
-      <c r="D41" s="62">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="F41" s="35" t="s">
-        <v>130</v>
-      </c>
-      <c r="G41" s="76" t="s">
-        <v>35</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="I41" s="26" t="s">
-        <v>131</v>
-      </c>
-      <c r="J41" s="81"/>
-      <c r="K41" s="88"/>
-      <c r="L41" s="47"/>
-    </row>
-    <row r="42" spans="1:12" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="55" t="s">
-        <v>43</v>
-      </c>
-      <c r="B42" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="C42" s="67">
-        <v>41</v>
-      </c>
-      <c r="D42" s="68">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="E42" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="F42" s="39" t="s">
-        <v>132</v>
-      </c>
-      <c r="G42" s="78" t="s">
-        <v>35</v>
-      </c>
-      <c r="H42" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="I42" s="29" t="s">
-        <v>133</v>
-      </c>
-      <c r="J42" s="84"/>
-      <c r="K42" s="90"/>
-      <c r="L42" s="44"/>
+      <c r="J42" s="81"/>
+      <c r="K42" s="87"/>
+      <c r="L42" s="42"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:L42" xr:uid="{370A0B0F-C0FD-4EC3-B4F7-C3AB5FE65C83}"/>
   <mergeCells count="18">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="A37:A41"/>
@@ -3223,13 +3258,6 @@
     <mergeCell ref="A28:A36"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B36"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:G1048576">
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Y">

</xml_diff>

<commit_message>
Added more detail to TC30
</commit_message>
<xml_diff>
--- a/TESTCASES/TestCases.xlsx
+++ b/TESTCASES/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andra\OneDrive - University of Greenwich\PhD\Application\ObjectController\TESTCASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F826D8-BBE6-4BC6-A9D7-04146219FE1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B9964E7-438A-45D6-888B-0AE1F88C94B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="178">
   <si>
     <t>Vertices and attachment points are correct relative to CoR</t>
   </si>
@@ -1527,6 +1527,15 @@
     <xf numFmtId="49" fontId="0" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1534,15 +1543,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1936,7 +1936,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I35" sqref="I35"/>
+      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1993,10 +1993,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="96" t="s">
+      <c r="A2" s="99" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="96" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="55">
@@ -2027,8 +2027,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="97"/>
-      <c r="B3" s="100"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="97"/>
       <c r="C3" s="57">
         <v>2</v>
       </c>
@@ -2059,8 +2059,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="97"/>
-      <c r="B4" s="100" t="s">
+      <c r="A4" s="100"/>
+      <c r="B4" s="97" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="57">
@@ -2091,8 +2091,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="97"/>
-      <c r="B5" s="100"/>
+      <c r="A5" s="100"/>
+      <c r="B5" s="97"/>
       <c r="C5" s="57">
         <v>4</v>
       </c>
@@ -2121,8 +2121,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="97"/>
-      <c r="B6" s="100" t="s">
+      <c r="A6" s="100"/>
+      <c r="B6" s="97" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="57">
@@ -2153,8 +2153,8 @@
       <c r="L6" s="44"/>
     </row>
     <row r="7" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="98"/>
-      <c r="B7" s="101"/>
+      <c r="A7" s="101"/>
+      <c r="B7" s="98"/>
       <c r="C7" s="59">
         <v>6</v>
       </c>
@@ -2183,10 +2183,10 @@
       <c r="L7" s="45"/>
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="96" t="s">
+      <c r="A8" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="99" t="s">
+      <c r="B8" s="96" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="55">
@@ -2217,8 +2217,8 @@
       <c r="L8" s="43"/>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="97"/>
-      <c r="B9" s="100"/>
+      <c r="A9" s="100"/>
+      <c r="B9" s="97"/>
       <c r="C9" s="57">
         <v>8</v>
       </c>
@@ -2249,8 +2249,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="97"/>
-      <c r="B10" s="100"/>
+      <c r="A10" s="100"/>
+      <c r="B10" s="97"/>
       <c r="C10" s="57">
         <v>9</v>
       </c>
@@ -2281,8 +2281,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="97"/>
-      <c r="B11" s="100" t="s">
+      <c r="A11" s="100"/>
+      <c r="B11" s="97" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="57">
@@ -2313,8 +2313,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="97"/>
-      <c r="B12" s="100"/>
+      <c r="A12" s="100"/>
+      <c r="B12" s="97"/>
       <c r="C12" s="57">
         <v>11</v>
       </c>
@@ -2343,8 +2343,8 @@
       <c r="L12" s="44"/>
     </row>
     <row r="13" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="98"/>
-      <c r="B13" s="101"/>
+      <c r="A13" s="101"/>
+      <c r="B13" s="98"/>
       <c r="C13" s="59">
         <v>12</v>
       </c>
@@ -2373,10 +2373,10 @@
       <c r="L13" s="45"/>
     </row>
     <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="96" t="s">
+      <c r="A14" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="99" t="s">
+      <c r="B14" s="96" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="55">
@@ -2407,8 +2407,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="97"/>
-      <c r="B15" s="100"/>
+      <c r="A15" s="100"/>
+      <c r="B15" s="97"/>
       <c r="C15" s="57">
         <v>14</v>
       </c>
@@ -2437,8 +2437,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A16" s="97"/>
-      <c r="B16" s="100" t="s">
+      <c r="A16" s="100"/>
+      <c r="B16" s="97" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="57">
@@ -2467,8 +2467,8 @@
       <c r="L16" s="44"/>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="97"/>
-      <c r="B17" s="100"/>
+      <c r="A17" s="100"/>
+      <c r="B17" s="97"/>
       <c r="C17" s="57">
         <v>16</v>
       </c>
@@ -2497,8 +2497,8 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="97"/>
-      <c r="B18" s="100" t="s">
+      <c r="A18" s="100"/>
+      <c r="B18" s="97" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="57">
@@ -2531,8 +2531,8 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="97"/>
-      <c r="B19" s="100"/>
+      <c r="A19" s="100"/>
+      <c r="B19" s="97"/>
       <c r="C19" s="57">
         <v>18</v>
       </c>
@@ -2561,8 +2561,8 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="97"/>
-      <c r="B20" s="100"/>
+      <c r="A20" s="100"/>
+      <c r="B20" s="97"/>
       <c r="C20" s="57">
         <v>19</v>
       </c>
@@ -2591,8 +2591,8 @@
       <c r="L20" s="44"/>
     </row>
     <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="97"/>
-      <c r="B21" s="100"/>
+      <c r="A21" s="100"/>
+      <c r="B21" s="97"/>
       <c r="C21" s="57">
         <v>20</v>
       </c>
@@ -2621,8 +2621,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="97"/>
-      <c r="B22" s="100"/>
+      <c r="A22" s="100"/>
+      <c r="B22" s="97"/>
       <c r="C22" s="57">
         <v>21</v>
       </c>
@@ -2651,8 +2651,8 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="97"/>
-      <c r="B23" s="100"/>
+      <c r="A23" s="100"/>
+      <c r="B23" s="97"/>
       <c r="C23" s="57">
         <v>22</v>
       </c>
@@ -2681,8 +2681,8 @@
       <c r="L23" s="44"/>
     </row>
     <row r="24" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="97"/>
-      <c r="B24" s="100" t="s">
+      <c r="A24" s="100"/>
+      <c r="B24" s="97" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="57">
@@ -2713,8 +2713,8 @@
       <c r="L24" s="44"/>
     </row>
     <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="97"/>
-      <c r="B25" s="100"/>
+      <c r="A25" s="100"/>
+      <c r="B25" s="97"/>
       <c r="C25" s="57">
         <v>24</v>
       </c>
@@ -2743,8 +2743,8 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="97"/>
-      <c r="B26" s="100"/>
+      <c r="A26" s="100"/>
+      <c r="B26" s="97"/>
       <c r="C26" s="57">
         <v>25</v>
       </c>
@@ -2775,8 +2775,8 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="98"/>
-      <c r="B27" s="101"/>
+      <c r="A27" s="101"/>
+      <c r="B27" s="98"/>
       <c r="C27" s="59">
         <v>26</v>
       </c>
@@ -2839,8 +2839,8 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="97"/>
-      <c r="B29" s="100"/>
+      <c r="A29" s="100"/>
+      <c r="B29" s="97"/>
       <c r="C29" s="57">
         <v>28</v>
       </c>
@@ -2869,8 +2869,8 @@
       <c r="L29" s="44"/>
     </row>
     <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="97"/>
-      <c r="B30" s="100"/>
+      <c r="A30" s="100"/>
+      <c r="B30" s="97"/>
       <c r="C30" s="57">
         <v>29</v>
       </c>
@@ -2899,8 +2899,8 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="97"/>
-      <c r="B31" s="100" t="s">
+      <c r="A31" s="100"/>
+      <c r="B31" s="97" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="57">
@@ -2924,13 +2924,15 @@
       <c r="I31" s="22" t="s">
         <v>167</v>
       </c>
-      <c r="J31" s="77"/>
+      <c r="J31" s="77" t="s">
+        <v>34</v>
+      </c>
       <c r="K31" s="82"/>
       <c r="L31" s="44"/>
     </row>
     <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="97"/>
-      <c r="B32" s="100"/>
+      <c r="A32" s="100"/>
+      <c r="B32" s="97"/>
       <c r="C32" s="57">
         <v>31</v>
       </c>
@@ -2959,8 +2961,8 @@
       </c>
     </row>
     <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="97"/>
-      <c r="B33" s="100"/>
+      <c r="A33" s="100"/>
+      <c r="B33" s="97"/>
       <c r="C33" s="57">
         <v>32</v>
       </c>
@@ -2989,8 +2991,8 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="97"/>
-      <c r="B34" s="100"/>
+      <c r="A34" s="100"/>
+      <c r="B34" s="97"/>
       <c r="C34" s="57">
         <v>33</v>
       </c>
@@ -3019,8 +3021,8 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="97"/>
-      <c r="B35" s="100"/>
+      <c r="A35" s="100"/>
+      <c r="B35" s="97"/>
       <c r="C35" s="57">
         <v>34</v>
       </c>
@@ -3079,10 +3081,10 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="96" t="s">
+      <c r="A37" s="99" t="s">
         <v>82</v>
       </c>
-      <c r="B37" s="99" t="s">
+      <c r="B37" s="96" t="s">
         <v>41</v>
       </c>
       <c r="C37" s="55">
@@ -3109,8 +3111,8 @@
       <c r="L37" s="43"/>
     </row>
     <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="97"/>
-      <c r="B38" s="100"/>
+      <c r="A38" s="100"/>
+      <c r="B38" s="97"/>
       <c r="C38" s="57">
         <v>37</v>
       </c>
@@ -3135,8 +3137,8 @@
       <c r="L38" s="44"/>
     </row>
     <row r="39" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="97"/>
-      <c r="B39" s="100" t="s">
+      <c r="A39" s="100"/>
+      <c r="B39" s="97" t="s">
         <v>43</v>
       </c>
       <c r="C39" s="57">
@@ -3163,8 +3165,8 @@
       <c r="L39" s="44"/>
     </row>
     <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="97"/>
-      <c r="B40" s="100"/>
+      <c r="A40" s="100"/>
+      <c r="B40" s="97"/>
       <c r="C40" s="57">
         <v>39</v>
       </c>
@@ -3189,8 +3191,8 @@
       <c r="L40" s="44"/>
     </row>
     <row r="41" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="98"/>
-      <c r="B41" s="101"/>
+      <c r="A41" s="101"/>
+      <c r="B41" s="98"/>
       <c r="C41" s="59">
         <v>40</v>
       </c>
@@ -3247,6 +3249,13 @@
   </sheetData>
   <autoFilter ref="A1:L42" xr:uid="{370A0B0F-C0FD-4EC3-B4F7-C3AB5FE65C83}"/>
   <mergeCells count="18">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="B37:B38"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="A37:A41"/>
@@ -3258,13 +3267,6 @@
     <mergeCell ref="A28:A36"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B36"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:G1048576">
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Y">

</xml_diff>

<commit_message>
All TC folder IDs *10 to make space for adding new ones between
</commit_message>
<xml_diff>
--- a/TESTCASES/TestCases.xlsx
+++ b/TESTCASES/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andra\OneDrive - University of Greenwich\PhD\Application\ObjectController\TESTCASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1EC2FBC-9DCC-4FC8-9F6D-8405EFA142C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6A1506-9207-4CC2-A561-3B115089963F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
   </bookViews>
@@ -389,9 +389,6 @@
     <t>Notes</t>
   </si>
   <si>
-    <t>Results are together with 7</t>
-  </si>
-  <si>
     <t>Layers in AI file may not correspond to orientation</t>
   </si>
   <si>
@@ -416,9 +413,6 @@
 Airport.mta</t>
   </si>
   <si>
-    <t>Removed as too similar to 5</t>
-  </si>
-  <si>
     <t>ID in Thesis</t>
   </si>
   <si>
@@ -435,42 +429,21 @@
     <t>Person and object detect immanent collisions and take action to avoid based on relative drives.</t>
   </si>
   <si>
-    <t>Done in TC17</t>
-  </si>
-  <si>
     <t>Rectangle_W4L40.csv</t>
   </si>
   <si>
     <t>Object and object detect immanent collisions and take action to avoid based on relative drives.</t>
   </si>
   <si>
-    <t>Combined with TC18 and 21</t>
-  </si>
-  <si>
-    <t>Done in TC19</t>
-  </si>
-  <si>
     <t>Corridor2.mta</t>
   </si>
   <si>
-    <t>Covered in TC 30</t>
-  </si>
-  <si>
-    <t>Covered in TC 31</t>
-  </si>
-  <si>
-    <t>Covered in TC 23</t>
-  </si>
-  <si>
     <t>Object/Person waits at entrance of thin corridor/doorway for object with higher drive to pass in contra-flow</t>
   </si>
   <si>
     <t>Object1 starts on thin side, Object2/person starts on wide side. Move counter. See if object2/person waits for object1. Try with different drives</t>
   </si>
   <si>
-    <t>Covered in TC25</t>
-  </si>
-  <si>
     <t>Object placed on left, goal on right. Let object move, add people to block its path, watch object move to edge of A* cor. Check cor is expanded</t>
   </si>
   <si>
@@ -537,9 +510,6 @@
     <t>Test 10 different combinations. Check all entities eventually end up at their goal (nothing gets stuck)</t>
   </si>
   <si>
-    <t>Could take a long time and not be worth it. Similar to TC 30</t>
-  </si>
-  <si>
     <t>Realistic Scenarios</t>
   </si>
   <si>
@@ -553,6 +523,36 @@
   </si>
   <si>
     <t>Set tasks for people to pick up and drop off object. Check they can do this and the appropriate prep time is achieved. Check multiple pickups work for same attendants</t>
+  </si>
+  <si>
+    <t>Results are together with 70</t>
+  </si>
+  <si>
+    <t>Removed as too similar to 50</t>
+  </si>
+  <si>
+    <t>Combined with TC180 and 210</t>
+  </si>
+  <si>
+    <t>Done in TC170</t>
+  </si>
+  <si>
+    <t>Done in TC190</t>
+  </si>
+  <si>
+    <t>Covered in TC 230</t>
+  </si>
+  <si>
+    <t>Covered in TC250</t>
+  </si>
+  <si>
+    <t>Could take a long time and not be worth it. Similar to TC 300</t>
+  </si>
+  <si>
+    <t>Covered in TC 300</t>
+  </si>
+  <si>
+    <t>Covered in TC 310</t>
   </si>
 </sst>
 </file>
@@ -1911,8 +1911,8 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G38" sqref="G38"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1938,10 +1938,10 @@
         <v>2</v>
       </c>
       <c r="C1" s="46" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>29</v>
@@ -1976,7 +1976,7 @@
         <v>3</v>
       </c>
       <c r="C2" s="54">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="D2" s="55"/>
       <c r="E2" s="16" t="s">
@@ -1999,18 +1999,16 @@
       </c>
       <c r="K2" s="83"/>
       <c r="L2" s="43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="100"/>
       <c r="B3" s="103"/>
       <c r="C3" s="56">
-        <v>2</v>
-      </c>
-      <c r="D3" s="57">
-        <v>1</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="D3" s="57"/>
       <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
@@ -2040,7 +2038,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="56">
-        <v>3</v>
+        <v>30</v>
       </c>
       <c r="D4" s="57"/>
       <c r="E4" s="17" t="s">
@@ -2063,14 +2061,14 @@
       </c>
       <c r="K4" s="81"/>
       <c r="L4" s="44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="100"/>
       <c r="B5" s="103"/>
       <c r="C5" s="56">
-        <v>4</v>
+        <v>40</v>
       </c>
       <c r="D5" s="57"/>
       <c r="E5" s="17" t="s">
@@ -2093,7 +2091,7 @@
       </c>
       <c r="K5" s="81"/>
       <c r="L5" s="44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -2102,11 +2100,9 @@
         <v>24</v>
       </c>
       <c r="C6" s="56">
-        <v>5</v>
-      </c>
-      <c r="D6" s="57">
-        <v>2</v>
-      </c>
+        <v>50</v>
+      </c>
+      <c r="D6" s="57"/>
       <c r="E6" s="19" t="s">
         <v>17</v>
       </c>
@@ -2132,11 +2128,9 @@
       <c r="A7" s="101"/>
       <c r="B7" s="104"/>
       <c r="C7" s="58">
-        <v>6</v>
-      </c>
-      <c r="D7" s="59">
-        <v>3</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="D7" s="59"/>
       <c r="E7" s="20" t="s">
         <v>18</v>
       </c>
@@ -2166,11 +2160,9 @@
         <v>7</v>
       </c>
       <c r="C8" s="54">
-        <v>7</v>
-      </c>
-      <c r="D8" s="55">
-        <v>4</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="D8" s="55"/>
       <c r="E8" s="9" t="s">
         <v>59</v>
       </c>
@@ -2196,11 +2188,9 @@
       <c r="A9" s="100"/>
       <c r="B9" s="103"/>
       <c r="C9" s="56">
-        <v>8</v>
-      </c>
-      <c r="D9" s="57">
-        <v>5</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="D9" s="57"/>
       <c r="E9" s="10" t="s">
         <v>60</v>
       </c>
@@ -2221,18 +2211,16 @@
       </c>
       <c r="K9" s="81"/>
       <c r="L9" s="44" t="s">
-        <v>114</v>
+        <v>157</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="100"/>
       <c r="B10" s="103"/>
       <c r="C10" s="56">
-        <v>9</v>
-      </c>
-      <c r="D10" s="57">
-        <v>6</v>
-      </c>
+        <v>90</v>
+      </c>
+      <c r="D10" s="57"/>
       <c r="E10" s="10" t="s">
         <v>9</v>
       </c>
@@ -2243,7 +2231,7 @@
         <v>33</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="I10" s="48" t="s">
         <v>63</v>
@@ -2253,7 +2241,7 @@
       </c>
       <c r="K10" s="81"/>
       <c r="L10" s="44" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -2262,7 +2250,7 @@
         <v>8</v>
       </c>
       <c r="C11" s="56">
-        <v>10</v>
+        <v>100</v>
       </c>
       <c r="D11" s="57"/>
       <c r="E11" s="17" t="s">
@@ -2285,29 +2273,27 @@
       </c>
       <c r="K11" s="81"/>
       <c r="L11" s="44" t="s">
-        <v>121</v>
+        <v>158</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A12" s="100"/>
       <c r="B12" s="103"/>
       <c r="C12" s="56">
-        <v>11</v>
-      </c>
-      <c r="D12" s="57">
-        <v>7</v>
-      </c>
+        <v>110</v>
+      </c>
+      <c r="D12" s="57"/>
       <c r="E12" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="F12" s="30" t="s">
+        <v>117</v>
+      </c>
+      <c r="G12" s="67" t="s">
+        <v>33</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>116</v>
-      </c>
-      <c r="F12" s="30" t="s">
-        <v>118</v>
-      </c>
-      <c r="G12" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>117</v>
       </c>
       <c r="I12" s="48" t="s">
         <v>69</v>
@@ -2322,11 +2308,9 @@
       <c r="A13" s="101"/>
       <c r="B13" s="104"/>
       <c r="C13" s="58">
-        <v>12</v>
-      </c>
-      <c r="D13" s="59">
-        <v>8</v>
-      </c>
+        <v>120</v>
+      </c>
+      <c r="D13" s="59"/>
       <c r="E13" s="20" t="s">
         <v>10</v>
       </c>
@@ -2337,7 +2321,7 @@
         <v>33</v>
       </c>
       <c r="H13" s="20" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="I13" s="51" t="s">
         <v>71</v>
@@ -2356,7 +2340,7 @@
         <v>12</v>
       </c>
       <c r="C14" s="54">
-        <v>13</v>
+        <v>130</v>
       </c>
       <c r="D14" s="55"/>
       <c r="E14" s="18" t="s">
@@ -2369,7 +2353,7 @@
         <v>34</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="I14" s="26" t="s">
         <v>74</v>
@@ -2379,14 +2363,14 @@
       </c>
       <c r="K14" s="83"/>
       <c r="L14" s="43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="100"/>
       <c r="B15" s="103"/>
       <c r="C15" s="56">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="D15" s="57"/>
       <c r="E15" s="17" t="s">
@@ -2409,7 +2393,7 @@
       </c>
       <c r="K15" s="81"/>
       <c r="L15" s="44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.25">
@@ -2418,16 +2402,14 @@
         <v>13</v>
       </c>
       <c r="C16" s="56">
-        <v>15</v>
-      </c>
-      <c r="D16" s="57">
-        <v>9</v>
-      </c>
+        <v>150</v>
+      </c>
+      <c r="D16" s="57"/>
       <c r="E16" s="19" t="s">
         <v>15</v>
       </c>
       <c r="F16" s="32" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="G16" s="69" t="s">
         <v>34</v>
@@ -2448,7 +2430,7 @@
       <c r="A17" s="100"/>
       <c r="B17" s="103"/>
       <c r="C17" s="56">
-        <v>16</v>
+        <v>160</v>
       </c>
       <c r="D17" s="57"/>
       <c r="E17" s="17" t="s">
@@ -2471,7 +2453,7 @@
       </c>
       <c r="K17" s="81"/>
       <c r="L17" s="44" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
@@ -2480,22 +2462,20 @@
         <v>14</v>
       </c>
       <c r="C18" s="56">
-        <v>17</v>
-      </c>
-      <c r="D18" s="57">
-        <v>10</v>
-      </c>
+        <v>170</v>
+      </c>
+      <c r="D18" s="57"/>
       <c r="E18" s="19" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="F18" s="32" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="G18" s="69" t="s">
         <v>34</v>
       </c>
       <c r="H18" s="19" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="I18" s="24" t="s">
         <v>83</v>
@@ -2505,14 +2485,14 @@
       </c>
       <c r="K18" s="81"/>
       <c r="L18" s="44" t="s">
-        <v>130</v>
+        <v>159</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A19" s="100"/>
       <c r="B19" s="103"/>
       <c r="C19" s="56">
-        <v>18</v>
+        <v>180</v>
       </c>
       <c r="D19" s="57"/>
       <c r="E19" s="87" t="s">
@@ -2535,29 +2515,27 @@
       </c>
       <c r="K19" s="81"/>
       <c r="L19" s="44" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="100"/>
       <c r="B20" s="103"/>
       <c r="C20" s="56">
-        <v>19</v>
-      </c>
-      <c r="D20" s="57">
-        <v>11</v>
-      </c>
+        <v>190</v>
+      </c>
+      <c r="D20" s="57"/>
       <c r="E20" s="19" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="F20" s="32" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="G20" s="69" t="s">
         <v>33</v>
       </c>
       <c r="H20" s="19" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="I20" s="24" t="s">
         <v>83</v>
@@ -2572,7 +2550,7 @@
       <c r="A21" s="100"/>
       <c r="B21" s="103"/>
       <c r="C21" s="56">
-        <v>20</v>
+        <v>200</v>
       </c>
       <c r="D21" s="57"/>
       <c r="E21" s="17" t="s">
@@ -2585,7 +2563,7 @@
         <v>33</v>
       </c>
       <c r="H21" s="17" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="I21" s="23" t="s">
         <v>83</v>
@@ -2595,14 +2573,14 @@
       </c>
       <c r="K21" s="81"/>
       <c r="L21" s="44" t="s">
-        <v>131</v>
+        <v>161</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="100"/>
       <c r="B22" s="103"/>
       <c r="C22" s="56">
-        <v>21</v>
+        <v>210</v>
       </c>
       <c r="D22" s="57"/>
       <c r="E22" s="17" t="s">
@@ -2625,23 +2603,21 @@
       </c>
       <c r="K22" s="81"/>
       <c r="L22" s="44" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A23" s="100"/>
       <c r="B23" s="103"/>
       <c r="C23" s="56">
-        <v>22</v>
-      </c>
-      <c r="D23" s="57">
-        <v>12</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="D23" s="57"/>
       <c r="E23" s="19" t="s">
         <v>22</v>
       </c>
       <c r="F23" s="32" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="G23" s="69" t="s">
         <v>33</v>
@@ -2650,7 +2626,7 @@
         <v>55</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="J23" s="76" t="s">
         <v>34</v>
@@ -2664,16 +2640,14 @@
         <v>27</v>
       </c>
       <c r="C24" s="56">
-        <v>23</v>
-      </c>
-      <c r="D24" s="57">
-        <v>13</v>
-      </c>
+        <v>230</v>
+      </c>
+      <c r="D24" s="57"/>
       <c r="E24" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="F24" s="30" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="G24" s="67" t="s">
         <v>34</v>
@@ -2694,7 +2668,7 @@
       <c r="A25" s="100"/>
       <c r="B25" s="103"/>
       <c r="C25" s="56">
-        <v>24</v>
+        <v>240</v>
       </c>
       <c r="D25" s="57"/>
       <c r="E25" s="17" t="s">
@@ -2717,29 +2691,27 @@
       </c>
       <c r="K25" s="81"/>
       <c r="L25" s="44" t="s">
-        <v>135</v>
+        <v>162</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="100"/>
       <c r="B26" s="103"/>
       <c r="C26" s="56">
-        <v>25</v>
-      </c>
-      <c r="D26" s="57">
-        <v>14</v>
-      </c>
+        <v>250</v>
+      </c>
+      <c r="D26" s="57"/>
       <c r="E26" s="10" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="F26" s="30" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="G26" s="67" t="s">
         <v>34</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="I26" s="22" t="s">
         <v>83</v>
@@ -2749,14 +2721,14 @@
       </c>
       <c r="K26" s="81"/>
       <c r="L26" s="44" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="101"/>
       <c r="B27" s="104"/>
       <c r="C27" s="58">
-        <v>26</v>
+        <v>260</v>
       </c>
       <c r="D27" s="59"/>
       <c r="E27" s="91" t="s">
@@ -2779,7 +2751,7 @@
       </c>
       <c r="K27" s="84"/>
       <c r="L27" s="45" t="s">
-        <v>138</v>
+        <v>163</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -2790,7 +2762,7 @@
         <v>35</v>
       </c>
       <c r="C28" s="60">
-        <v>27</v>
+        <v>270</v>
       </c>
       <c r="D28" s="61"/>
       <c r="E28" s="18" t="s">
@@ -2813,23 +2785,21 @@
       </c>
       <c r="K28" s="85"/>
       <c r="L28" s="43" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="100"/>
       <c r="B29" s="103"/>
       <c r="C29" s="56">
-        <v>28</v>
-      </c>
-      <c r="D29" s="57">
-        <v>15</v>
-      </c>
+        <v>280</v>
+      </c>
+      <c r="D29" s="57"/>
       <c r="E29" s="19" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="F29" s="32" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="G29" s="69" t="s">
         <v>33</v>
@@ -2838,7 +2808,7 @@
         <v>93</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="J29" s="76" t="s">
         <v>34</v>
@@ -2850,14 +2820,14 @@
       <c r="A30" s="100"/>
       <c r="B30" s="103"/>
       <c r="C30" s="56">
-        <v>29</v>
+        <v>290</v>
       </c>
       <c r="D30" s="57"/>
       <c r="E30" s="17" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="F30" s="31" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="G30" s="68" t="s">
         <v>33</v>
@@ -2873,7 +2843,7 @@
       </c>
       <c r="K30" s="81"/>
       <c r="L30" s="44" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
@@ -2882,16 +2852,14 @@
         <v>36</v>
       </c>
       <c r="C31" s="56">
-        <v>30</v>
-      </c>
-      <c r="D31" s="57">
-        <v>16</v>
-      </c>
+        <v>300</v>
+      </c>
+      <c r="D31" s="57"/>
       <c r="E31" s="10" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F31" s="30" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="G31" s="67" t="s">
         <v>33</v>
@@ -2900,7 +2868,7 @@
         <v>95</v>
       </c>
       <c r="I31" s="22" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="J31" s="76" t="s">
         <v>34</v>
@@ -2912,14 +2880,14 @@
       <c r="A32" s="100"/>
       <c r="B32" s="103"/>
       <c r="C32" s="56">
-        <v>31</v>
+        <v>310</v>
       </c>
       <c r="D32" s="57"/>
       <c r="E32" s="17" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="F32" s="31" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="G32" s="68" t="s">
         <v>34</v>
@@ -2928,21 +2896,21 @@
         <v>98</v>
       </c>
       <c r="I32" s="23" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="J32" s="76" t="s">
         <v>33</v>
       </c>
       <c r="K32" s="81"/>
       <c r="L32" s="44" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="100"/>
       <c r="B33" s="103"/>
       <c r="C33" s="56">
-        <v>32</v>
+        <v>320</v>
       </c>
       <c r="D33" s="57"/>
       <c r="E33" s="17" t="s">
@@ -2965,14 +2933,14 @@
       </c>
       <c r="K33" s="81"/>
       <c r="L33" s="44" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="100"/>
       <c r="B34" s="103"/>
       <c r="C34" s="56">
-        <v>33</v>
+        <v>330</v>
       </c>
       <c r="D34" s="57"/>
       <c r="E34" s="17" t="s">
@@ -2995,14 +2963,14 @@
       </c>
       <c r="K34" s="81"/>
       <c r="L34" s="44" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="100"/>
       <c r="B35" s="103"/>
       <c r="C35" s="56">
-        <v>34</v>
+        <v>340</v>
       </c>
       <c r="D35" s="57"/>
       <c r="E35" s="17" t="s">
@@ -3025,14 +2993,14 @@
       </c>
       <c r="K35" s="81"/>
       <c r="L35" s="44" t="s">
-        <v>133</v>
+        <v>165</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="106"/>
       <c r="B36" s="108"/>
       <c r="C36" s="62">
-        <v>35</v>
+        <v>350</v>
       </c>
       <c r="D36" s="63"/>
       <c r="E36" s="88" t="s">
@@ -3055,31 +3023,29 @@
       </c>
       <c r="K36" s="82"/>
       <c r="L36" s="45" t="s">
-        <v>134</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="99" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="B37" s="96"/>
       <c r="C37" s="54">
-        <v>36</v>
-      </c>
-      <c r="D37" s="55">
-        <v>18</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="D37" s="55"/>
       <c r="E37" s="9" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="F37" s="36" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="G37" s="71" t="s">
         <v>34</v>
       </c>
       <c r="H37" s="9" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="I37" s="27" t="s">
         <v>78</v>
@@ -3092,7 +3058,7 @@
       <c r="A38" s="100"/>
       <c r="B38" s="97"/>
       <c r="C38" s="56">
-        <v>37</v>
+        <v>370</v>
       </c>
       <c r="D38" s="57"/>
       <c r="E38" s="10"/>
@@ -3108,7 +3074,7 @@
       <c r="A39" s="100"/>
       <c r="B39" s="97"/>
       <c r="C39" s="56">
-        <v>38</v>
+        <v>380</v>
       </c>
       <c r="D39" s="57"/>
       <c r="E39" s="10"/>
@@ -3124,7 +3090,7 @@
       <c r="A40" s="100"/>
       <c r="B40" s="97"/>
       <c r="C40" s="56">
-        <v>39</v>
+        <v>390</v>
       </c>
       <c r="D40" s="57"/>
       <c r="E40" s="10"/>
@@ -3140,7 +3106,7 @@
       <c r="A41" s="101"/>
       <c r="B41" s="98"/>
       <c r="C41" s="58">
-        <v>40</v>
+        <v>400</v>
       </c>
       <c r="D41" s="59"/>
       <c r="E41" s="11"/>
@@ -3160,14 +3126,14 @@
         <v>43</v>
       </c>
       <c r="C42" s="64">
-        <v>41</v>
+        <v>410</v>
       </c>
       <c r="D42" s="65"/>
       <c r="E42" s="12" t="s">
         <v>44</v>
       </c>
       <c r="F42" s="37" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="G42" s="74" t="s">
         <v>34</v>
@@ -3185,6 +3151,13 @@
   </sheetData>
   <autoFilter ref="A1:L42" xr:uid="{370A0B0F-C0FD-4EC3-B4F7-C3AB5FE65C83}"/>
   <mergeCells count="16">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="A37:A41"/>
     <mergeCell ref="A14:A27"/>
     <mergeCell ref="B14:B15"/>
@@ -3194,13 +3167,6 @@
     <mergeCell ref="A28:A36"/>
     <mergeCell ref="B28:B30"/>
     <mergeCell ref="B31:B36"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:G1048576">
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Y">

</xml_diff>

<commit_message>
Added HB to init
</commit_message>
<xml_diff>
--- a/TESTCASES/TestCases.xlsx
+++ b/TESTCASES/TestCases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andra\OneDrive - University of Greenwich\PhD\Application\ObjectController\TESTCASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73790501-6224-4CB8-B91B-DD60E61D723D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35A1BD5-BAB1-432A-89F6-8EFFCDFA45E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
   </bookViews>
@@ -513,9 +513,6 @@
     <t>Object down stairs with people overtaking</t>
   </si>
   <si>
-    <t>Lots of doglegged stairs, people entering from side doors while its going down. People overtaking</t>
-  </si>
-  <si>
     <t>LongStairs.mta</t>
   </si>
   <si>
@@ -552,9 +549,6 @@
     <t>Covered in TC 310</t>
   </si>
   <si>
-    <t>Wheelchair user moves self to refuge area. Attentant comes with EC. Puts person in chair and proceeds to exit.</t>
-  </si>
-  <si>
     <t>2FloorSimple.exo</t>
   </si>
   <si>
@@ -564,10 +558,16 @@
     <t>Patient in HB 1) evacuated to safe compartment in HB, 2) moved to RS and evacuated, 3) moved to EC and evacuated</t>
   </si>
   <si>
-    <t>Evacuation of hospital patient with and without device</t>
-  </si>
-  <si>
     <t>Evacuation of wheelchair user at refuge area</t>
+  </si>
+  <si>
+    <t>Evacuation of hospital patient with device or bed</t>
+  </si>
+  <si>
+    <t>Wheelchair user moves self to refuge area. Attentant comes with EC, puts PRM in EC and proceeds to exit.</t>
+  </si>
+  <si>
+    <t>Lots of doglegged stairs, people entering from side doors while its going down. People overtaking. Use ST (2) to check no overtake and EC (3) to check there is overtake</t>
   </si>
 </sst>
 </file>
@@ -1428,6 +1428,69 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1440,71 +1503,8 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1884,8 +1884,8 @@
   <dimension ref="A1:L40"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E38" sqref="E38"/>
+      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1911,7 +1911,7 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>120</v>
@@ -1942,10 +1942,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="82" t="s">
+      <c r="A2" s="103" t="s">
         <v>39</v>
       </c>
-      <c r="B2" s="85" t="s">
+      <c r="B2" s="106" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="47">
@@ -1976,8 +1976,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="83"/>
-      <c r="B3" s="86"/>
+      <c r="A3" s="104"/>
+      <c r="B3" s="99"/>
       <c r="C3" s="49">
         <v>20</v>
       </c>
@@ -2006,8 +2006,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="83"/>
-      <c r="B4" s="86" t="s">
+      <c r="A4" s="104"/>
+      <c r="B4" s="99" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="49">
@@ -2038,8 +2038,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="83"/>
-      <c r="B5" s="86"/>
+      <c r="A5" s="104"/>
+      <c r="B5" s="99"/>
       <c r="C5" s="49">
         <v>40</v>
       </c>
@@ -2068,8 +2068,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="83"/>
-      <c r="B6" s="86" t="s">
+      <c r="A6" s="104"/>
+      <c r="B6" s="99" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="49">
@@ -2098,8 +2098,8 @@
       <c r="L6" s="37"/>
     </row>
     <row r="7" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="84"/>
-      <c r="B7" s="87"/>
+      <c r="A7" s="105"/>
+      <c r="B7" s="107"/>
       <c r="C7" s="51">
         <v>60</v>
       </c>
@@ -2126,10 +2126,10 @@
       <c r="L7" s="38"/>
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="103" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="106" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="47">
@@ -2158,8 +2158,8 @@
       <c r="L8" s="36"/>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="83"/>
-      <c r="B9" s="86"/>
+      <c r="A9" s="104"/>
+      <c r="B9" s="99"/>
       <c r="C9" s="49">
         <v>80</v>
       </c>
@@ -2184,12 +2184,12 @@
       </c>
       <c r="K9" s="71"/>
       <c r="L9" s="37" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="83"/>
-      <c r="B10" s="86"/>
+      <c r="A10" s="104"/>
+      <c r="B10" s="99"/>
       <c r="C10" s="49">
         <v>90</v>
       </c>
@@ -2218,8 +2218,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="83"/>
-      <c r="B11" s="86" t="s">
+      <c r="A11" s="104"/>
+      <c r="B11" s="99" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="49">
@@ -2246,12 +2246,12 @@
       </c>
       <c r="K11" s="71"/>
       <c r="L11" s="37" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="83"/>
-      <c r="B12" s="86"/>
+      <c r="A12" s="104"/>
+      <c r="B12" s="99"/>
       <c r="C12" s="49">
         <v>110</v>
       </c>
@@ -2278,8 +2278,8 @@
       <c r="L12" s="37"/>
     </row>
     <row r="13" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="84"/>
-      <c r="B13" s="87"/>
+      <c r="A13" s="105"/>
+      <c r="B13" s="107"/>
       <c r="C13" s="51">
         <v>120</v>
       </c>
@@ -2306,10 +2306,10 @@
       <c r="L13" s="38"/>
     </row>
     <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="82" t="s">
+      <c r="A14" s="103" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="106" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="47">
@@ -2340,8 +2340,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="83"/>
-      <c r="B15" s="86"/>
+      <c r="A15" s="104"/>
+      <c r="B15" s="99"/>
       <c r="C15" s="49">
         <v>140</v>
       </c>
@@ -2370,8 +2370,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="83"/>
-      <c r="B16" s="86" t="s">
+      <c r="A16" s="104"/>
+      <c r="B16" s="99" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="49">
@@ -2382,7 +2382,7 @@
         <v>15</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G16" s="62" t="s">
         <v>34</v>
@@ -2400,8 +2400,8 @@
       <c r="L16" s="37"/>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="83"/>
-      <c r="B17" s="86"/>
+      <c r="A17" s="104"/>
+      <c r="B17" s="99"/>
       <c r="C17" s="49">
         <v>160</v>
       </c>
@@ -2430,8 +2430,8 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="83"/>
-      <c r="B18" s="86" t="s">
+      <c r="A18" s="104"/>
+      <c r="B18" s="99" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="49">
@@ -2458,12 +2458,12 @@
       </c>
       <c r="K18" s="71"/>
       <c r="L18" s="37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="83"/>
-      <c r="B19" s="86"/>
+      <c r="A19" s="104"/>
+      <c r="B19" s="99"/>
       <c r="C19" s="49">
         <v>180</v>
       </c>
@@ -2488,12 +2488,12 @@
       </c>
       <c r="K19" s="71"/>
       <c r="L19" s="37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="83"/>
-      <c r="B20" s="86"/>
+      <c r="A20" s="104"/>
+      <c r="B20" s="99"/>
       <c r="C20" s="49">
         <v>190</v>
       </c>
@@ -2520,8 +2520,8 @@
       <c r="L20" s="37"/>
     </row>
     <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="83"/>
-      <c r="B21" s="86"/>
+      <c r="A21" s="104"/>
+      <c r="B21" s="99"/>
       <c r="C21" s="49">
         <v>200</v>
       </c>
@@ -2546,12 +2546,12 @@
       </c>
       <c r="K21" s="71"/>
       <c r="L21" s="37" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="83"/>
-      <c r="B22" s="86"/>
+      <c r="A22" s="104"/>
+      <c r="B22" s="99"/>
       <c r="C22" s="49">
         <v>210</v>
       </c>
@@ -2576,12 +2576,12 @@
       </c>
       <c r="K22" s="71"/>
       <c r="L22" s="37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
-      <c r="B23" s="86"/>
+      <c r="A23" s="104"/>
+      <c r="B23" s="99"/>
       <c r="C23" s="49">
         <v>220</v>
       </c>
@@ -2608,8 +2608,8 @@
       <c r="L23" s="37"/>
     </row>
     <row r="24" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="83"/>
-      <c r="B24" s="86" t="s">
+      <c r="A24" s="104"/>
+      <c r="B24" s="99" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="49">
@@ -2638,8 +2638,8 @@
       <c r="L24" s="37"/>
     </row>
     <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="83"/>
-      <c r="B25" s="86"/>
+      <c r="A25" s="104"/>
+      <c r="B25" s="99"/>
       <c r="C25" s="49">
         <v>240</v>
       </c>
@@ -2664,12 +2664,12 @@
       </c>
       <c r="K25" s="71"/>
       <c r="L25" s="37" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="83"/>
-      <c r="B26" s="86"/>
+      <c r="A26" s="104"/>
+      <c r="B26" s="99"/>
       <c r="C26" s="49">
         <v>250</v>
       </c>
@@ -2698,8 +2698,8 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="84"/>
-      <c r="B27" s="87"/>
+      <c r="A27" s="105"/>
+      <c r="B27" s="107"/>
       <c r="C27" s="51">
         <v>260</v>
       </c>
@@ -2724,14 +2724,14 @@
       </c>
       <c r="K27" s="74"/>
       <c r="L27" s="38" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="90" t="s">
+      <c r="A28" s="101" t="s">
         <v>25</v>
       </c>
-      <c r="B28" s="88" t="s">
+      <c r="B28" s="98" t="s">
         <v>35</v>
       </c>
       <c r="C28" s="53">
@@ -2762,8 +2762,8 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="91"/>
-      <c r="B29" s="86"/>
+      <c r="A29" s="102"/>
+      <c r="B29" s="99"/>
       <c r="C29" s="49">
         <v>280</v>
       </c>
@@ -2790,8 +2790,8 @@
       <c r="L29" s="37"/>
     </row>
     <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="91"/>
-      <c r="B30" s="86"/>
+      <c r="A30" s="102"/>
+      <c r="B30" s="99"/>
       <c r="C30" s="49">
         <v>290</v>
       </c>
@@ -2820,8 +2820,8 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="91"/>
-      <c r="B31" s="86" t="s">
+      <c r="A31" s="102"/>
+      <c r="B31" s="99" t="s">
         <v>36</v>
       </c>
       <c r="C31" s="49">
@@ -2850,8 +2850,8 @@
       <c r="L31" s="37"/>
     </row>
     <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="91"/>
-      <c r="B32" s="86"/>
+      <c r="A32" s="102"/>
+      <c r="B32" s="99"/>
       <c r="C32" s="49">
         <v>310</v>
       </c>
@@ -2876,12 +2876,12 @@
       </c>
       <c r="K32" s="71"/>
       <c r="L32" s="37" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="91"/>
-      <c r="B33" s="86"/>
+      <c r="A33" s="102"/>
+      <c r="B33" s="99"/>
       <c r="C33" s="49">
         <v>320</v>
       </c>
@@ -2906,12 +2906,12 @@
       </c>
       <c r="K33" s="71"/>
       <c r="L33" s="37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="91"/>
-      <c r="B34" s="86"/>
+      <c r="A34" s="102"/>
+      <c r="B34" s="99"/>
       <c r="C34" s="49">
         <v>330</v>
       </c>
@@ -2936,12 +2936,12 @@
       </c>
       <c r="K34" s="71"/>
       <c r="L34" s="37" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="91"/>
-      <c r="B35" s="86"/>
+      <c r="A35" s="102"/>
+      <c r="B35" s="99"/>
       <c r="C35" s="49">
         <v>340</v>
       </c>
@@ -2966,12 +2966,12 @@
       </c>
       <c r="K35" s="71"/>
       <c r="L35" s="37" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="91"/>
-      <c r="B36" s="86"/>
+      <c r="A36" s="102"/>
+      <c r="B36" s="99"/>
       <c r="C36" s="49">
         <v>350</v>
       </c>
@@ -2996,55 +2996,55 @@
       </c>
       <c r="K36" s="71"/>
       <c r="L36" s="37" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="91"/>
-      <c r="B37" s="89" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A37" s="102"/>
+      <c r="B37" s="100" t="s">
         <v>151</v>
       </c>
       <c r="C37" s="53">
         <v>360</v>
       </c>
       <c r="D37" s="54"/>
-      <c r="E37" s="92" t="s">
+      <c r="E37" s="82" t="s">
         <v>152</v>
       </c>
-      <c r="F37" s="93" t="s">
+      <c r="F37" s="83" t="s">
+        <v>171</v>
+      </c>
+      <c r="G37" s="84" t="s">
+        <v>34</v>
+      </c>
+      <c r="H37" s="82" t="s">
         <v>153</v>
       </c>
-      <c r="G37" s="94" t="s">
-        <v>34</v>
-      </c>
-      <c r="H37" s="92" t="s">
-        <v>154</v>
-      </c>
-      <c r="I37" s="95" t="s">
+      <c r="I37" s="85" t="s">
         <v>78</v>
       </c>
       <c r="J37" s="69"/>
       <c r="K37" s="75"/>
-      <c r="L37" s="96"/>
+      <c r="L37" s="86"/>
     </row>
     <row r="38" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="91"/>
-      <c r="B38" s="89"/>
+      <c r="A38" s="102"/>
+      <c r="B38" s="100"/>
       <c r="C38" s="49">
         <v>370</v>
       </c>
       <c r="D38" s="50"/>
       <c r="E38" s="10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>166</v>
+        <v>170</v>
       </c>
       <c r="G38" s="60" t="s">
         <v>34</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I38" s="20" t="s">
         <v>78</v>
@@ -3054,28 +3054,28 @@
       <c r="L38" s="37"/>
     </row>
     <row r="39" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="91"/>
-      <c r="B39" s="89"/>
+      <c r="A39" s="102"/>
+      <c r="B39" s="100"/>
       <c r="C39" s="55">
         <v>380</v>
       </c>
       <c r="D39" s="56"/>
-      <c r="E39" s="97" t="s">
-        <v>170</v>
-      </c>
-      <c r="F39" s="98" t="s">
+      <c r="E39" s="87" t="s">
         <v>169</v>
       </c>
-      <c r="G39" s="99" t="s">
-        <v>34</v>
-      </c>
-      <c r="H39" s="97"/>
-      <c r="I39" s="100" t="s">
+      <c r="F39" s="88" t="s">
+        <v>167</v>
+      </c>
+      <c r="G39" s="89" t="s">
+        <v>34</v>
+      </c>
+      <c r="H39" s="87"/>
+      <c r="I39" s="90" t="s">
         <v>78</v>
       </c>
       <c r="J39" s="70"/>
       <c r="K39" s="72"/>
-      <c r="L39" s="101"/>
+      <c r="L39" s="91"/>
     </row>
     <row r="40" spans="1:12" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="46" t="s">
@@ -3086,23 +3086,23 @@
       </c>
       <c r="C40" s="57"/>
       <c r="D40" s="58"/>
-      <c r="E40" s="102" t="s">
+      <c r="E40" s="92" t="s">
         <v>44</v>
       </c>
-      <c r="F40" s="103" t="s">
+      <c r="F40" s="93" t="s">
         <v>136</v>
       </c>
-      <c r="G40" s="104" t="s">
-        <v>34</v>
-      </c>
-      <c r="H40" s="102" t="s">
+      <c r="G40" s="94" t="s">
+        <v>34</v>
+      </c>
+      <c r="H40" s="92" t="s">
         <v>75</v>
       </c>
-      <c r="I40" s="105" t="s">
+      <c r="I40" s="95" t="s">
         <v>102</v>
       </c>
-      <c r="J40" s="106"/>
-      <c r="K40" s="107"/>
+      <c r="J40" s="96"/>
+      <c r="K40" s="97"/>
       <c r="L40" s="35"/>
     </row>
   </sheetData>
@@ -3115,15 +3115,15 @@
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B8:B10"/>
+    <mergeCell ref="B28:B30"/>
+    <mergeCell ref="B31:B36"/>
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="A28:A39"/>
     <mergeCell ref="A14:A27"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="A28:A39"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:G1048576">
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Y">

</xml_diff>

<commit_message>
Started TC360 and making Ghent.exo
</commit_message>
<xml_diff>
--- a/TESTCASES/TestCases.xlsx
+++ b/TESTCASES/TestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andra\OneDrive - University of Greenwich\PhD\Application\ObjectController\TESTCASES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uogcloud-my.sharepoint.com/personal/mj4126n_gre_ac_uk/Documents/PhD/Application/ObjectController/TESTCASES/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C35A1BD5-BAB1-432A-89F6-8EFFCDFA45E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{C35A1BD5-BAB1-432A-89F6-8EFFCDFA45E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D2D1247-F3C9-4D81-9C7D-2BF9BAA4EFB7}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="169">
   <si>
     <t>Vertices and attachment points are correct relative to CoR</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Relative Movement</t>
   </si>
   <si>
-    <t>Large  Cases</t>
-  </si>
-  <si>
     <t>Person going up stairs moves out of the way of a passing object (with high drive) going down</t>
   </si>
   <si>
@@ -141,12 +138,6 @@
   </si>
   <si>
     <t>Y</t>
-  </si>
-  <si>
-    <t>Large Geometries</t>
-  </si>
-  <si>
-    <t>Many Entities</t>
   </si>
   <si>
     <t>One object can navigate around many people in an open space (cross-flow)</t>
@@ -262,9 +253,6 @@
   </si>
   <si>
     <t>Screenshots</t>
-  </si>
-  <si>
-    <t>Ghent.mta</t>
   </si>
   <si>
     <t>2FloorSimple_W3L10x2.mta</t>
@@ -513,9 +501,6 @@
     <t>Object down stairs with people overtaking</t>
   </si>
   <si>
-    <t>LongStairs.mta</t>
-  </si>
-  <si>
     <t>Set tasks for people to pick up and drop off object. Check they can do this and the appropriate prep time is achieved. Check multiple pickups work for same attendants</t>
   </si>
   <si>
@@ -549,9 +534,6 @@
     <t>Covered in TC 310</t>
   </si>
   <si>
-    <t>2FloorSimple.exo</t>
-  </si>
-  <si>
     <t>Folder ID</t>
   </si>
   <si>
@@ -568,6 +550,15 @@
   </si>
   <si>
     <t>Lots of doglegged stairs, people entering from side doors while its going down. People overtaking. Use ST (2) to check no overtake and EC (3) to check there is overtake</t>
+  </si>
+  <si>
+    <t>Ghent.exo</t>
+  </si>
+  <si>
+    <t>Extreme Scenarios</t>
+  </si>
+  <si>
+    <t>Scenarios</t>
   </si>
 </sst>
 </file>
@@ -646,7 +637,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="40">
+  <borders count="41">
     <border>
       <left/>
       <right/>
@@ -1179,11 +1170,24 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="108">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1476,12 +1480,27 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1491,19 +1510,7 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1885,7 +1892,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1911,41 +1918,41 @@
         <v>2</v>
       </c>
       <c r="C1" s="39" t="s">
-        <v>166</v>
+        <v>160</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="31" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="H1" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="8" t="s">
-        <v>65</v>
-      </c>
-      <c r="I1" s="19" t="s">
-        <v>32</v>
-      </c>
       <c r="J1" s="32" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="K1" s="34" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="L1" s="33" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="103" t="s">
-        <v>39</v>
-      </c>
-      <c r="B2" s="106" t="s">
+      <c r="A2" s="98" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="101" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="47">
@@ -1956,28 +1963,28 @@
         <v>0</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="G2" s="59" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="I2" s="40" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="J2" s="66" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K2" s="73"/>
       <c r="L2" s="36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="104"/>
-      <c r="B3" s="99"/>
+      <c r="A3" s="99"/>
+      <c r="B3" s="102"/>
       <c r="C3" s="49">
         <v>20</v>
       </c>
@@ -1986,28 +1993,28 @@
         <v>4</v>
       </c>
       <c r="F3" s="25" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="G3" s="60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" s="10" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I3" s="41" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J3" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K3" s="71"/>
       <c r="L3" s="37" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="104"/>
-      <c r="B4" s="99" t="s">
+      <c r="A4" s="99"/>
+      <c r="B4" s="102" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="49">
@@ -2015,31 +2022,31 @@
       </c>
       <c r="D4" s="50"/>
       <c r="E4" s="15" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F4" s="26" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="G4" s="61" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="I4" s="42" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="J4" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K4" s="71"/>
       <c r="L4" s="37" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="104"/>
-      <c r="B5" s="99"/>
+      <c r="A5" s="99"/>
+      <c r="B5" s="102"/>
       <c r="C5" s="49">
         <v>40</v>
       </c>
@@ -2048,28 +2055,28 @@
         <v>5</v>
       </c>
       <c r="F5" s="26" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G5" s="61" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="I5" s="42" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="J5" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K5" s="71"/>
       <c r="L5" s="37" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="104"/>
-      <c r="B6" s="99" t="s">
+      <c r="A6" s="99"/>
+      <c r="B6" s="102" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="49">
@@ -2080,26 +2087,26 @@
         <v>17</v>
       </c>
       <c r="F6" s="27" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="G6" s="62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H6" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I6" s="43" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="J6" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K6" s="71"/>
       <c r="L6" s="37"/>
     </row>
     <row r="7" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="105"/>
-      <c r="B7" s="107"/>
+      <c r="A7" s="100"/>
+      <c r="B7" s="103"/>
       <c r="C7" s="51">
         <v>60</v>
       </c>
@@ -2108,28 +2115,28 @@
         <v>18</v>
       </c>
       <c r="F7" s="28" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="G7" s="63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="I7" s="44" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="J7" s="68" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K7" s="74"/>
       <c r="L7" s="38"/>
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="103" t="s">
+      <c r="A8" s="98" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="106" t="s">
+      <c r="B8" s="101" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="47">
@@ -2137,59 +2144,59 @@
       </c>
       <c r="D8" s="48"/>
       <c r="E8" s="9" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="G8" s="64" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I8" s="45" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J8" s="69" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K8" s="75"/>
       <c r="L8" s="36"/>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="104"/>
-      <c r="B9" s="99"/>
+      <c r="A9" s="99"/>
+      <c r="B9" s="102"/>
       <c r="C9" s="49">
         <v>80</v>
       </c>
       <c r="D9" s="50"/>
       <c r="E9" s="10" t="s">
-        <v>60</v>
+        <v>57</v>
       </c>
       <c r="F9" s="25" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="G9" s="60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="I9" s="41" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="J9" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K9" s="71"/>
       <c r="L9" s="37" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="104"/>
-      <c r="B10" s="99"/>
+      <c r="A10" s="99"/>
+      <c r="B10" s="102"/>
       <c r="C10" s="49">
         <v>90</v>
       </c>
@@ -2198,28 +2205,28 @@
         <v>9</v>
       </c>
       <c r="F10" s="25" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="G10" s="60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="I10" s="41" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="J10" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K10" s="71"/>
       <c r="L10" s="37" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="104"/>
-      <c r="B11" s="99" t="s">
+      <c r="A11" s="99"/>
+      <c r="B11" s="102" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="49">
@@ -2227,59 +2234,59 @@
       </c>
       <c r="D11" s="50"/>
       <c r="E11" s="15" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="F11" s="26" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="G11" s="61" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I11" s="42" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="J11" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K11" s="71"/>
       <c r="L11" s="37" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
     </row>
     <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="104"/>
-      <c r="B12" s="99"/>
+      <c r="A12" s="99"/>
+      <c r="B12" s="102"/>
       <c r="C12" s="49">
         <v>110</v>
       </c>
       <c r="D12" s="50"/>
       <c r="E12" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="F12" s="25" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="G12" s="60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="I12" s="41" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="J12" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K12" s="71"/>
       <c r="L12" s="37"/>
     </row>
     <row r="13" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="105"/>
-      <c r="B13" s="107"/>
+      <c r="A13" s="100"/>
+      <c r="B13" s="103"/>
       <c r="C13" s="51">
         <v>120</v>
       </c>
@@ -2288,28 +2295,28 @@
         <v>10</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="G13" s="63" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="I13" s="44" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="J13" s="70" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K13" s="72"/>
       <c r="L13" s="38"/>
     </row>
     <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="103" t="s">
+      <c r="A14" s="98" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="106" t="s">
+      <c r="B14" s="101" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="47">
@@ -2317,61 +2324,61 @@
       </c>
       <c r="D14" s="48"/>
       <c r="E14" s="16" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="F14" s="29" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="G14" s="65" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H14" s="16" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="I14" s="23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J14" s="66" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K14" s="73"/>
       <c r="L14" s="36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="104"/>
-      <c r="B15" s="99"/>
+      <c r="A15" s="99"/>
+      <c r="B15" s="102"/>
       <c r="C15" s="49">
         <v>140</v>
       </c>
       <c r="D15" s="50"/>
       <c r="E15" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F15" s="26" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="F15" s="26" t="s">
-        <v>81</v>
-      </c>
-      <c r="G15" s="61" t="s">
-        <v>34</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>76</v>
-      </c>
       <c r="I15" s="21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J15" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K15" s="71"/>
       <c r="L15" s="37" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="104"/>
-      <c r="B16" s="99" t="s">
+      <c r="A16" s="99"/>
+      <c r="B16" s="102" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="49">
@@ -2382,26 +2389,26 @@
         <v>15</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="G16" s="62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I16" s="22" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J16" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K16" s="71"/>
       <c r="L16" s="37"/>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="104"/>
-      <c r="B17" s="99"/>
+      <c r="A17" s="99"/>
+      <c r="B17" s="102"/>
       <c r="C17" s="49">
         <v>160</v>
       </c>
@@ -2410,28 +2417,28 @@
         <v>16</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="G17" s="61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H17" s="15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="I17" s="21" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J17" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K17" s="71"/>
       <c r="L17" s="37" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="104"/>
-      <c r="B18" s="99" t="s">
+      <c r="A18" s="99"/>
+      <c r="B18" s="102" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="49">
@@ -2439,31 +2446,31 @@
       </c>
       <c r="D18" s="50"/>
       <c r="E18" s="17" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="F18" s="27" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="G18" s="62" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H18" s="17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="I18" s="22" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J18" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K18" s="71"/>
       <c r="L18" s="37" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="104"/>
-      <c r="B19" s="99"/>
+      <c r="A19" s="99"/>
+      <c r="B19" s="102"/>
       <c r="C19" s="49">
         <v>180</v>
       </c>
@@ -2472,56 +2479,56 @@
         <v>19</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="G19" s="61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H19" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I19" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J19" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K19" s="71"/>
       <c r="L19" s="37" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="104"/>
-      <c r="B20" s="99"/>
+      <c r="A20" s="99"/>
+      <c r="B20" s="102"/>
       <c r="C20" s="49">
         <v>190</v>
       </c>
       <c r="D20" s="50"/>
       <c r="E20" s="17" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F20" s="27" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="G20" s="62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J20" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K20" s="71"/>
       <c r="L20" s="37"/>
     </row>
     <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="104"/>
-      <c r="B21" s="99"/>
+      <c r="A21" s="99"/>
+      <c r="B21" s="102"/>
       <c r="C21" s="49">
         <v>200</v>
       </c>
@@ -2530,28 +2537,28 @@
         <v>20</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="G21" s="61" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H21" s="15" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="I21" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J21" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K21" s="71"/>
       <c r="L21" s="37" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="104"/>
-      <c r="B22" s="99"/>
+      <c r="A22" s="99"/>
+      <c r="B22" s="102"/>
       <c r="C22" s="49">
         <v>210</v>
       </c>
@@ -2560,28 +2567,28 @@
         <v>21</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="G22" s="61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H22" s="15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I22" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J22" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K22" s="71"/>
       <c r="L22" s="37" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="104"/>
-      <c r="B23" s="99"/>
+      <c r="A23" s="99"/>
+      <c r="B23" s="102"/>
       <c r="C23" s="49">
         <v>220</v>
       </c>
@@ -2590,488 +2597,488 @@
         <v>22</v>
       </c>
       <c r="F23" s="27" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G23" s="62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="J23" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K23" s="71"/>
       <c r="L23" s="37"/>
     </row>
     <row r="24" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="104"/>
-      <c r="B24" s="99" t="s">
-        <v>27</v>
+      <c r="A24" s="99"/>
+      <c r="B24" s="102" t="s">
+        <v>26</v>
       </c>
       <c r="C24" s="49">
         <v>230</v>
       </c>
       <c r="D24" s="50"/>
       <c r="E24" s="10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="F24" s="25" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="G24" s="60" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H24" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I24" s="20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J24" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K24" s="71"/>
       <c r="L24" s="37"/>
     </row>
     <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="104"/>
-      <c r="B25" s="99"/>
+      <c r="A25" s="99"/>
+      <c r="B25" s="102"/>
       <c r="C25" s="49">
         <v>240</v>
       </c>
       <c r="D25" s="50"/>
       <c r="E25" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F25" s="26" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="G25" s="61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H25" s="15" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="I25" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J25" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K25" s="71"/>
       <c r="L25" s="37" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="104"/>
-      <c r="B26" s="99"/>
+      <c r="A26" s="99"/>
+      <c r="B26" s="102"/>
       <c r="C26" s="49">
         <v>250</v>
       </c>
       <c r="D26" s="50"/>
       <c r="E26" s="10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="F26" s="25" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="G26" s="60" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H26" s="10" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="I26" s="20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J26" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K26" s="71"/>
       <c r="L26" s="37" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="105"/>
-      <c r="B27" s="107"/>
+      <c r="A27" s="100"/>
+      <c r="B27" s="103"/>
       <c r="C27" s="51">
         <v>260</v>
       </c>
       <c r="D27" s="52"/>
       <c r="E27" s="77" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F27" s="78" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="G27" s="79" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H27" s="77" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="I27" s="80" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J27" s="68" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K27" s="74"/>
       <c r="L27" s="38" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="101" t="s">
-        <v>25</v>
-      </c>
-      <c r="B28" s="98" t="s">
-        <v>35</v>
+      <c r="A28" s="106" t="s">
+        <v>168</v>
+      </c>
+      <c r="B28" s="108" t="s">
+        <v>167</v>
       </c>
       <c r="C28" s="53">
         <v>270</v>
       </c>
       <c r="D28" s="54"/>
       <c r="E28" s="16" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="F28" s="29" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="G28" s="65" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H28" s="16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I28" s="23" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="J28" s="69" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K28" s="75"/>
       <c r="L28" s="36" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="102"/>
-      <c r="B29" s="99"/>
+      <c r="A29" s="107"/>
+      <c r="B29" s="105"/>
       <c r="C29" s="49">
         <v>280</v>
       </c>
       <c r="D29" s="50"/>
       <c r="E29" s="17" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F29" s="27" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
       <c r="G29" s="62" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H29" s="17" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="I29" s="22" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="J29" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K29" s="71"/>
       <c r="L29" s="37"/>
     </row>
     <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="102"/>
-      <c r="B30" s="99"/>
+      <c r="A30" s="107"/>
+      <c r="B30" s="105"/>
       <c r="C30" s="49">
         <v>290</v>
       </c>
       <c r="D30" s="50"/>
       <c r="E30" s="15" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="F30" s="26" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="G30" s="61" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H30" s="15" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I30" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J30" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K30" s="71"/>
       <c r="L30" s="37" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="102"/>
-      <c r="B31" s="99" t="s">
-        <v>36</v>
-      </c>
+      <c r="A31" s="107"/>
+      <c r="B31" s="105"/>
       <c r="C31" s="49">
         <v>300</v>
       </c>
       <c r="D31" s="50"/>
       <c r="E31" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F31" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F31" s="25" t="s">
-        <v>149</v>
-      </c>
       <c r="G31" s="60" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="I31" s="20" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="J31" s="67" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="K31" s="71"/>
       <c r="L31" s="37"/>
     </row>
     <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="102"/>
-      <c r="B32" s="99"/>
+      <c r="A32" s="107"/>
+      <c r="B32" s="105"/>
       <c r="C32" s="49">
         <v>310</v>
       </c>
       <c r="D32" s="50"/>
       <c r="E32" s="15" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="F32" s="26" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="G32" s="61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H32" s="15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I32" s="21" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="J32" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K32" s="71"/>
       <c r="L32" s="37" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="102"/>
-      <c r="B33" s="99"/>
+      <c r="A33" s="107"/>
+      <c r="B33" s="105"/>
       <c r="C33" s="49">
         <v>320</v>
       </c>
       <c r="D33" s="50"/>
       <c r="E33" s="15" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="F33" s="26" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="G33" s="61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H33" s="15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J33" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K33" s="71"/>
       <c r="L33" s="37" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="102"/>
-      <c r="B34" s="99"/>
+      <c r="A34" s="107"/>
+      <c r="B34" s="105"/>
       <c r="C34" s="49">
         <v>330</v>
       </c>
       <c r="D34" s="50"/>
       <c r="E34" s="15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="G34" s="61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I34" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J34" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K34" s="71"/>
       <c r="L34" s="37" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="102"/>
-      <c r="B35" s="99"/>
+      <c r="A35" s="107"/>
+      <c r="B35" s="105"/>
       <c r="C35" s="49">
         <v>340</v>
       </c>
       <c r="D35" s="50"/>
       <c r="E35" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="F35" s="26" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="G35" s="61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="I35" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J35" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K35" s="71"/>
       <c r="L35" s="37" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="102"/>
-      <c r="B36" s="99"/>
+      <c r="A36" s="107"/>
+      <c r="B36" s="104"/>
       <c r="C36" s="49">
         <v>350</v>
       </c>
       <c r="D36" s="50"/>
       <c r="E36" s="15" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="F36" s="26" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="G36" s="61" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="I36" s="21" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="J36" s="67" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K36" s="71"/>
       <c r="L36" s="37" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="102"/>
-      <c r="B37" s="100" t="s">
-        <v>151</v>
+      <c r="A37" s="107"/>
+      <c r="B37" s="105" t="s">
+        <v>147</v>
       </c>
       <c r="C37" s="53">
         <v>360</v>
       </c>
       <c r="D37" s="54"/>
       <c r="E37" s="82" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="F37" s="83" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="G37" s="84" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H37" s="82" t="s">
-        <v>153</v>
+        <v>166</v>
       </c>
       <c r="I37" s="85" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J37" s="69"/>
       <c r="K37" s="75"/>
       <c r="L37" s="86"/>
     </row>
     <row r="38" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="102"/>
-      <c r="B38" s="100"/>
+      <c r="A38" s="107"/>
+      <c r="B38" s="105"/>
       <c r="C38" s="49">
         <v>370</v>
       </c>
       <c r="D38" s="50"/>
       <c r="E38" s="10" t="s">
-        <v>168</v>
+        <v>162</v>
       </c>
       <c r="F38" s="25" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="G38" s="60" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H38" s="10" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="I38" s="20" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J38" s="67"/>
       <c r="K38" s="71"/>
       <c r="L38" s="37"/>
     </row>
     <row r="39" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="102"/>
-      <c r="B39" s="100"/>
+      <c r="A39" s="107"/>
+      <c r="B39" s="105"/>
       <c r="C39" s="55">
         <v>380</v>
       </c>
       <c r="D39" s="56"/>
       <c r="E39" s="87" t="s">
-        <v>169</v>
+        <v>163</v>
       </c>
       <c r="F39" s="88" t="s">
-        <v>167</v>
+        <v>161</v>
       </c>
       <c r="G39" s="89" t="s">
-        <v>34</v>
-      </c>
-      <c r="H39" s="87"/>
+        <v>33</v>
+      </c>
+      <c r="H39" s="87" t="s">
+        <v>166</v>
+      </c>
       <c r="I39" s="90" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="J39" s="70"/>
       <c r="K39" s="72"/>
@@ -3079,27 +3086,29 @@
     </row>
     <row r="40" spans="1:12" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="46" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="B40" s="81" t="s">
-        <v>43</v>
-      </c>
-      <c r="C40" s="57"/>
+      <c r="C40" s="57">
+        <v>390</v>
+      </c>
       <c r="D40" s="58"/>
       <c r="E40" s="92" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F40" s="93" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="G40" s="94" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="H40" s="92" t="s">
-        <v>75</v>
+        <v>166</v>
       </c>
       <c r="I40" s="95" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="J40" s="96"/>
       <c r="K40" s="97"/>
@@ -3107,7 +3116,15 @@
     </row>
   </sheetData>
   <autoFilter ref="A1:L40" xr:uid="{370A0B0F-C0FD-4EC3-B4F7-C3AB5FE65C83}"/>
-  <mergeCells count="16">
+  <mergeCells count="15">
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="A28:A39"/>
+    <mergeCell ref="A14:A27"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B23"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="B28:B36"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B5"/>
@@ -3115,15 +3132,6 @@
     <mergeCell ref="A8:A13"/>
     <mergeCell ref="B11:B13"/>
     <mergeCell ref="B8:B10"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B31:B36"/>
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="A28:A39"/>
-    <mergeCell ref="A14:A27"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B18:B23"/>
-    <mergeCell ref="B24:B27"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:G1048576">
     <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Y">

</xml_diff>

<commit_message>
Bug fixes and test case 295
</commit_message>
<xml_diff>
--- a/TESTCASES/TestCases.xlsx
+++ b/TESTCASES/TestCases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uogcloud-my.sharepoint.com/personal/mj4126n_gre_ac_uk/Documents/PhD/Application/ObjectController/TESTCASES/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andra\OneDrive - University of Greenwich\PhD\Application\ObjectController\TESTCASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="10" documentId="13_ncr:1_{C35A1BD5-BAB1-432A-89F6-8EFFCDFA45E4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6D2D1247-F3C9-4D81-9C7D-2BF9BAA4EFB7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168F1A50-708F-4D3D-A850-76A2A9A1B824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$40</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="172">
   <si>
     <t>Vertices and attachment points are correct relative to CoR</t>
   </si>
@@ -559,6 +559,15 @@
   </si>
   <si>
     <t>Scenarios</t>
+  </si>
+  <si>
+    <t>Large group of people with low drive will move out of the way of object with high drive</t>
+  </si>
+  <si>
+    <t>Large room, object on left heading right, largew group of people on right heading left. Test with different densities of people</t>
+  </si>
+  <si>
+    <t>LargeGroup</t>
   </si>
 </sst>
 </file>
@@ -1187,7 +1196,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="109">
+  <cellXfs count="110">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1480,6 +1489,9 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1498,9 +1510,6 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1511,6 +1520,9 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1888,11 +1900,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD7B405C-B925-43EB-A348-6C5A23DE5406}">
-  <dimension ref="A1:L40"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F37" sqref="F37"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L33" sqref="L33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1949,10 +1961,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="98" t="s">
+      <c r="A2" s="99" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="102" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="47">
@@ -1983,8 +1995,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="99"/>
-      <c r="B3" s="102"/>
+      <c r="A3" s="100"/>
+      <c r="B3" s="103"/>
       <c r="C3" s="49">
         <v>20</v>
       </c>
@@ -2013,8 +2025,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="99"/>
-      <c r="B4" s="102" t="s">
+      <c r="A4" s="100"/>
+      <c r="B4" s="103" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="49">
@@ -2045,8 +2057,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="99"/>
-      <c r="B5" s="102"/>
+      <c r="A5" s="100"/>
+      <c r="B5" s="103"/>
       <c r="C5" s="49">
         <v>40</v>
       </c>
@@ -2075,8 +2087,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="99"/>
-      <c r="B6" s="102" t="s">
+      <c r="A6" s="100"/>
+      <c r="B6" s="103" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="49">
@@ -2105,8 +2117,8 @@
       <c r="L6" s="37"/>
     </row>
     <row r="7" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="100"/>
-      <c r="B7" s="103"/>
+      <c r="A7" s="101"/>
+      <c r="B7" s="104"/>
       <c r="C7" s="51">
         <v>60</v>
       </c>
@@ -2133,10 +2145,10 @@
       <c r="L7" s="38"/>
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="98" t="s">
+      <c r="A8" s="99" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="101" t="s">
+      <c r="B8" s="102" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="47">
@@ -2165,8 +2177,8 @@
       <c r="L8" s="36"/>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="99"/>
-      <c r="B9" s="102"/>
+      <c r="A9" s="100"/>
+      <c r="B9" s="103"/>
       <c r="C9" s="49">
         <v>80</v>
       </c>
@@ -2195,8 +2207,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="99"/>
-      <c r="B10" s="102"/>
+      <c r="A10" s="100"/>
+      <c r="B10" s="103"/>
       <c r="C10" s="49">
         <v>90</v>
       </c>
@@ -2225,8 +2237,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="99"/>
-      <c r="B11" s="102" t="s">
+      <c r="A11" s="100"/>
+      <c r="B11" s="103" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="49">
@@ -2257,8 +2269,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="99"/>
-      <c r="B12" s="102"/>
+      <c r="A12" s="100"/>
+      <c r="B12" s="103"/>
       <c r="C12" s="49">
         <v>110</v>
       </c>
@@ -2285,8 +2297,8 @@
       <c r="L12" s="37"/>
     </row>
     <row r="13" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="100"/>
-      <c r="B13" s="103"/>
+      <c r="A13" s="101"/>
+      <c r="B13" s="104"/>
       <c r="C13" s="51">
         <v>120</v>
       </c>
@@ -2313,10 +2325,10 @@
       <c r="L13" s="38"/>
     </row>
     <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="98" t="s">
+      <c r="A14" s="99" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="101" t="s">
+      <c r="B14" s="102" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="47">
@@ -2347,8 +2359,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="99"/>
-      <c r="B15" s="102"/>
+      <c r="A15" s="100"/>
+      <c r="B15" s="103"/>
       <c r="C15" s="49">
         <v>140</v>
       </c>
@@ -2377,8 +2389,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="99"/>
-      <c r="B16" s="102" t="s">
+      <c r="A16" s="100"/>
+      <c r="B16" s="103" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="49">
@@ -2407,8 +2419,8 @@
       <c r="L16" s="37"/>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="99"/>
-      <c r="B17" s="102"/>
+      <c r="A17" s="100"/>
+      <c r="B17" s="103"/>
       <c r="C17" s="49">
         <v>160</v>
       </c>
@@ -2437,8 +2449,8 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="99"/>
-      <c r="B18" s="102" t="s">
+      <c r="A18" s="100"/>
+      <c r="B18" s="103" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="49">
@@ -2469,8 +2481,8 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="99"/>
-      <c r="B19" s="102"/>
+      <c r="A19" s="100"/>
+      <c r="B19" s="103"/>
       <c r="C19" s="49">
         <v>180</v>
       </c>
@@ -2499,8 +2511,8 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="99"/>
-      <c r="B20" s="102"/>
+      <c r="A20" s="100"/>
+      <c r="B20" s="103"/>
       <c r="C20" s="49">
         <v>190</v>
       </c>
@@ -2527,8 +2539,8 @@
       <c r="L20" s="37"/>
     </row>
     <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="99"/>
-      <c r="B21" s="102"/>
+      <c r="A21" s="100"/>
+      <c r="B21" s="103"/>
       <c r="C21" s="49">
         <v>200</v>
       </c>
@@ -2557,8 +2569,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="99"/>
-      <c r="B22" s="102"/>
+      <c r="A22" s="100"/>
+      <c r="B22" s="103"/>
       <c r="C22" s="49">
         <v>210</v>
       </c>
@@ -2587,8 +2599,8 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="99"/>
-      <c r="B23" s="102"/>
+      <c r="A23" s="100"/>
+      <c r="B23" s="103"/>
       <c r="C23" s="49">
         <v>220</v>
       </c>
@@ -2615,8 +2627,8 @@
       <c r="L23" s="37"/>
     </row>
     <row r="24" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="99"/>
-      <c r="B24" s="102" t="s">
+      <c r="A24" s="100"/>
+      <c r="B24" s="103" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="49">
@@ -2645,8 +2657,8 @@
       <c r="L24" s="37"/>
     </row>
     <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="99"/>
-      <c r="B25" s="102"/>
+      <c r="A25" s="100"/>
+      <c r="B25" s="103"/>
       <c r="C25" s="49">
         <v>240</v>
       </c>
@@ -2675,8 +2687,8 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="99"/>
-      <c r="B26" s="102"/>
+      <c r="A26" s="100"/>
+      <c r="B26" s="103"/>
       <c r="C26" s="49">
         <v>250</v>
       </c>
@@ -2705,8 +2717,8 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="100"/>
-      <c r="B27" s="103"/>
+      <c r="A27" s="101"/>
+      <c r="B27" s="104"/>
       <c r="C27" s="51">
         <v>260</v>
       </c>
@@ -2830,25 +2842,25 @@
       <c r="A31" s="107"/>
       <c r="B31" s="105"/>
       <c r="C31" s="49">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="D31" s="50"/>
-      <c r="E31" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F31" s="25" t="s">
-        <v>145</v>
-      </c>
-      <c r="G31" s="60" t="s">
-        <v>32</v>
-      </c>
-      <c r="H31" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I31" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="J31" s="67" t="s">
+      <c r="E31" s="17" t="s">
+        <v>169</v>
+      </c>
+      <c r="F31" s="27" t="s">
+        <v>170</v>
+      </c>
+      <c r="G31" s="62" t="s">
+        <v>33</v>
+      </c>
+      <c r="H31" s="17" t="s">
+        <v>171</v>
+      </c>
+      <c r="I31" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="J31" s="98" t="s">
         <v>33</v>
       </c>
       <c r="K31" s="71"/>
@@ -2858,44 +2870,42 @@
       <c r="A32" s="107"/>
       <c r="B32" s="105"/>
       <c r="C32" s="49">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="D32" s="50"/>
-      <c r="E32" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="F32" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="G32" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="H32" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I32" s="21" t="s">
-        <v>138</v>
+      <c r="E32" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="F32" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="G32" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>139</v>
       </c>
       <c r="J32" s="67" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K32" s="71"/>
-      <c r="L32" s="37" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="L32" s="37"/>
+    </row>
+    <row r="33" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="107"/>
       <c r="B33" s="105"/>
       <c r="C33" s="49">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="D33" s="50"/>
       <c r="E33" s="15" t="s">
-        <v>34</v>
+        <v>140</v>
       </c>
       <c r="F33" s="26" t="s">
-        <v>96</v>
+        <v>146</v>
       </c>
       <c r="G33" s="61" t="s">
         <v>33</v>
@@ -2904,34 +2914,34 @@
         <v>94</v>
       </c>
       <c r="I33" s="21" t="s">
-        <v>79</v>
+        <v>138</v>
       </c>
       <c r="J33" s="67" t="s">
         <v>32</v>
       </c>
       <c r="K33" s="71"/>
       <c r="L33" s="37" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="107"/>
       <c r="B34" s="105"/>
       <c r="C34" s="49">
-        <v>330</v>
+        <v>320</v>
       </c>
       <c r="D34" s="50"/>
       <c r="E34" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F34" s="26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="G34" s="61" t="s">
         <v>33</v>
       </c>
       <c r="H34" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I34" s="21" t="s">
         <v>79</v>
@@ -2941,27 +2951,27 @@
       </c>
       <c r="K34" s="71"/>
       <c r="L34" s="37" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="107"/>
       <c r="B35" s="105"/>
       <c r="C35" s="49">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="D35" s="50"/>
       <c r="E35" s="15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F35" s="26" t="s">
-        <v>92</v>
+        <v>97</v>
       </c>
       <c r="G35" s="61" t="s">
         <v>33</v>
       </c>
       <c r="H35" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="I35" s="21" t="s">
         <v>79</v>
@@ -2971,27 +2981,27 @@
       </c>
       <c r="K35" s="71"/>
       <c r="L35" s="37" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="107"/>
-      <c r="B36" s="104"/>
+      <c r="B36" s="105"/>
       <c r="C36" s="49">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="D36" s="50"/>
       <c r="E36" s="15" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F36" s="26" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G36" s="61" t="s">
         <v>33</v>
       </c>
       <c r="H36" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="I36" s="21" t="s">
         <v>79</v>
@@ -3001,130 +3011,160 @@
       </c>
       <c r="K36" s="71"/>
       <c r="L36" s="37" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="107"/>
+      <c r="B37" s="109"/>
+      <c r="C37" s="49">
+        <v>350</v>
+      </c>
+      <c r="D37" s="50"/>
+      <c r="E37" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F37" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="G37" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I37" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="J37" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="K37" s="71"/>
+      <c r="L37" s="37" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A37" s="107"/>
-      <c r="B37" s="105" t="s">
+    <row r="38" spans="1:12" ht="60" x14ac:dyDescent="0.25">
+      <c r="A38" s="107"/>
+      <c r="B38" s="105" t="s">
         <v>147</v>
       </c>
-      <c r="C37" s="53">
+      <c r="C38" s="53">
         <v>360</v>
       </c>
-      <c r="D37" s="54"/>
-      <c r="E37" s="82" t="s">
+      <c r="D38" s="54"/>
+      <c r="E38" s="82" t="s">
         <v>148</v>
       </c>
-      <c r="F37" s="83" t="s">
+      <c r="F38" s="83" t="s">
         <v>165</v>
       </c>
-      <c r="G37" s="84" t="s">
-        <v>33</v>
-      </c>
-      <c r="H37" s="82" t="s">
+      <c r="G38" s="84" t="s">
+        <v>33</v>
+      </c>
+      <c r="H38" s="82" t="s">
         <v>166</v>
       </c>
-      <c r="I37" s="85" t="s">
+      <c r="I38" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="J37" s="69"/>
-      <c r="K37" s="75"/>
-      <c r="L37" s="86"/>
-    </row>
-    <row r="38" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="107"/>
-      <c r="B38" s="105"/>
-      <c r="C38" s="49">
-        <v>370</v>
-      </c>
-      <c r="D38" s="50"/>
-      <c r="E38" s="10" t="s">
-        <v>162</v>
-      </c>
-      <c r="F38" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="G38" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="H38" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="I38" s="20" t="s">
-        <v>74</v>
-      </c>
-      <c r="J38" s="67"/>
-      <c r="K38" s="71"/>
-      <c r="L38" s="37"/>
-    </row>
-    <row r="39" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J38" s="69"/>
+      <c r="K38" s="75"/>
+      <c r="L38" s="86"/>
+    </row>
+    <row r="39" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="107"/>
       <c r="B39" s="105"/>
-      <c r="C39" s="55">
+      <c r="C39" s="49">
+        <v>370</v>
+      </c>
+      <c r="D39" s="50"/>
+      <c r="E39" s="10" t="s">
+        <v>162</v>
+      </c>
+      <c r="F39" s="25" t="s">
+        <v>164</v>
+      </c>
+      <c r="G39" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" s="10" t="s">
+        <v>166</v>
+      </c>
+      <c r="I39" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="J39" s="67"/>
+      <c r="K39" s="71"/>
+      <c r="L39" s="37"/>
+    </row>
+    <row r="40" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="107"/>
+      <c r="B40" s="105"/>
+      <c r="C40" s="55">
         <v>380</v>
       </c>
-      <c r="D39" s="56"/>
-      <c r="E39" s="87" t="s">
+      <c r="D40" s="56"/>
+      <c r="E40" s="87" t="s">
         <v>163</v>
       </c>
-      <c r="F39" s="88" t="s">
+      <c r="F40" s="88" t="s">
         <v>161</v>
       </c>
-      <c r="G39" s="89" t="s">
-        <v>33</v>
-      </c>
-      <c r="H39" s="87" t="s">
+      <c r="G40" s="89" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="87" t="s">
         <v>166</v>
       </c>
-      <c r="I39" s="90" t="s">
+      <c r="I40" s="90" t="s">
         <v>74</v>
       </c>
-      <c r="J39" s="70"/>
-      <c r="K39" s="72"/>
-      <c r="L39" s="91"/>
-    </row>
-    <row r="40" spans="1:12" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="46" t="s">
+      <c r="J40" s="70"/>
+      <c r="K40" s="72"/>
+      <c r="L40" s="91"/>
+    </row>
+    <row r="41" spans="1:12" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="B40" s="81" t="s">
+      <c r="B41" s="81" t="s">
         <v>40</v>
       </c>
-      <c r="C40" s="57">
+      <c r="C41" s="57">
         <v>390</v>
       </c>
-      <c r="D40" s="58"/>
-      <c r="E40" s="92" t="s">
+      <c r="D41" s="58"/>
+      <c r="E41" s="92" t="s">
         <v>41</v>
       </c>
-      <c r="F40" s="93" t="s">
+      <c r="F41" s="93" t="s">
         <v>132</v>
       </c>
-      <c r="G40" s="94" t="s">
-        <v>33</v>
-      </c>
-      <c r="H40" s="92" t="s">
+      <c r="G41" s="94" t="s">
+        <v>33</v>
+      </c>
+      <c r="H41" s="92" t="s">
         <v>166</v>
       </c>
-      <c r="I40" s="95" t="s">
+      <c r="I41" s="95" t="s">
         <v>98</v>
       </c>
-      <c r="J40" s="96"/>
-      <c r="K40" s="97"/>
-      <c r="L40" s="35"/>
+      <c r="J41" s="96"/>
+      <c r="K41" s="97"/>
+      <c r="L41" s="35"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L40" xr:uid="{370A0B0F-C0FD-4EC3-B4F7-C3AB5FE65C83}"/>
+  <autoFilter ref="A1:L41" xr:uid="{370A0B0F-C0FD-4EC3-B4F7-C3AB5FE65C83}"/>
   <mergeCells count="15">
-    <mergeCell ref="B37:B39"/>
-    <mergeCell ref="A28:A39"/>
+    <mergeCell ref="B38:B40"/>
+    <mergeCell ref="A28:A40"/>
     <mergeCell ref="A14:A27"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="B24:B27"/>
-    <mergeCell ref="B28:B36"/>
+    <mergeCell ref="B28:B37"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B5"/>
@@ -3141,7 +3181,7 @@
       <formula>NOT(ISERROR(SEARCH("N",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:K40">
+  <conditionalFormatting sqref="J2:K41">
     <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",J2)))</formula>
     </cfRule>
@@ -3154,7 +3194,7 @@
       <formula>NOT(ISERROR(SEARCH("N",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D40">
+  <conditionalFormatting sqref="D2:D41">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added Time to tcp log
</commit_message>
<xml_diff>
--- a/TESTCASES/TestCases.xlsx
+++ b/TESTCASES/TestCases.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andra\OneDrive - University of Greenwich\PhD\Application\ObjectController\TESTCASES\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{168F1A50-708F-4D3D-A850-76A2A9A1B824}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5ED2DCB6-A1EB-4027-B354-27BDF14EB99D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="173">
   <si>
     <t>Vertices and attachment points are correct relative to CoR</t>
   </si>
@@ -568,6 +568,9 @@
   </si>
   <si>
     <t>LargeGroup</t>
+  </si>
+  <si>
+    <t>R</t>
   </si>
 </sst>
 </file>
@@ -1492,6 +1495,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1508,15 +1520,6 @@
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1529,7 +1532,77 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C5700"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1903,8 +1976,8 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L33" sqref="L33"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1961,10 +2034,10 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="A2" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="105" t="s">
         <v>3</v>
       </c>
       <c r="C2" s="47">
@@ -1995,8 +2068,8 @@
       </c>
     </row>
     <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="100"/>
-      <c r="B3" s="103"/>
+      <c r="A3" s="103"/>
+      <c r="B3" s="106"/>
       <c r="C3" s="49">
         <v>20</v>
       </c>
@@ -2025,8 +2098,8 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="100"/>
-      <c r="B4" s="103" t="s">
+      <c r="A4" s="103"/>
+      <c r="B4" s="106" t="s">
         <v>23</v>
       </c>
       <c r="C4" s="49">
@@ -2057,8 +2130,8 @@
       </c>
     </row>
     <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="100"/>
-      <c r="B5" s="103"/>
+      <c r="A5" s="103"/>
+      <c r="B5" s="106"/>
       <c r="C5" s="49">
         <v>40</v>
       </c>
@@ -2087,8 +2160,8 @@
       </c>
     </row>
     <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="100"/>
-      <c r="B6" s="103" t="s">
+      <c r="A6" s="103"/>
+      <c r="B6" s="106" t="s">
         <v>24</v>
       </c>
       <c r="C6" s="49">
@@ -2117,8 +2190,8 @@
       <c r="L6" s="37"/>
     </row>
     <row r="7" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="101"/>
-      <c r="B7" s="104"/>
+      <c r="A7" s="104"/>
+      <c r="B7" s="107"/>
       <c r="C7" s="51">
         <v>60</v>
       </c>
@@ -2145,10 +2218,10 @@
       <c r="L7" s="38"/>
     </row>
     <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="99" t="s">
+      <c r="A8" s="102" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="105" t="s">
         <v>7</v>
       </c>
       <c r="C8" s="47">
@@ -2177,8 +2250,8 @@
       <c r="L8" s="36"/>
     </row>
     <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="100"/>
-      <c r="B9" s="103"/>
+      <c r="A9" s="103"/>
+      <c r="B9" s="106"/>
       <c r="C9" s="49">
         <v>80</v>
       </c>
@@ -2207,8 +2280,8 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="100"/>
-      <c r="B10" s="103"/>
+      <c r="A10" s="103"/>
+      <c r="B10" s="106"/>
       <c r="C10" s="49">
         <v>90</v>
       </c>
@@ -2237,8 +2310,8 @@
       </c>
     </row>
     <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="100"/>
-      <c r="B11" s="103" t="s">
+      <c r="A11" s="103"/>
+      <c r="B11" s="106" t="s">
         <v>8</v>
       </c>
       <c r="C11" s="49">
@@ -2269,8 +2342,8 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="100"/>
-      <c r="B12" s="103"/>
+      <c r="A12" s="103"/>
+      <c r="B12" s="106"/>
       <c r="C12" s="49">
         <v>110</v>
       </c>
@@ -2297,8 +2370,8 @@
       <c r="L12" s="37"/>
     </row>
     <row r="13" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="101"/>
-      <c r="B13" s="104"/>
+      <c r="A13" s="104"/>
+      <c r="B13" s="107"/>
       <c r="C13" s="51">
         <v>120</v>
       </c>
@@ -2325,10 +2398,10 @@
       <c r="L13" s="38"/>
     </row>
     <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="99" t="s">
+      <c r="A14" s="102" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="102" t="s">
+      <c r="B14" s="105" t="s">
         <v>12</v>
       </c>
       <c r="C14" s="47">
@@ -2359,8 +2432,8 @@
       </c>
     </row>
     <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="100"/>
-      <c r="B15" s="103"/>
+      <c r="A15" s="103"/>
+      <c r="B15" s="106"/>
       <c r="C15" s="49">
         <v>140</v>
       </c>
@@ -2389,8 +2462,8 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="100"/>
-      <c r="B16" s="103" t="s">
+      <c r="A16" s="103"/>
+      <c r="B16" s="106" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="49">
@@ -2419,8 +2492,8 @@
       <c r="L16" s="37"/>
     </row>
     <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="100"/>
-      <c r="B17" s="103"/>
+      <c r="A17" s="103"/>
+      <c r="B17" s="106"/>
       <c r="C17" s="49">
         <v>160</v>
       </c>
@@ -2449,8 +2522,8 @@
       </c>
     </row>
     <row r="18" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A18" s="100"/>
-      <c r="B18" s="103" t="s">
+      <c r="A18" s="103"/>
+      <c r="B18" s="106" t="s">
         <v>14</v>
       </c>
       <c r="C18" s="49">
@@ -2481,8 +2554,8 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A19" s="100"/>
-      <c r="B19" s="103"/>
+      <c r="A19" s="103"/>
+      <c r="B19" s="106"/>
       <c r="C19" s="49">
         <v>180</v>
       </c>
@@ -2511,8 +2584,8 @@
       </c>
     </row>
     <row r="20" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A20" s="100"/>
-      <c r="B20" s="103"/>
+      <c r="A20" s="103"/>
+      <c r="B20" s="106"/>
       <c r="C20" s="49">
         <v>190</v>
       </c>
@@ -2539,8 +2612,8 @@
       <c r="L20" s="37"/>
     </row>
     <row r="21" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="100"/>
-      <c r="B21" s="103"/>
+      <c r="A21" s="103"/>
+      <c r="B21" s="106"/>
       <c r="C21" s="49">
         <v>200</v>
       </c>
@@ -2569,8 +2642,8 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="100"/>
-      <c r="B22" s="103"/>
+      <c r="A22" s="103"/>
+      <c r="B22" s="106"/>
       <c r="C22" s="49">
         <v>210</v>
       </c>
@@ -2599,8 +2672,8 @@
       </c>
     </row>
     <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="100"/>
-      <c r="B23" s="103"/>
+      <c r="A23" s="103"/>
+      <c r="B23" s="106"/>
       <c r="C23" s="49">
         <v>220</v>
       </c>
@@ -2627,8 +2700,8 @@
       <c r="L23" s="37"/>
     </row>
     <row r="24" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A24" s="100"/>
-      <c r="B24" s="103" t="s">
+      <c r="A24" s="103"/>
+      <c r="B24" s="106" t="s">
         <v>26</v>
       </c>
       <c r="C24" s="49">
@@ -2657,8 +2730,8 @@
       <c r="L24" s="37"/>
     </row>
     <row r="25" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="100"/>
-      <c r="B25" s="103"/>
+      <c r="A25" s="103"/>
+      <c r="B25" s="106"/>
       <c r="C25" s="49">
         <v>240</v>
       </c>
@@ -2687,8 +2760,8 @@
       </c>
     </row>
     <row r="26" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A26" s="100"/>
-      <c r="B26" s="103"/>
+      <c r="A26" s="103"/>
+      <c r="B26" s="106"/>
       <c r="C26" s="49">
         <v>250</v>
       </c>
@@ -2709,7 +2782,7 @@
         <v>79</v>
       </c>
       <c r="J26" s="67" t="s">
-        <v>33</v>
+        <v>172</v>
       </c>
       <c r="K26" s="71"/>
       <c r="L26" s="37" t="s">
@@ -2717,8 +2790,8 @@
       </c>
     </row>
     <row r="27" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="101"/>
-      <c r="B27" s="104"/>
+      <c r="A27" s="104"/>
+      <c r="B27" s="107"/>
       <c r="C27" s="51">
         <v>260</v>
       </c>
@@ -2747,7 +2820,7 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="106" t="s">
+      <c r="A28" s="100" t="s">
         <v>168</v>
       </c>
       <c r="B28" s="108" t="s">
@@ -2781,8 +2854,8 @@
       </c>
     </row>
     <row r="29" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A29" s="107"/>
-      <c r="B29" s="105"/>
+      <c r="A29" s="101"/>
+      <c r="B29" s="99"/>
       <c r="C29" s="49">
         <v>280</v>
       </c>
@@ -2809,8 +2882,8 @@
       <c r="L29" s="37"/>
     </row>
     <row r="30" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="107"/>
-      <c r="B30" s="105"/>
+      <c r="A30" s="101"/>
+      <c r="B30" s="99"/>
       <c r="C30" s="49">
         <v>290</v>
       </c>
@@ -2839,8 +2912,8 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="107"/>
-      <c r="B31" s="105"/>
+      <c r="A31" s="101"/>
+      <c r="B31" s="99"/>
       <c r="C31" s="49">
         <v>295</v>
       </c>
@@ -2861,14 +2934,14 @@
         <v>74</v>
       </c>
       <c r="J31" s="98" t="s">
-        <v>33</v>
+        <v>172</v>
       </c>
       <c r="K31" s="71"/>
       <c r="L31" s="37"/>
     </row>
     <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="107"/>
-      <c r="B32" s="105"/>
+      <c r="A32" s="101"/>
+      <c r="B32" s="99"/>
       <c r="C32" s="49">
         <v>300</v>
       </c>
@@ -2895,8 +2968,8 @@
       <c r="L32" s="37"/>
     </row>
     <row r="33" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="107"/>
-      <c r="B33" s="105"/>
+      <c r="A33" s="101"/>
+      <c r="B33" s="99"/>
       <c r="C33" s="49">
         <v>310</v>
       </c>
@@ -2925,8 +2998,8 @@
       </c>
     </row>
     <row r="34" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="107"/>
-      <c r="B34" s="105"/>
+      <c r="A34" s="101"/>
+      <c r="B34" s="99"/>
       <c r="C34" s="49">
         <v>320</v>
       </c>
@@ -2955,8 +3028,8 @@
       </c>
     </row>
     <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="107"/>
-      <c r="B35" s="105"/>
+      <c r="A35" s="101"/>
+      <c r="B35" s="99"/>
       <c r="C35" s="49">
         <v>330</v>
       </c>
@@ -2985,8 +3058,8 @@
       </c>
     </row>
     <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="107"/>
-      <c r="B36" s="105"/>
+      <c r="A36" s="101"/>
+      <c r="B36" s="99"/>
       <c r="C36" s="49">
         <v>340</v>
       </c>
@@ -3015,7 +3088,7 @@
       </c>
     </row>
     <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="107"/>
+      <c r="A37" s="101"/>
       <c r="B37" s="109"/>
       <c r="C37" s="49">
         <v>350</v>
@@ -3045,8 +3118,8 @@
       </c>
     </row>
     <row r="38" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A38" s="107"/>
-      <c r="B38" s="105" t="s">
+      <c r="A38" s="101"/>
+      <c r="B38" s="99" t="s">
         <v>147</v>
       </c>
       <c r="C38" s="53">
@@ -3073,8 +3146,8 @@
       <c r="L38" s="86"/>
     </row>
     <row r="39" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A39" s="107"/>
-      <c r="B39" s="105"/>
+      <c r="A39" s="101"/>
+      <c r="B39" s="99"/>
       <c r="C39" s="49">
         <v>370</v>
       </c>
@@ -3099,8 +3172,8 @@
       <c r="L39" s="37"/>
     </row>
     <row r="40" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="107"/>
-      <c r="B40" s="105"/>
+      <c r="A40" s="101"/>
+      <c r="B40" s="99"/>
       <c r="C40" s="55">
         <v>380</v>
       </c>
@@ -3157,6 +3230,13 @@
   </sheetData>
   <autoFilter ref="A1:L41" xr:uid="{370A0B0F-C0FD-4EC3-B4F7-C3AB5FE65C83}"/>
   <mergeCells count="15">
+    <mergeCell ref="A2:A7"/>
+    <mergeCell ref="B2:B3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A8:A13"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="B38:B40"/>
     <mergeCell ref="A28:A40"/>
     <mergeCell ref="A14:A27"/>
@@ -3165,38 +3245,36 @@
     <mergeCell ref="B18:B23"/>
     <mergeCell ref="B24:B27"/>
     <mergeCell ref="B28:B37"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="B8:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:G1048576">
-    <cfRule type="containsText" dxfId="5" priority="6" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="12" priority="7" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",G2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="7" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="11" priority="8" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:K41">
-    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="P">
+    <cfRule type="containsText" dxfId="10" priority="4" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",J2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="Y">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Y">
       <formula>NOT(ISERROR(SEARCH("Y",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="containsText" dxfId="1" priority="2" operator="containsText" text="N">
+    <cfRule type="containsText" dxfId="8" priority="3" operator="containsText" text="N">
       <formula>NOT(ISERROR(SEARCH("N",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D2:D41">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="equal">
       <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J2:J41">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",J2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Marked cases as main text / appendix
</commit_message>
<xml_diff>
--- a/TESTCASES/TestCases.xlsx
+++ b/TESTCASES/TestCases.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andra\OneDrive - University of Greenwich\PhD\Application\ObjectController\TESTCASES\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike1\Documents\TestCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A5A9B10-A5EC-4ACA-A774-919E92A91F50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F742C8F-026B-47F1-B731-FD6769B663A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$L$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="181">
   <si>
     <t>Vertices and attachment points are correct relative to CoR</t>
   </si>
@@ -340,9 +340,6 @@
   </si>
   <si>
     <t>Results Collected</t>
-  </si>
-  <si>
-    <t>Results Written</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -580,6 +577,24 @@
   </si>
   <si>
     <t>Corridor20x10.exo</t>
+  </si>
+  <si>
+    <t>Appendix/Main Text/Not Include</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>M</t>
+  </si>
+  <si>
+    <t>Include 80 in results</t>
+  </si>
+  <si>
+    <t>Moveable attachment points change which corners are passable</t>
+  </si>
+  <si>
+    <t>Test different geo with unmoveable attachment point until it fails. Then test same one with moveable and see if it can now go around</t>
   </si>
 </sst>
 </file>
@@ -658,7 +673,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="42">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -1162,17 +1177,6 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right style="thin">
         <color indexed="64"/>
       </right>
@@ -1211,6 +1215,80 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -1221,15 +1299,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="111">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1247,70 +1325,61 @@
     <xf numFmtId="49" fontId="1" fillId="2" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="18" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="27" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1319,43 +1388,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="11" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1406,10 +1460,7 @@
     <xf numFmtId="49" fontId="4" fillId="5" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1433,90 +1484,63 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="5" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="28" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
@@ -1535,23 +1559,53 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="42" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="43" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="44" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="41" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1938,1303 +1992,1424 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD7B405C-B925-43EB-A348-6C5A23DE5406}">
-  <dimension ref="A1:L42"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L18" sqref="L18"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.140625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" style="3" customWidth="1"/>
-    <col min="3" max="4" width="11.28515625" style="2" customWidth="1"/>
-    <col min="5" max="6" width="44.85546875" style="11" customWidth="1"/>
-    <col min="7" max="7" width="12.7109375" style="12" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="28.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="28.28515625" style="13" customWidth="1"/>
-    <col min="10" max="10" width="13.85546875" style="2" customWidth="1"/>
-    <col min="11" max="11" width="12.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="35.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="10.109375" style="3" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="3" customWidth="1"/>
+    <col min="3" max="4" width="11.33203125" style="2" customWidth="1"/>
+    <col min="5" max="6" width="44.88671875" style="11" customWidth="1"/>
+    <col min="7" max="7" width="12" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="28.5546875" style="11" customWidth="1"/>
+    <col min="9" max="9" width="28.33203125" style="13" customWidth="1"/>
+    <col min="10" max="10" width="13.88671875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="20.88671875" style="1" customWidth="1"/>
+    <col min="12" max="12" width="12.5546875" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="4" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" s="4" customFormat="1" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="39" t="s">
-        <v>160</v>
+      <c r="C1" s="32" t="s">
+        <v>159</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E1" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="F1" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="28" t="s">
         <v>30</v>
       </c>
       <c r="H1" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="I1" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="J1" s="32" t="s">
+      <c r="J1" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="K1" s="34" t="s">
-        <v>100</v>
-      </c>
-      <c r="L1" s="33" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A2" s="99" t="s">
+      <c r="K1" s="93" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="100" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="81" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="102" t="s">
+      <c r="B2" s="84" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="39">
         <v>10</v>
       </c>
-      <c r="D2" s="48"/>
+      <c r="D2" s="40"/>
       <c r="E2" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="F2" s="24" t="s">
+      <c r="F2" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="G2" s="59" t="s">
+      <c r="G2" s="51" t="s">
         <v>32</v>
       </c>
       <c r="H2" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="I2" s="40" t="s">
+      <c r="I2" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="J2" s="66" t="s">
-        <v>33</v>
-      </c>
-      <c r="K2" s="73"/>
-      <c r="L2" s="36" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" ht="90" x14ac:dyDescent="0.25">
-      <c r="A3" s="100"/>
-      <c r="B3" s="103"/>
-      <c r="C3" s="49">
+      <c r="J2" s="57" t="s">
+        <v>33</v>
+      </c>
+      <c r="K2" s="94" t="s">
+        <v>117</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="82"/>
+      <c r="B3" s="85"/>
+      <c r="C3" s="41">
         <v>20</v>
       </c>
-      <c r="D3" s="50"/>
+      <c r="D3" s="42"/>
       <c r="E3" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="23" t="s">
         <v>43</v>
       </c>
-      <c r="G3" s="60" t="s">
+      <c r="G3" s="52" t="s">
         <v>32</v>
       </c>
       <c r="H3" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="I3" s="41" t="s">
+      <c r="I3" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K3" s="71"/>
-      <c r="L3" s="37" t="s">
+      <c r="J3" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K3" s="95" t="s">
+        <v>100</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="82"/>
+      <c r="B4" s="85" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" s="41">
+        <v>30</v>
+      </c>
+      <c r="D4" s="42"/>
+      <c r="E4" s="15" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A4" s="100"/>
-      <c r="B4" s="103" t="s">
-        <v>23</v>
-      </c>
-      <c r="C4" s="49">
-        <v>30</v>
-      </c>
-      <c r="D4" s="50"/>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="24" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="F4" s="26" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="H4" s="15" t="s">
+      <c r="I4" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="I4" s="42" t="s">
-        <v>104</v>
-      </c>
-      <c r="J4" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K4" s="71"/>
-      <c r="L4" s="37" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="100"/>
-      <c r="B5" s="103"/>
-      <c r="C5" s="49">
+      <c r="J4" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K4" s="95" t="s">
+        <v>117</v>
+      </c>
+      <c r="L4" s="30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="82"/>
+      <c r="B5" s="85"/>
+      <c r="C5" s="41">
         <v>40</v>
       </c>
-      <c r="D5" s="50"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="26" t="s">
+      <c r="F5" s="24" t="s">
         <v>45</v>
       </c>
-      <c r="G5" s="61" t="s">
+      <c r="G5" s="53" t="s">
         <v>32</v>
       </c>
       <c r="H5" s="15" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="J5" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="71"/>
-      <c r="L5" s="37" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A6" s="100"/>
-      <c r="B6" s="103" t="s">
+      <c r="J5" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K5" s="95" t="s">
+        <v>117</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="82"/>
+      <c r="B6" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="49">
+      <c r="C6" s="41">
         <v>50</v>
       </c>
-      <c r="D6" s="50"/>
-      <c r="E6" s="17" t="s">
+      <c r="D6" s="42"/>
+      <c r="E6" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="23" t="s">
+        <v>105</v>
+      </c>
+      <c r="G6" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I6" s="34" t="s">
         <v>106</v>
       </c>
-      <c r="G6" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="H6" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="I6" s="43" t="s">
-        <v>107</v>
-      </c>
-      <c r="J6" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K6" s="71"/>
-      <c r="L6" s="37"/>
-    </row>
-    <row r="7" spans="1:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="101"/>
-      <c r="B7" s="104"/>
-      <c r="C7" s="51">
+      <c r="J6" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K6" s="95"/>
+      <c r="L6" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="83"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="43">
         <v>60</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="E7" s="18" t="s">
+      <c r="D7" s="44"/>
+      <c r="E7" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="28" t="s">
+      <c r="F7" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="G7" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H7" s="18" t="s">
+      <c r="G7" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="H7" s="17" t="s">
         <v>64</v>
       </c>
-      <c r="I7" s="44" t="s">
+      <c r="I7" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="68" t="s">
-        <v>33</v>
-      </c>
-      <c r="K7" s="74"/>
-      <c r="L7" s="38"/>
-    </row>
-    <row r="8" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="99" t="s">
+      <c r="J7" s="59" t="s">
+        <v>33</v>
+      </c>
+      <c r="K7" s="96"/>
+      <c r="L7" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8" s="81" t="s">
         <v>6</v>
       </c>
-      <c r="B8" s="102" t="s">
+      <c r="B8" s="84" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="47">
+      <c r="C8" s="39">
         <v>70</v>
       </c>
-      <c r="D8" s="48"/>
+      <c r="D8" s="40"/>
       <c r="E8" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="F8" s="30" t="s">
+      <c r="F8" s="27" t="s">
         <v>54</v>
       </c>
-      <c r="G8" s="64" t="s">
+      <c r="G8" s="55" t="s">
         <v>32</v>
       </c>
       <c r="H8" s="9" t="s">
-        <v>108</v>
-      </c>
-      <c r="I8" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="I8" s="37" t="s">
         <v>55</v>
       </c>
-      <c r="J8" s="69" t="s">
-        <v>33</v>
-      </c>
-      <c r="K8" s="75"/>
-      <c r="L8" s="36"/>
-    </row>
-    <row r="9" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="100"/>
-      <c r="B9" s="103"/>
-      <c r="C9" s="49">
+      <c r="J8" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="K8" s="94" t="s">
+        <v>178</v>
+      </c>
+      <c r="L8" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="82"/>
+      <c r="B9" s="85"/>
+      <c r="C9" s="41">
         <v>80</v>
       </c>
-      <c r="D9" s="50"/>
+      <c r="D9" s="42"/>
       <c r="E9" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="F9" s="25" t="s">
+      <c r="F9" s="23" t="s">
         <v>58</v>
       </c>
-      <c r="G9" s="60" t="s">
+      <c r="G9" s="52" t="s">
         <v>32</v>
       </c>
       <c r="H9" s="10" t="s">
-        <v>108</v>
-      </c>
-      <c r="I9" s="41" t="s">
+        <v>107</v>
+      </c>
+      <c r="I9" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="J9" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K9" s="71"/>
-      <c r="L9" s="37" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A10" s="100"/>
-      <c r="B10" s="103"/>
-      <c r="C10" s="49">
+      <c r="J9" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" s="95" t="s">
+        <v>149</v>
+      </c>
+      <c r="L9" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="82"/>
+      <c r="B10" s="85"/>
+      <c r="C10" s="41">
         <v>90</v>
       </c>
-      <c r="D10" s="50"/>
+      <c r="D10" s="42"/>
       <c r="E10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="25" t="s">
+      <c r="F10" s="23" t="s">
         <v>59</v>
       </c>
-      <c r="G10" s="60" t="s">
+      <c r="G10" s="52" t="s">
         <v>32</v>
       </c>
       <c r="H10" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="I10" s="41" t="s">
+        <v>113</v>
+      </c>
+      <c r="I10" s="34" t="s">
         <v>60</v>
       </c>
-      <c r="J10" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K10" s="71"/>
-      <c r="L10" s="37" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="100"/>
-      <c r="B11" s="103" t="s">
+      <c r="J10" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K10" s="95" t="s">
+        <v>109</v>
+      </c>
+      <c r="L10" s="30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="82"/>
+      <c r="B11" s="85" t="s">
         <v>8</v>
       </c>
-      <c r="C11" s="49">
+      <c r="C11" s="41">
         <v>100</v>
       </c>
-      <c r="D11" s="50"/>
+      <c r="D11" s="42"/>
       <c r="E11" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="F11" s="26" t="s">
-        <v>105</v>
-      </c>
-      <c r="G11" s="61" t="s">
+      <c r="F11" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="G11" s="53" t="s">
         <v>32</v>
       </c>
       <c r="H11" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="I11" s="42" t="s">
+      <c r="I11" s="35" t="s">
         <v>65</v>
       </c>
-      <c r="J11" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K11" s="71"/>
-      <c r="L11" s="37" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A12" s="100"/>
-      <c r="B12" s="103"/>
-      <c r="C12" s="49">
+      <c r="J11" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K11" s="95" t="s">
+        <v>150</v>
+      </c>
+      <c r="L11" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A12" s="82"/>
+      <c r="B12" s="85"/>
+      <c r="C12" s="41">
         <v>110</v>
       </c>
-      <c r="D12" s="50"/>
+      <c r="D12" s="42"/>
       <c r="E12" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="F12" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="G12" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="H12" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="F12" s="25" t="s">
-        <v>113</v>
-      </c>
-      <c r="G12" s="60" t="s">
-        <v>32</v>
-      </c>
-      <c r="H12" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="I12" s="41" t="s">
+      <c r="I12" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="J12" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K12" s="71"/>
-      <c r="L12" s="37"/>
-    </row>
-    <row r="13" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J12" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K12" s="95"/>
+      <c r="L12" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="101"/>
-      <c r="B13" s="104"/>
-      <c r="C13" s="51">
+      <c r="B13" s="92"/>
+      <c r="C13" s="47">
+        <v>115</v>
+      </c>
+      <c r="D13" s="48"/>
+      <c r="E13" s="72" t="s">
+        <v>179</v>
+      </c>
+      <c r="F13" s="73" t="s">
+        <v>180</v>
+      </c>
+      <c r="G13" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="H13" s="72" t="s">
+        <v>111</v>
+      </c>
+      <c r="I13" s="102" t="s">
+        <v>74</v>
+      </c>
+      <c r="J13" s="61"/>
+      <c r="K13" s="98"/>
+      <c r="L13" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="83"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="43">
         <v>120</v>
       </c>
-      <c r="D13" s="52"/>
-      <c r="E13" s="18" t="s">
+      <c r="D14" s="44"/>
+      <c r="E14" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="F13" s="28" t="s">
+      <c r="F14" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="G13" s="63" t="s">
-        <v>32</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>117</v>
-      </c>
-      <c r="I13" s="44" t="s">
+      <c r="G14" s="54" t="s">
+        <v>32</v>
+      </c>
+      <c r="H14" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="I14" s="36" t="s">
         <v>68</v>
       </c>
-      <c r="J13" s="70" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" s="72"/>
-      <c r="L13" s="38"/>
-    </row>
-    <row r="14" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A14" s="99" t="s">
+      <c r="J14" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" s="96"/>
+      <c r="L14" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="81" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="102" t="s">
+      <c r="B15" s="84" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="47">
+      <c r="C15" s="39">
         <v>130</v>
       </c>
-      <c r="D14" s="48"/>
-      <c r="E14" s="16" t="s">
+      <c r="D15" s="40"/>
+      <c r="E15" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F15" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="G14" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="H14" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="I14" s="23" t="s">
-        <v>71</v>
-      </c>
-      <c r="J14" s="66" t="s">
-        <v>32</v>
-      </c>
-      <c r="K14" s="73"/>
-      <c r="L14" s="36" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="100"/>
-      <c r="B15" s="103"/>
-      <c r="C15" s="49">
-        <v>140</v>
-      </c>
-      <c r="D15" s="50"/>
-      <c r="E15" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="F15" s="26" t="s">
-        <v>77</v>
-      </c>
-      <c r="G15" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>72</v>
+      <c r="G15" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>114</v>
       </c>
       <c r="I15" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="J15" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K15" s="71"/>
-      <c r="L15" s="37" t="s">
+      <c r="J15" s="57" t="s">
+        <v>32</v>
+      </c>
+      <c r="K15" s="94" t="s">
+        <v>117</v>
+      </c>
+      <c r="L15" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="82"/>
+      <c r="B16" s="85"/>
+      <c r="C16" s="41">
+        <v>140</v>
+      </c>
+      <c r="D16" s="42"/>
+      <c r="E16" s="15" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="G16" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="H16" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="I16" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="J16" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K16" s="95" t="s">
+        <v>117</v>
+      </c>
+      <c r="L16" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="82"/>
+      <c r="B17" s="85" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" s="41">
+        <v>150</v>
+      </c>
+      <c r="D17" s="42"/>
+      <c r="E17" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="F17" s="23" t="s">
+        <v>148</v>
+      </c>
+      <c r="G17" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="H17" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="I17" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="J17" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K17" s="95"/>
+      <c r="L17" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="82"/>
+      <c r="B18" s="85"/>
+      <c r="C18" s="41">
+        <v>160</v>
+      </c>
+      <c r="D18" s="42"/>
+      <c r="E18" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="F18" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G18" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="H18" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="I18" s="20" t="s">
+        <v>74</v>
+      </c>
+      <c r="J18" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K18" s="95" t="s">
+        <v>117</v>
+      </c>
+      <c r="L18" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="82"/>
+      <c r="B19" s="92" t="s">
+        <v>14</v>
+      </c>
+      <c r="C19" s="41">
+        <v>165</v>
+      </c>
+      <c r="D19" s="42"/>
+      <c r="E19" s="10" t="s">
+        <v>172</v>
+      </c>
+      <c r="F19" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="G19" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="10" t="s">
+        <v>174</v>
+      </c>
+      <c r="I19" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="J19" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K19" s="95"/>
+      <c r="L19" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="72" x14ac:dyDescent="0.3">
+      <c r="A20" s="82"/>
+      <c r="B20" s="87"/>
+      <c r="C20" s="41">
+        <v>170</v>
+      </c>
+      <c r="D20" s="42"/>
+      <c r="E20" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="F20" s="23" t="s">
+        <v>141</v>
+      </c>
+      <c r="G20" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="H20" s="10" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A16" s="100"/>
-      <c r="B16" s="103" t="s">
-        <v>13</v>
-      </c>
-      <c r="C16" s="49">
-        <v>150</v>
-      </c>
-      <c r="D16" s="50"/>
-      <c r="E16" s="17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F16" s="27" t="s">
-        <v>149</v>
-      </c>
-      <c r="G16" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="H16" s="17" t="s">
-        <v>73</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="J16" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K16" s="71"/>
-      <c r="L16" s="37"/>
-    </row>
-    <row r="17" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="100"/>
-      <c r="B17" s="103"/>
-      <c r="C17" s="49">
-        <v>160</v>
-      </c>
-      <c r="D17" s="50"/>
-      <c r="E17" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="F17" s="26" t="s">
-        <v>75</v>
-      </c>
-      <c r="G17" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="I17" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="J17" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K17" s="71"/>
-      <c r="L17" s="37" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A18" s="100"/>
-      <c r="B18" s="110" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="49">
-        <v>165</v>
-      </c>
-      <c r="D18" s="50"/>
-      <c r="E18" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="F18" s="27" t="s">
-        <v>174</v>
-      </c>
-      <c r="G18" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="H18" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="I18" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="J18" s="67"/>
-      <c r="K18" s="71"/>
-      <c r="L18" s="37"/>
-    </row>
-    <row r="19" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A19" s="100"/>
-      <c r="B19" s="105"/>
-      <c r="C19" s="49">
-        <v>170</v>
-      </c>
-      <c r="D19" s="50"/>
-      <c r="E19" s="17" t="s">
+      <c r="I20" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="J20" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K20" s="95" t="s">
+        <v>151</v>
+      </c>
+      <c r="L20" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="82"/>
+      <c r="B21" s="87"/>
+      <c r="C21" s="41">
+        <v>180</v>
+      </c>
+      <c r="D21" s="42"/>
+      <c r="E21" s="62" t="s">
+        <v>19</v>
+      </c>
+      <c r="F21" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="G21" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="J21" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K21" s="95" t="s">
+        <v>152</v>
+      </c>
+      <c r="L21" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="82"/>
+      <c r="B22" s="87"/>
+      <c r="C22" s="41">
+        <v>190</v>
+      </c>
+      <c r="D22" s="42"/>
+      <c r="E22" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="F22" s="23" t="s">
+        <v>142</v>
+      </c>
+      <c r="G22" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="H22" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="I22" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="J22" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K22" s="95"/>
+      <c r="L22" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="82"/>
+      <c r="B23" s="87"/>
+      <c r="C23" s="41">
+        <v>200</v>
+      </c>
+      <c r="D23" s="42"/>
+      <c r="E23" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="F23" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="G23" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="H23" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="F19" s="27" t="s">
-        <v>142</v>
-      </c>
-      <c r="G19" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="H19" s="17" t="s">
-        <v>119</v>
-      </c>
-      <c r="I19" s="22" t="s">
+      <c r="I23" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="J19" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K19" s="71"/>
-      <c r="L19" s="37" t="s">
+      <c r="J23" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K23" s="95" t="s">
+        <v>153</v>
+      </c>
+      <c r="L23" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="82"/>
+      <c r="B24" s="87"/>
+      <c r="C24" s="41">
+        <v>210</v>
+      </c>
+      <c r="D24" s="42"/>
+      <c r="E24" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F24" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="G24" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="I24" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="J24" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K24" s="95" t="s">
         <v>152</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="100"/>
-      <c r="B20" s="105"/>
-      <c r="C20" s="49">
-        <v>180</v>
-      </c>
-      <c r="D20" s="50"/>
-      <c r="E20" s="76" t="s">
-        <v>19</v>
-      </c>
-      <c r="F20" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="G20" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="I20" s="21" t="s">
+      <c r="L24" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="82"/>
+      <c r="B25" s="91"/>
+      <c r="C25" s="41">
+        <v>220</v>
+      </c>
+      <c r="D25" s="42"/>
+      <c r="E25" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="F25" s="23" t="s">
+        <v>125</v>
+      </c>
+      <c r="G25" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="I25" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="J25" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K25" s="95"/>
+      <c r="L25" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="82"/>
+      <c r="B26" s="85" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="41">
+        <v>230</v>
+      </c>
+      <c r="D26" s="42"/>
+      <c r="E26" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="F26" s="23" t="s">
+        <v>128</v>
+      </c>
+      <c r="G26" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="I26" s="19" t="s">
         <v>79</v>
       </c>
-      <c r="J20" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K20" s="71"/>
-      <c r="L20" s="37" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="75" x14ac:dyDescent="0.25">
-      <c r="A21" s="100"/>
-      <c r="B21" s="105"/>
-      <c r="C21" s="49">
-        <v>190</v>
-      </c>
-      <c r="D21" s="50"/>
-      <c r="E21" s="17" t="s">
-        <v>122</v>
-      </c>
-      <c r="F21" s="27" t="s">
-        <v>143</v>
-      </c>
-      <c r="G21" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="H21" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="I21" s="22" t="s">
-        <v>79</v>
-      </c>
-      <c r="J21" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K21" s="71"/>
-      <c r="L21" s="37"/>
-    </row>
-    <row r="22" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="100"/>
-      <c r="B22" s="105"/>
-      <c r="C22" s="49">
-        <v>200</v>
-      </c>
-      <c r="D22" s="50"/>
-      <c r="E22" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="G22" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="I22" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="J22" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K22" s="71"/>
-      <c r="L22" s="37" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A23" s="100"/>
-      <c r="B23" s="105"/>
-      <c r="C23" s="49">
-        <v>210</v>
-      </c>
-      <c r="D23" s="50"/>
-      <c r="E23" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="F23" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="G23" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="H23" s="15" t="s">
-        <v>81</v>
-      </c>
-      <c r="I23" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="J23" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K23" s="71"/>
-      <c r="L23" s="37" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="100"/>
-      <c r="B24" s="109"/>
-      <c r="C24" s="49">
-        <v>220</v>
-      </c>
-      <c r="D24" s="50"/>
-      <c r="E24" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="F24" s="27" t="s">
-        <v>126</v>
-      </c>
-      <c r="G24" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="H24" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="I24" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="J24" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K24" s="71"/>
-      <c r="L24" s="37"/>
-    </row>
-    <row r="25" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A25" s="100"/>
-      <c r="B25" s="103" t="s">
-        <v>26</v>
-      </c>
-      <c r="C25" s="49">
-        <v>230</v>
-      </c>
-      <c r="D25" s="50"/>
-      <c r="E25" s="10" t="s">
-        <v>128</v>
-      </c>
-      <c r="F25" s="25" t="s">
-        <v>129</v>
-      </c>
-      <c r="G25" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="H25" s="10" t="s">
+      <c r="J26" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K26" s="95"/>
+      <c r="L26" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="82"/>
+      <c r="B27" s="85"/>
+      <c r="C27" s="41">
+        <v>240</v>
+      </c>
+      <c r="D27" s="42"/>
+      <c r="E27" s="15" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="G27" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="H27" s="15" t="s">
         <v>72</v>
-      </c>
-      <c r="I25" s="20" t="s">
-        <v>79</v>
-      </c>
-      <c r="J25" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K25" s="71"/>
-      <c r="L25" s="37"/>
-    </row>
-    <row r="26" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="100"/>
-      <c r="B26" s="103"/>
-      <c r="C26" s="49">
-        <v>240</v>
-      </c>
-      <c r="D26" s="50"/>
-      <c r="E26" s="15" t="s">
-        <v>25</v>
-      </c>
-      <c r="F26" s="26" t="s">
-        <v>84</v>
-      </c>
-      <c r="G26" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="H26" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="I26" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="J26" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K26" s="71"/>
-      <c r="L26" s="37" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="100"/>
-      <c r="B27" s="103"/>
-      <c r="C27" s="49">
-        <v>250</v>
-      </c>
-      <c r="D27" s="50"/>
-      <c r="E27" s="10" t="s">
-        <v>124</v>
-      </c>
-      <c r="F27" s="25" t="s">
-        <v>125</v>
-      </c>
-      <c r="G27" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="H27" s="10" t="s">
-        <v>130</v>
       </c>
       <c r="I27" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="J27" s="67" t="s">
-        <v>172</v>
-      </c>
-      <c r="K27" s="71"/>
-      <c r="L27" s="37" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="101"/>
-      <c r="B28" s="104"/>
-      <c r="C28" s="51">
+      <c r="J27" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K27" s="95" t="s">
+        <v>154</v>
+      </c>
+      <c r="L27" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A28" s="82"/>
+      <c r="B28" s="85"/>
+      <c r="C28" s="41">
+        <v>250</v>
+      </c>
+      <c r="D28" s="42"/>
+      <c r="E28" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="F28" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="G28" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="H28" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="I28" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="J28" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="K28" s="95" t="s">
+        <v>130</v>
+      </c>
+      <c r="L28" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" ht="43.8" hidden="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="83"/>
+      <c r="B29" s="86"/>
+      <c r="C29" s="43">
         <v>260</v>
       </c>
-      <c r="D28" s="52"/>
-      <c r="E28" s="77" t="s">
+      <c r="D29" s="44"/>
+      <c r="E29" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="F28" s="78" t="s">
+      <c r="F29" s="64" t="s">
         <v>86</v>
       </c>
-      <c r="G28" s="79" t="s">
-        <v>33</v>
-      </c>
-      <c r="H28" s="77" t="s">
+      <c r="G29" s="65" t="s">
+        <v>33</v>
+      </c>
+      <c r="H29" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="I28" s="80" t="s">
+      <c r="I29" s="66" t="s">
         <v>79</v>
       </c>
-      <c r="J28" s="68" t="s">
-        <v>32</v>
-      </c>
-      <c r="K28" s="74"/>
-      <c r="L28" s="38" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="106" t="s">
+      <c r="J29" s="59" t="s">
+        <v>32</v>
+      </c>
+      <c r="K29" s="96" t="s">
+        <v>155</v>
+      </c>
+      <c r="L29" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" ht="45" hidden="1" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="88" t="s">
+        <v>167</v>
+      </c>
+      <c r="B30" s="90" t="s">
+        <v>166</v>
+      </c>
+      <c r="C30" s="45">
+        <v>270</v>
+      </c>
+      <c r="D30" s="46"/>
+      <c r="E30" s="16" t="s">
+        <v>88</v>
+      </c>
+      <c r="F30" s="26" t="s">
+        <v>78</v>
+      </c>
+      <c r="G30" s="56" t="s">
+        <v>33</v>
+      </c>
+      <c r="H30" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="I30" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="60" t="s">
+        <v>32</v>
+      </c>
+      <c r="K30" s="94" t="s">
+        <v>117</v>
+      </c>
+      <c r="L30" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="89"/>
+      <c r="B31" s="87"/>
+      <c r="C31" s="41">
+        <v>280</v>
+      </c>
+      <c r="D31" s="42"/>
+      <c r="E31" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F31" s="23" t="s">
+        <v>143</v>
+      </c>
+      <c r="G31" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="H31" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="I31" s="19" t="s">
+        <v>132</v>
+      </c>
+      <c r="J31" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K31" s="95"/>
+      <c r="L31" s="30" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="89"/>
+      <c r="B32" s="87"/>
+      <c r="C32" s="41">
+        <v>290</v>
+      </c>
+      <c r="D32" s="42"/>
+      <c r="E32" s="15" t="s">
+        <v>135</v>
+      </c>
+      <c r="F32" s="24" t="s">
+        <v>134</v>
+      </c>
+      <c r="G32" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="H32" s="15" t="s">
+        <v>90</v>
+      </c>
+      <c r="I32" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="J32" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K32" s="95" t="s">
+        <v>136</v>
+      </c>
+      <c r="L32" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A33" s="89"/>
+      <c r="B33" s="87"/>
+      <c r="C33" s="41">
+        <v>295</v>
+      </c>
+      <c r="D33" s="42"/>
+      <c r="E33" s="10" t="s">
         <v>168</v>
       </c>
-      <c r="B29" s="108" t="s">
-        <v>167</v>
-      </c>
-      <c r="C29" s="53">
-        <v>270</v>
-      </c>
-      <c r="D29" s="54"/>
-      <c r="E29" s="16" t="s">
-        <v>88</v>
-      </c>
-      <c r="F29" s="29" t="s">
-        <v>78</v>
-      </c>
-      <c r="G29" s="65" t="s">
-        <v>33</v>
-      </c>
-      <c r="H29" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="I29" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="J29" s="69" t="s">
-        <v>32</v>
-      </c>
-      <c r="K29" s="75"/>
-      <c r="L29" s="36" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A30" s="107"/>
-      <c r="B30" s="105"/>
-      <c r="C30" s="49">
-        <v>280</v>
-      </c>
-      <c r="D30" s="50"/>
-      <c r="E30" s="17" t="s">
-        <v>134</v>
-      </c>
-      <c r="F30" s="27" t="s">
+      <c r="F33" s="23" t="s">
+        <v>169</v>
+      </c>
+      <c r="G33" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="H33" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="I33" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="J33" s="58" t="s">
+        <v>171</v>
+      </c>
+      <c r="K33" s="95"/>
+      <c r="L33" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="89"/>
+      <c r="B34" s="87"/>
+      <c r="C34" s="41">
+        <v>300</v>
+      </c>
+      <c r="D34" s="42"/>
+      <c r="E34" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="F34" s="23" t="s">
         <v>144</v>
       </c>
-      <c r="G30" s="62" t="s">
-        <v>32</v>
-      </c>
-      <c r="H30" s="17" t="s">
-        <v>89</v>
-      </c>
-      <c r="I30" s="22" t="s">
-        <v>133</v>
-      </c>
-      <c r="J30" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K30" s="71"/>
-      <c r="L30" s="37"/>
-    </row>
-    <row r="31" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="107"/>
-      <c r="B31" s="105"/>
-      <c r="C31" s="49">
-        <v>290</v>
-      </c>
-      <c r="D31" s="50"/>
-      <c r="E31" s="15" t="s">
-        <v>136</v>
-      </c>
-      <c r="F31" s="26" t="s">
-        <v>135</v>
-      </c>
-      <c r="G31" s="61" t="s">
-        <v>32</v>
-      </c>
-      <c r="H31" s="15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I31" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="J31" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K31" s="71"/>
-      <c r="L31" s="37" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="107"/>
-      <c r="B32" s="105"/>
-      <c r="C32" s="49">
-        <v>295</v>
-      </c>
-      <c r="D32" s="50"/>
-      <c r="E32" s="17" t="s">
-        <v>169</v>
-      </c>
-      <c r="F32" s="27" t="s">
-        <v>170</v>
-      </c>
-      <c r="G32" s="62" t="s">
-        <v>33</v>
-      </c>
-      <c r="H32" s="17" t="s">
-        <v>171</v>
-      </c>
-      <c r="I32" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="J32" s="98" t="s">
-        <v>172</v>
-      </c>
-      <c r="K32" s="71"/>
-      <c r="L32" s="37"/>
-    </row>
-    <row r="33" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A33" s="107"/>
-      <c r="B33" s="105"/>
-      <c r="C33" s="49">
-        <v>300</v>
-      </c>
-      <c r="D33" s="50"/>
-      <c r="E33" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="F33" s="25" t="s">
+      <c r="G34" s="52" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I34" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="J34" s="58" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" s="95"/>
+      <c r="L34" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="89"/>
+      <c r="B35" s="87"/>
+      <c r="C35" s="41">
+        <v>310</v>
+      </c>
+      <c r="D35" s="42"/>
+      <c r="E35" s="15" t="s">
+        <v>139</v>
+      </c>
+      <c r="F35" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="G33" s="60" t="s">
-        <v>32</v>
-      </c>
-      <c r="H33" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I33" s="20" t="s">
-        <v>139</v>
-      </c>
-      <c r="J33" s="67" t="s">
-        <v>33</v>
-      </c>
-      <c r="K33" s="71"/>
-      <c r="L33" s="37"/>
-    </row>
-    <row r="34" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="107"/>
-      <c r="B34" s="105"/>
-      <c r="C34" s="49">
-        <v>310</v>
-      </c>
-      <c r="D34" s="50"/>
-      <c r="E34" s="15" t="s">
-        <v>140</v>
-      </c>
-      <c r="F34" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="G34" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="H34" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I34" s="21" t="s">
-        <v>138</v>
-      </c>
-      <c r="J34" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K34" s="71"/>
-      <c r="L34" s="37" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="107"/>
-      <c r="B35" s="105"/>
-      <c r="C35" s="49">
-        <v>320</v>
-      </c>
-      <c r="D35" s="50"/>
-      <c r="E35" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="F35" s="26" t="s">
-        <v>96</v>
-      </c>
-      <c r="G35" s="61" t="s">
+      <c r="G35" s="53" t="s">
         <v>33</v>
       </c>
       <c r="H35" s="15" t="s">
         <v>94</v>
       </c>
-      <c r="I35" s="21" t="s">
+      <c r="I35" s="20" t="s">
+        <v>137</v>
+      </c>
+      <c r="J35" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K35" s="95" t="s">
+        <v>156</v>
+      </c>
+      <c r="L35" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="89"/>
+      <c r="B36" s="87"/>
+      <c r="C36" s="41">
+        <v>320</v>
+      </c>
+      <c r="D36" s="42"/>
+      <c r="E36" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="F36" s="24" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="H36" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I36" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="J35" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K35" s="71"/>
-      <c r="L35" s="37" t="s">
+      <c r="J36" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K36" s="95" t="s">
+        <v>157</v>
+      </c>
+      <c r="L36" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="89"/>
+      <c r="B37" s="87"/>
+      <c r="C37" s="41">
+        <v>330</v>
+      </c>
+      <c r="D37" s="42"/>
+      <c r="E37" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F37" s="24" t="s">
+        <v>97</v>
+      </c>
+      <c r="G37" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="H37" s="15" t="s">
+        <v>95</v>
+      </c>
+      <c r="I37" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="J37" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K37" s="95" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="36" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="107"/>
-      <c r="B36" s="105"/>
-      <c r="C36" s="49">
-        <v>330</v>
-      </c>
-      <c r="D36" s="50"/>
-      <c r="E36" s="15" t="s">
-        <v>35</v>
-      </c>
-      <c r="F36" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="G36" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="H36" s="15" t="s">
+      <c r="L37" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="89"/>
+      <c r="B38" s="87"/>
+      <c r="C38" s="41">
+        <v>340</v>
+      </c>
+      <c r="D38" s="42"/>
+      <c r="E38" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F38" s="24" t="s">
+        <v>92</v>
+      </c>
+      <c r="G38" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="H38" s="15" t="s">
+        <v>94</v>
+      </c>
+      <c r="I38" s="20" t="s">
+        <v>79</v>
+      </c>
+      <c r="J38" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K38" s="95" t="s">
+        <v>157</v>
+      </c>
+      <c r="L38" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="89"/>
+      <c r="B39" s="91"/>
+      <c r="C39" s="41">
+        <v>350</v>
+      </c>
+      <c r="D39" s="42"/>
+      <c r="E39" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="F39" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="G39" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="H39" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="I36" s="21" t="s">
+      <c r="I39" s="20" t="s">
         <v>79</v>
       </c>
-      <c r="J36" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K36" s="71"/>
-      <c r="L36" s="37" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A37" s="107"/>
-      <c r="B37" s="105"/>
-      <c r="C37" s="49">
-        <v>340</v>
-      </c>
-      <c r="D37" s="50"/>
-      <c r="E37" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F37" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="G37" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="H37" s="15" t="s">
-        <v>94</v>
-      </c>
-      <c r="I37" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="J37" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K37" s="71"/>
-      <c r="L37" s="37" t="s">
+      <c r="J39" s="58" t="s">
+        <v>32</v>
+      </c>
+      <c r="K39" s="95" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" ht="30" x14ac:dyDescent="0.25">
-      <c r="A38" s="107"/>
-      <c r="B38" s="109"/>
-      <c r="C38" s="49">
-        <v>350</v>
-      </c>
-      <c r="D38" s="50"/>
-      <c r="E38" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="F38" s="26" t="s">
-        <v>93</v>
-      </c>
-      <c r="G38" s="61" t="s">
-        <v>33</v>
-      </c>
-      <c r="H38" s="15" t="s">
-        <v>95</v>
-      </c>
-      <c r="I38" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="J38" s="67" t="s">
-        <v>32</v>
-      </c>
-      <c r="K38" s="71"/>
-      <c r="L38" s="37" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="39" spans="1:12" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="107"/>
-      <c r="B39" s="105" t="s">
+      <c r="L39" s="30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A40" s="89"/>
+      <c r="B40" s="87" t="s">
+        <v>146</v>
+      </c>
+      <c r="C40" s="45">
+        <v>360</v>
+      </c>
+      <c r="D40" s="46"/>
+      <c r="E40" s="68" t="s">
         <v>147</v>
       </c>
-      <c r="C39" s="53">
-        <v>360</v>
-      </c>
-      <c r="D39" s="54"/>
-      <c r="E39" s="82" t="s">
-        <v>148</v>
-      </c>
-      <c r="F39" s="83" t="s">
+      <c r="F40" s="69" t="s">
+        <v>164</v>
+      </c>
+      <c r="G40" s="70" t="s">
+        <v>33</v>
+      </c>
+      <c r="H40" s="68" t="s">
         <v>165</v>
       </c>
-      <c r="G39" s="84" t="s">
-        <v>33</v>
-      </c>
-      <c r="H39" s="82" t="s">
-        <v>166</v>
-      </c>
-      <c r="I39" s="85" t="s">
+      <c r="I40" s="71" t="s">
         <v>74</v>
       </c>
-      <c r="J39" s="69"/>
-      <c r="K39" s="75"/>
-      <c r="L39" s="86"/>
-    </row>
-    <row r="40" spans="1:12" ht="45" x14ac:dyDescent="0.25">
-      <c r="A40" s="107"/>
-      <c r="B40" s="105"/>
-      <c r="C40" s="49">
+      <c r="J40" s="60"/>
+      <c r="K40" s="97"/>
+      <c r="L40" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41" s="89"/>
+      <c r="B41" s="87"/>
+      <c r="C41" s="41">
         <v>370</v>
       </c>
-      <c r="D40" s="50"/>
-      <c r="E40" s="10" t="s">
+      <c r="D41" s="42"/>
+      <c r="E41" s="10" t="s">
+        <v>161</v>
+      </c>
+      <c r="F41" s="23" t="s">
+        <v>163</v>
+      </c>
+      <c r="G41" s="52" t="s">
+        <v>33</v>
+      </c>
+      <c r="H41" s="10" t="s">
+        <v>165</v>
+      </c>
+      <c r="I41" s="19" t="s">
+        <v>74</v>
+      </c>
+      <c r="J41" s="58"/>
+      <c r="K41" s="95"/>
+      <c r="L41" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="89"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="47">
+        <v>380</v>
+      </c>
+      <c r="D42" s="48"/>
+      <c r="E42" s="72" t="s">
         <v>162</v>
       </c>
-      <c r="F40" s="25" t="s">
-        <v>164</v>
-      </c>
-      <c r="G40" s="60" t="s">
-        <v>33</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>166</v>
-      </c>
-      <c r="I40" s="20" t="s">
+      <c r="F42" s="73" t="s">
+        <v>160</v>
+      </c>
+      <c r="G42" s="74" t="s">
+        <v>33</v>
+      </c>
+      <c r="H42" s="72" t="s">
+        <v>165</v>
+      </c>
+      <c r="I42" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="J40" s="67"/>
-      <c r="K40" s="71"/>
-      <c r="L40" s="37"/>
-    </row>
-    <row r="41" spans="1:12" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="107"/>
-      <c r="B41" s="105"/>
-      <c r="C41" s="55">
-        <v>380</v>
-      </c>
-      <c r="D41" s="56"/>
-      <c r="E41" s="87" t="s">
-        <v>163</v>
-      </c>
-      <c r="F41" s="88" t="s">
-        <v>161</v>
-      </c>
-      <c r="G41" s="89" t="s">
-        <v>33</v>
-      </c>
-      <c r="H41" s="87" t="s">
-        <v>166</v>
-      </c>
-      <c r="I41" s="90" t="s">
-        <v>74</v>
-      </c>
-      <c r="J41" s="70"/>
-      <c r="K41" s="72"/>
-      <c r="L41" s="91"/>
-    </row>
-    <row r="42" spans="1:12" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="46" t="s">
+      <c r="J42" s="61"/>
+      <c r="K42" s="98"/>
+      <c r="L42" s="30" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" ht="115.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="38" t="s">
         <v>37</v>
       </c>
-      <c r="B42" s="81" t="s">
+      <c r="B43" s="67" t="s">
         <v>40</v>
       </c>
-      <c r="C42" s="57">
+      <c r="C43" s="49">
         <v>390</v>
       </c>
-      <c r="D42" s="58"/>
-      <c r="E42" s="92" t="s">
+      <c r="D43" s="50"/>
+      <c r="E43" s="76" t="s">
         <v>41</v>
       </c>
-      <c r="F42" s="93" t="s">
-        <v>132</v>
-      </c>
-      <c r="G42" s="94" t="s">
-        <v>33</v>
-      </c>
-      <c r="H42" s="92" t="s">
-        <v>166</v>
-      </c>
-      <c r="I42" s="95" t="s">
+      <c r="F43" s="77" t="s">
+        <v>131</v>
+      </c>
+      <c r="G43" s="78" t="s">
+        <v>33</v>
+      </c>
+      <c r="H43" s="76" t="s">
+        <v>165</v>
+      </c>
+      <c r="I43" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="J42" s="96"/>
-      <c r="K42" s="97"/>
-      <c r="L42" s="35"/>
+      <c r="J43" s="80"/>
+      <c r="K43" s="99"/>
+      <c r="L43" s="31" t="s">
+        <v>177</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:L42" xr:uid="{370A0B0F-C0FD-4EC3-B4F7-C3AB5FE65C83}"/>
+  <autoFilter ref="A1:L43" xr:uid="{CD7B405C-B925-43EB-A348-6C5A23DE5406}">
+    <filterColumn colId="11">
+      <filters>
+        <filter val="M"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <mergeCells count="15">
-    <mergeCell ref="B39:B41"/>
-    <mergeCell ref="A29:A41"/>
-    <mergeCell ref="A14:A28"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="B25:B28"/>
-    <mergeCell ref="B29:B38"/>
-    <mergeCell ref="B18:B24"/>
+    <mergeCell ref="B40:B42"/>
+    <mergeCell ref="A30:A42"/>
+    <mergeCell ref="A15:A29"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="B17:B18"/>
+    <mergeCell ref="B26:B29"/>
+    <mergeCell ref="B30:B39"/>
+    <mergeCell ref="B19:B25"/>
     <mergeCell ref="A2:A7"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="B4:B5"/>
     <mergeCell ref="B6:B7"/>
-    <mergeCell ref="A8:A13"/>
-    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A8:A14"/>
+    <mergeCell ref="B11:B14"/>
     <mergeCell ref="B8:B10"/>
   </mergeCells>
   <conditionalFormatting sqref="G2:G1048576">
@@ -3245,7 +3420,7 @@
       <formula>NOT(ISERROR(SEARCH("N",G2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:K42">
+  <conditionalFormatting sqref="J2:J43">
     <cfRule type="containsText" dxfId="4" priority="4" operator="containsText" text="P">
       <formula>NOT(ISERROR(SEARCH("P",J2)))</formula>
     </cfRule>
@@ -3258,12 +3433,12 @@
       <formula>NOT(ISERROR(SEARCH("N",J1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="D2:D42">
+  <conditionalFormatting sqref="D2:D43">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J2:J42">
+  <conditionalFormatting sqref="J2:J43">
     <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="R">
       <formula>NOT(ISERROR(SEARCH("R",J2)))</formula>
     </cfRule>

</xml_diff>

<commit_message>
sync pc with git2
</commit_message>
<xml_diff>
--- a/TESTCASES/TestCases.xlsx
+++ b/TESTCASES/TestCases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike1\Documents\TestCase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3557D4-1121-4D7A-A9AC-8AD0A7C435EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CD5D413-0FB9-4918-9FC2-DE460F2F44CD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
   </bookViews>
@@ -438,9 +438,6 @@
     <t>Test 10 different combinations. Check all entities eventually end up at their goal (nothing gets stuck)</t>
   </si>
   <si>
-    <t>Object down stairs with people overtaking</t>
-  </si>
-  <si>
     <t>Set tasks for people to pick up and drop off object. Check they can do this and the appropriate prep time is achieved. Check multiple pickups work for same attendants</t>
   </si>
   <si>
@@ -558,24 +555,6 @@
     <t>Object follows its stair and landing lanes</t>
   </si>
   <si>
-    <t>DS1</t>
-  </si>
-  <si>
-    <t>DS2</t>
-  </si>
-  <si>
-    <t>DS3</t>
-  </si>
-  <si>
-    <t>DS4</t>
-  </si>
-  <si>
-    <t>DS5</t>
-  </si>
-  <si>
-    <t>DS6</t>
-  </si>
-  <si>
     <t>IN8</t>
   </si>
   <si>
@@ -598,6 +577,27 @@
   </si>
   <si>
     <t>Issue with pick up person - waiting on peter</t>
+  </si>
+  <si>
+    <t>People can overtake an object going down stairs</t>
+  </si>
+  <si>
+    <t>FF2</t>
+  </si>
+  <si>
+    <t>FF3</t>
+  </si>
+  <si>
+    <t>FF1</t>
+  </si>
+  <si>
+    <t>FF5</t>
+  </si>
+  <si>
+    <t>FF6</t>
+  </si>
+  <si>
+    <t>FF4</t>
   </si>
 </sst>
 </file>
@@ -1137,7 +1137,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1149,8 +1149,8 @@
   <dimension ref="A1:J43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F41" sqref="F41"/>
+      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,7 +1168,7 @@
   <sheetData>
     <row r="1" spans="1:10" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>98</v>
@@ -1195,7 +1195,7 @@
         <v>91</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1225,7 +1225,7 @@
         <v>100</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
@@ -1255,7 +1255,7 @@
         <v>83</v>
       </c>
       <c r="J3" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
@@ -1285,7 +1285,7 @@
         <v>100</v>
       </c>
       <c r="J4" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1315,101 +1315,101 @@
         <v>100</v>
       </c>
       <c r="J5" s="14" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6" s="9">
+        <v>70</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="C6" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="H6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="J6" s="14" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="9">
         <v>50</v>
       </c>
-      <c r="B6" s="9" t="s">
-        <v>169</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="B7" s="9" t="s">
+        <v>176</v>
+      </c>
+      <c r="C7" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D7" s="10" t="s">
         <v>88</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="E7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="G7" s="12" t="s">
         <v>89</v>
       </c>
-      <c r="H6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="14"/>
-      <c r="J6" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="72" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="H7" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A8" s="9">
         <v>60</v>
       </c>
-      <c r="B7" s="9" t="s">
-        <v>170</v>
-      </c>
-      <c r="C7" s="10" t="s">
+      <c r="B8" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="C8" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D8" s="10" t="s">
         <v>32</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="E8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="G8" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="J7" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
-        <v>70</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>168</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="E8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="10" t="s">
-        <v>90</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>38</v>
-      </c>
       <c r="H8" s="13" t="s">
         <v>19</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="J8" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1436,7 +1436,7 @@
         <v>19</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="J9" s="14" t="s">
         <v>18</v>
@@ -1469,7 +1469,7 @@
         <v>92</v>
       </c>
       <c r="J10" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="11" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1496,56 +1496,56 @@
         <v>18</v>
       </c>
       <c r="I11" s="14" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="J11" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A12" s="9">
-        <v>110</v>
+        <v>120</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>93</v>
+        <v>166</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>95</v>
+        <v>50</v>
       </c>
       <c r="E12" s="11" t="s">
         <v>18</v>
       </c>
       <c r="F12" s="10" t="s">
-        <v>94</v>
+        <v>99</v>
       </c>
       <c r="G12" s="12" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="H12" s="13" t="s">
         <v>19</v>
       </c>
       <c r="I12" s="14" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="J12" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A13" s="9">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>173</v>
+        <v>179</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>155</v>
+        <v>93</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>156</v>
+        <v>95</v>
       </c>
       <c r="E13" s="11" t="s">
         <v>18</v>
@@ -1554,46 +1554,46 @@
         <v>94</v>
       </c>
       <c r="G13" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="H13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="I13" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="J13" s="14" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="9">
+        <v>115</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>154</v>
+      </c>
+      <c r="D14" s="10" t="s">
+        <v>155</v>
+      </c>
+      <c r="E14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>57</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="14"/>
-      <c r="J13" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
-        <v>120</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>171</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>167</v>
-      </c>
-      <c r="D14" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="E14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="10" t="s">
-        <v>99</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>51</v>
-      </c>
       <c r="H14" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I14" s="14" t="s">
-        <v>178</v>
-      </c>
+      <c r="I14" s="14"/>
       <c r="J14" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1661,13 +1661,13 @@
         <v>150</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C17" s="10" t="s">
         <v>4</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="E17" s="11" t="s">
         <v>19</v>
@@ -1683,7 +1683,7 @@
       </c>
       <c r="I17" s="14"/>
       <c r="J17" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1722,16 +1722,16 @@
       </c>
       <c r="B19" s="9"/>
       <c r="C19" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D19" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="D19" s="10" t="s">
+      <c r="E19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="10" t="s">
         <v>150</v>
-      </c>
-      <c r="E19" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="10" t="s">
-        <v>151</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>57</v>
@@ -1744,24 +1744,24 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
-        <v>170</v>
+        <v>190</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F20" s="10" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
       <c r="G20" s="12" t="s">
         <v>62</v>
@@ -1769,11 +1769,9 @@
       <c r="H20" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I20" s="14" t="s">
-        <v>132</v>
-      </c>
+      <c r="I20" s="14"/>
       <c r="J20" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1800,30 +1798,30 @@
         <v>18</v>
       </c>
       <c r="I21" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J21" s="14" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" ht="72" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="B22" s="19" t="s">
         <v>158</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>62</v>
@@ -1831,9 +1829,11 @@
       <c r="H22" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I22" s="14"/>
+      <c r="I22" s="14" t="s">
+        <v>131</v>
+      </c>
       <c r="J22" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -1860,7 +1860,7 @@
         <v>18</v>
       </c>
       <c r="I23" s="14" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="J23" s="14" t="s">
         <v>18</v>
@@ -1890,7 +1890,7 @@
         <v>18</v>
       </c>
       <c r="I24" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="J24" s="14" t="s">
         <v>18</v>
@@ -1901,7 +1901,7 @@
         <v>220</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>11</v>
@@ -1923,7 +1923,7 @@
       </c>
       <c r="I25" s="14"/>
       <c r="J25" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
@@ -1931,7 +1931,7 @@
         <v>230</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>110</v>
@@ -1953,7 +1953,7 @@
       </c>
       <c r="I26" s="14"/>
       <c r="J26" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -1980,7 +1980,7 @@
         <v>18</v>
       </c>
       <c r="I27" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="J27" s="14" t="s">
         <v>18</v>
@@ -1988,34 +1988,32 @@
     </row>
     <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
-        <v>250</v>
+        <v>360</v>
       </c>
       <c r="B28" s="19" t="s">
+        <v>161</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>175</v>
       </c>
-      <c r="C28" s="10" t="s">
-        <v>106</v>
-      </c>
       <c r="D28" s="10" t="s">
-        <v>107</v>
+        <v>169</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F28" s="10" t="s">
-        <v>112</v>
+        <v>144</v>
       </c>
       <c r="G28" s="12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="H28" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I28" s="14" t="s">
-        <v>180</v>
-      </c>
+      <c r="I28" s="14"/>
       <c r="J28" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2042,7 +2040,7 @@
         <v>18</v>
       </c>
       <c r="I29" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J29" s="14" t="s">
         <v>18</v>
@@ -2103,7 +2101,7 @@
       </c>
       <c r="I31" s="14"/>
       <c r="J31" s="14" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
@@ -2141,19 +2139,19 @@
         <v>295</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C33" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="D33" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="D33" s="10" t="s">
+      <c r="E33" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="10" t="s">
         <v>147</v>
-      </c>
-      <c r="E33" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>148</v>
       </c>
       <c r="G33" s="12" t="s">
         <v>57</v>
@@ -2163,7 +2161,7 @@
       </c>
       <c r="I33" s="14"/>
       <c r="J33" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
@@ -2171,7 +2169,7 @@
         <v>300</v>
       </c>
       <c r="B34" s="19" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="C34" s="10" t="s">
         <v>122</v>
@@ -2193,7 +2191,7 @@
       </c>
       <c r="I34" s="14"/>
       <c r="J34" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
@@ -2220,7 +2218,7 @@
         <v>18</v>
       </c>
       <c r="I35" s="14" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="J35" s="14" t="s">
         <v>18</v>
@@ -2250,7 +2248,7 @@
         <v>18</v>
       </c>
       <c r="I36" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J36" s="14" t="s">
         <v>18</v>
@@ -2280,7 +2278,7 @@
         <v>18</v>
       </c>
       <c r="I37" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J37" s="14" t="s">
         <v>18</v>
@@ -2310,7 +2308,7 @@
         <v>18</v>
       </c>
       <c r="I38" s="14" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="J38" s="14" t="s">
         <v>18</v>
@@ -2340,7 +2338,7 @@
         <v>18</v>
       </c>
       <c r="I39" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="J39" s="14" t="s">
         <v>18</v>
@@ -2348,98 +2346,100 @@
     </row>
     <row r="40" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40" s="19">
-        <v>360</v>
+        <v>250</v>
       </c>
       <c r="B40" s="19" t="s">
-        <v>162</v>
+        <v>168</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>176</v>
+        <v>107</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>145</v>
+        <v>112</v>
       </c>
       <c r="G40" s="12" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="H40" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="I40" s="14"/>
+      <c r="I40" s="14" t="s">
+        <v>173</v>
+      </c>
       <c r="J40" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="18">
-        <v>370</v>
+        <v>380</v>
       </c>
       <c r="B41" s="18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>142</v>
       </c>
       <c r="D41" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F41" s="10" t="s">
         <v>144</v>
-      </c>
-      <c r="E41" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" s="10" t="s">
-        <v>145</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>57</v>
       </c>
       <c r="H41" s="13"/>
-      <c r="I41" s="14" t="s">
-        <v>181</v>
-      </c>
+      <c r="I41" s="14"/>
       <c r="J41" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A42" s="18">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="B42" s="18" t="s">
         <v>164</v>
       </c>
       <c r="C42" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="D42" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="D42" s="10" t="s">
-        <v>141</v>
-      </c>
       <c r="E42" s="11" t="s">
         <v>19</v>
       </c>
       <c r="F42" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G42" s="12" t="s">
         <v>57</v>
       </c>
       <c r="H42" s="13"/>
-      <c r="I42" s="14"/>
+      <c r="I42" s="14" t="s">
+        <v>174</v>
+      </c>
       <c r="J42" s="14" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="115.2" x14ac:dyDescent="0.3">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" ht="123.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="18">
         <v>390</v>
       </c>
       <c r="B43" s="18" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>24</v>
@@ -2451,7 +2451,7 @@
         <v>19</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>81</v>
@@ -2459,7 +2459,7 @@
       <c r="H43" s="13"/>
       <c r="I43" s="14"/>
       <c r="J43" s="14" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2469,6 +2469,9 @@
         <filter val="M"/>
       </filters>
     </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:J43">
+      <sortCondition ref="B1:B43"/>
+    </sortState>
   </autoFilter>
   <conditionalFormatting sqref="E2:E1048576">
     <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Y">

</xml_diff>

<commit_message>
Added column for refs
</commit_message>
<xml_diff>
--- a/TESTCASES/TestCases.xlsx
+++ b/TESTCASES/TestCases.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mike1\Documents\TestCase\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\nsta-nas01.uwe.ac.uk\users3$\ms-joyce\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052D2390-1097-44D2-B8C8-44B5308479FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9EBD205-37E4-4B06-8FE8-C39A3CBCB5D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="503" xr2:uid="{B7A87242-D0EC-4C12-B664-5880765A3370}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$J$43</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$K$43</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="191">
   <si>
     <t>Vertices and attachment points are correct relative to CoR</t>
   </si>
@@ -600,6 +600,36 @@
   </si>
   <si>
     <t>F HS3</t>
+  </si>
+  <si>
+    <t>Ref to similar test</t>
+  </si>
+  <si>
+    <t>Ronchi2013 2.3
+Hunt2016 Component tests 1-12</t>
+  </si>
+  <si>
+    <t>Ronchi2013 2.8</t>
+  </si>
+  <si>
+    <t>Ronchi2013 2.9</t>
+  </si>
+  <si>
+    <t>Hunt2016 Component test 15</t>
+  </si>
+  <si>
+    <t>Ronchi2013 2.3
+Hunt2016 Component tests 1-12
+Hunt2016 Component test 18</t>
+  </si>
+  <si>
+    <t>Hunt2016 Component tests 22</t>
+  </si>
+  <si>
+    <t>Hunt2016 FD 7.7.3</t>
+  </si>
+  <si>
+    <t>Hunt2016 FD 7.7.1 &amp; 7.7.4</t>
   </si>
 </sst>
 </file>
@@ -778,16 +808,6 @@
   <dxfs count="7">
     <dxf>
       <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -843,6 +863,16 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1157,27 +1187,27 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD7B405C-B925-43EB-A348-6C5A23DE5406}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C26" sqref="C26"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="11.33203125" style="2" customWidth="1"/>
-    <col min="3" max="4" width="44.88671875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="12" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="28.5546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="28.33203125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="13.88671875" style="2" customWidth="1"/>
-    <col min="9" max="9" width="20.88671875" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.5546875" style="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="1"/>
+    <col min="1" max="2" width="11.28515625" style="2" customWidth="1"/>
+    <col min="3" max="5" width="44.85546875" style="4" customWidth="1"/>
+    <col min="6" max="6" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="28.5703125" style="4" customWidth="1"/>
+    <col min="8" max="8" width="28.28515625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="13.85546875" style="2" customWidth="1"/>
+    <col min="10" max="10" width="20.85546875" style="1" customWidth="1"/>
+    <col min="11" max="11" width="12.5703125" style="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="3" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>138</v>
       </c>
@@ -1191,25 +1221,28 @@
         <v>15</v>
       </c>
       <c r="E1" s="8" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>44</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="I1" s="7" t="s">
         <v>81</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="J1" s="7" t="s">
         <v>90</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" s="9">
         <v>10</v>
       </c>
@@ -1220,26 +1253,27 @@
       <c r="D2" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="E2" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="15" t="s">
+      <c r="E2" s="15"/>
+      <c r="F2" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="H2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="H2" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="14" t="s">
+      <c r="I2" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J2" s="14" t="s">
+      <c r="K2" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="86.4" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="90" hidden="1" x14ac:dyDescent="0.25">
       <c r="A3" s="9">
         <v>20</v>
       </c>
@@ -1250,26 +1284,27 @@
       <c r="D3" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="E3" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="10" t="s">
+      <c r="E3" s="10"/>
+      <c r="F3" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="H3" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I3" s="14" t="s">
+      <c r="I3" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="J3" s="14" t="s">
+      <c r="K3" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="57.6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A4" s="9">
         <v>30</v>
       </c>
@@ -1280,26 +1315,27 @@
       <c r="D4" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="E4" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="15" t="s">
+      <c r="E4" s="15"/>
+      <c r="F4" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="H4" s="17" t="s">
         <v>85</v>
       </c>
-      <c r="H4" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="K4" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9">
         <v>40</v>
       </c>
@@ -1310,26 +1346,27 @@
       <c r="D5" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="E5" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="15" t="s">
+      <c r="E5" s="15"/>
+      <c r="F5" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="H5" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="H5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="K5" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="9">
         <v>70</v>
       </c>
@@ -1342,26 +1379,27 @@
       <c r="D6" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="E6" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="10" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="G6" s="12" t="s">
+      <c r="H6" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="14" t="s">
         <v>157</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="K6" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="9">
         <v>50</v>
       </c>
@@ -1374,24 +1412,25 @@
       <c r="D7" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="E7" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="10" t="s">
+      <c r="E7" s="10"/>
+      <c r="F7" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G7" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="12" t="s">
+      <c r="H7" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="H7" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I7" s="14"/>
-      <c r="J7" s="14" t="s">
+      <c r="I7" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A8" s="9">
         <v>60</v>
       </c>
@@ -1404,26 +1443,27 @@
       <c r="D8" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="E8" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" s="10" t="s">
+      <c r="E8" s="10"/>
+      <c r="F8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="H8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="K8" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>80</v>
       </c>
@@ -1434,26 +1474,27 @@
       <c r="D9" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="10" t="s">
+      <c r="E9" s="10"/>
+      <c r="F9" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G9" s="10" t="s">
         <v>89</v>
       </c>
-      <c r="G9" s="12" t="s">
+      <c r="H9" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="H9" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="14" t="s">
         <v>128</v>
       </c>
-      <c r="J9" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K9" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>90</v>
       </c>
@@ -1464,26 +1505,27 @@
       <c r="D10" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="10" t="s">
+      <c r="E10" s="10"/>
+      <c r="F10" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" s="10" t="s">
         <v>95</v>
       </c>
-      <c r="G10" s="12" t="s">
+      <c r="H10" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="H10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="K10" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>100</v>
       </c>
@@ -1494,26 +1536,27 @@
       <c r="D11" s="15" t="s">
         <v>86</v>
       </c>
-      <c r="E11" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F11" s="15" t="s">
+      <c r="E11" s="15"/>
+      <c r="F11" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G11" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="H11" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I11" s="14" t="s">
+      <c r="I11" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J11" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="J11" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="K11" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>120</v>
       </c>
@@ -1526,26 +1569,27 @@
       <c r="D12" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E12" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F12" s="10" t="s">
+      <c r="E12" s="10"/>
+      <c r="F12" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>98</v>
       </c>
-      <c r="G12" s="12" t="s">
+      <c r="H12" s="12" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I12" s="14" t="s">
+      <c r="I12" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J12" s="14" t="s">
         <v>158</v>
       </c>
-      <c r="J12" s="14" t="s">
+      <c r="K12" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>110</v>
       </c>
@@ -1558,26 +1602,29 @@
       <c r="D13" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="E13" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F13" s="10" t="s">
+      <c r="E13" s="10" t="s">
+        <v>187</v>
+      </c>
+      <c r="F13" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="G13" s="12" t="s">
+      <c r="H13" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="14" t="s">
+      <c r="I13" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J13" s="14" t="s">
         <v>159</v>
       </c>
-      <c r="J13" s="14" t="s">
+      <c r="K13" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>115</v>
       </c>
@@ -1590,24 +1637,27 @@
       <c r="D14" s="10" t="s">
         <v>154</v>
       </c>
-      <c r="E14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F14" s="10" t="s">
+      <c r="E14" s="10" t="s">
+        <v>183</v>
+      </c>
+      <c r="F14" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="G14" s="12" t="s">
+      <c r="H14" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H14" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14" t="s">
+      <c r="I14" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="14"/>
+      <c r="K14" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9">
         <v>130</v>
       </c>
@@ -1618,26 +1668,27 @@
       <c r="D15" s="15" t="s">
         <v>58</v>
       </c>
-      <c r="E15" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F15" s="15" t="s">
+      <c r="E15" s="15"/>
+      <c r="F15" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="15" t="s">
         <v>96</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="H15" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H15" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I15" s="14" t="s">
+      <c r="I15" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J15" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K15" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9">
         <v>140</v>
       </c>
@@ -1648,26 +1699,27 @@
       <c r="D16" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F16" s="15" t="s">
+      <c r="E16" s="15"/>
+      <c r="F16" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G16" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="H16" s="17" t="s">
         <v>53</v>
       </c>
-      <c r="H16" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I16" s="14" t="s">
+      <c r="I16" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J16" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="K16" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A17" s="19">
         <v>150</v>
       </c>
@@ -1680,24 +1732,27 @@
       <c r="D17" s="10" t="s">
         <v>127</v>
       </c>
-      <c r="E17" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F17" s="10" t="s">
+      <c r="E17" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F17" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="10" t="s">
         <v>55</v>
       </c>
-      <c r="G17" s="12" t="s">
+      <c r="H17" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H17" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14" t="s">
+      <c r="I17" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="14"/>
+      <c r="K17" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9">
         <v>160</v>
       </c>
@@ -1708,26 +1763,27 @@
       <c r="D18" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="E18" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F18" s="15" t="s">
+      <c r="E18" s="15"/>
+      <c r="F18" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="H18" s="17" t="s">
         <v>56</v>
       </c>
-      <c r="H18" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I18" s="14" t="s">
+      <c r="I18" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J18" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K18" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" s="9">
         <v>165</v>
       </c>
@@ -1738,24 +1794,25 @@
       <c r="D19" s="10" t="s">
         <v>148</v>
       </c>
-      <c r="E19" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F19" s="10" t="s">
+      <c r="E19" s="10"/>
+      <c r="F19" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G19" s="10" t="s">
         <v>149</v>
       </c>
-      <c r="G19" s="12" t="s">
+      <c r="H19" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H19" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I19" s="14"/>
-      <c r="J19" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="I19" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J19" s="14"/>
+      <c r="K19" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A20" s="19">
         <v>190</v>
       </c>
@@ -1768,24 +1825,27 @@
       <c r="D20" s="10" t="s">
         <v>123</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F20" s="10" t="s">
+      <c r="E20" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F20" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G20" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="G20" s="12" t="s">
+      <c r="H20" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H20" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" s="14"/>
-      <c r="J20" s="14" t="s">
+      <c r="I20" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J20" s="14"/>
+      <c r="K20" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9">
         <v>180</v>
       </c>
@@ -1796,26 +1856,27 @@
       <c r="D21" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E21" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F21" s="15" t="s">
+      <c r="E21" s="15"/>
+      <c r="F21" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G21" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="H21" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="H21" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I21" s="14" t="s">
+      <c r="I21" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="J21" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="72" x14ac:dyDescent="0.3">
+      <c r="K21" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A22" s="19">
         <v>170</v>
       </c>
@@ -1828,26 +1889,29 @@
       <c r="D22" s="10" t="s">
         <v>122</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="10" t="s">
+      <c r="E22" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="G22" s="12" t="s">
+      <c r="H22" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H22" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I22" s="14" t="s">
+      <c r="I22" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J22" s="14" t="s">
         <v>130</v>
       </c>
-      <c r="J22" s="14" t="s">
+      <c r="K22" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" s="9">
         <v>200</v>
       </c>
@@ -1858,26 +1922,27 @@
       <c r="D23" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="E23" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F23" s="15" t="s">
+      <c r="E23" s="15"/>
+      <c r="F23" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G23" s="15" t="s">
         <v>102</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="H23" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="H23" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I23" s="14" t="s">
+      <c r="I23" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="14" t="s">
         <v>132</v>
       </c>
-      <c r="J23" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K23" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A24" s="9">
         <v>210</v>
       </c>
@@ -1888,26 +1953,27 @@
       <c r="D24" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="E24" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F24" s="15" t="s">
+      <c r="E24" s="15"/>
+      <c r="F24" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G24" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="H24" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="H24" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I24" s="14" t="s">
+      <c r="I24" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="J24" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="K24" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A25" s="19">
         <v>220</v>
       </c>
@@ -1920,24 +1986,25 @@
       <c r="D25" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F25" s="10" t="s">
+      <c r="E25" s="10"/>
+      <c r="F25" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G25" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="G25" s="12" t="s">
+      <c r="H25" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="H25" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I25" s="14"/>
-      <c r="J25" s="14" t="s">
+      <c r="I25" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A26" s="19">
         <v>230</v>
       </c>
@@ -1950,24 +2017,25 @@
       <c r="D26" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F26" s="10" t="s">
+      <c r="E26" s="10"/>
+      <c r="F26" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="G26" s="12" t="s">
+      <c r="H26" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H26" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14" t="s">
+      <c r="I26" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A27" s="9">
         <v>240</v>
       </c>
@@ -1978,26 +2046,27 @@
       <c r="D27" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="E27" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F27" s="15" t="s">
+      <c r="E27" s="15"/>
+      <c r="F27" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G27" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="H27" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="H27" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I27" s="14" t="s">
+      <c r="I27" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J27" s="14" t="s">
         <v>133</v>
       </c>
-      <c r="J27" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="K27" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="60" x14ac:dyDescent="0.25">
       <c r="A28" s="19">
         <v>250</v>
       </c>
@@ -2010,26 +2079,29 @@
       <c r="D28" s="10" t="s">
         <v>106</v>
       </c>
-      <c r="E28" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F28" s="10" t="s">
+      <c r="E28" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F28" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G28" s="10" t="s">
         <v>111</v>
       </c>
-      <c r="G28" s="12" t="s">
+      <c r="H28" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="H28" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I28" s="14" t="s">
+      <c r="I28" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J28" s="14" t="s">
         <v>160</v>
       </c>
-      <c r="J28" s="14" t="s">
+      <c r="K28" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29" s="9">
         <v>260</v>
       </c>
@@ -2040,26 +2112,27 @@
       <c r="D29" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="E29" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F29" s="15" t="s">
+      <c r="E29" s="15"/>
+      <c r="F29" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G29" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="H29" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="H29" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I29" s="14" t="s">
+      <c r="I29" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J29" s="14" t="s">
         <v>134</v>
       </c>
-      <c r="J29" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K29" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A30" s="9">
         <v>270</v>
       </c>
@@ -2070,26 +2143,27 @@
       <c r="D30" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="E30" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F30" s="15" t="s">
+      <c r="E30" s="15"/>
+      <c r="F30" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G30" s="15" t="s">
         <v>69</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="H30" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="H30" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I30" s="14" t="s">
+      <c r="I30" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J30" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="J30" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K30" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="45" hidden="1" x14ac:dyDescent="0.25">
       <c r="A31" s="9">
         <v>280</v>
       </c>
@@ -2100,24 +2174,25 @@
       <c r="D31" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="E31" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F31" s="10" t="s">
+      <c r="E31" s="10"/>
+      <c r="F31" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G31" s="10" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="12" t="s">
+      <c r="H31" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="H31" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I31" s="14"/>
-      <c r="J31" s="14" t="s">
+      <c r="I31" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A32" s="9">
         <v>290</v>
       </c>
@@ -2128,26 +2203,27 @@
       <c r="D32" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="E32" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="F32" s="15" t="s">
+      <c r="E32" s="15"/>
+      <c r="F32" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G32" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="G32" s="17" t="s">
+      <c r="H32" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="H32" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I32" s="14" t="s">
+      <c r="I32" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J32" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="J32" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="K32" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="18">
         <v>360</v>
       </c>
@@ -2160,24 +2236,27 @@
       <c r="D33" s="10" t="s">
         <v>156</v>
       </c>
-      <c r="E33" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F33" s="10" t="s">
+      <c r="E33" s="10" t="s">
+        <v>188</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G33" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="G33" s="12" t="s">
+      <c r="H33" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H33" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I33" s="14"/>
-      <c r="J33" s="14" t="s">
+      <c r="I33" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:10" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A34" s="18">
         <v>295</v>
       </c>
@@ -2190,24 +2269,27 @@
       <c r="D34" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="E34" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F34" s="10" t="s">
+      <c r="E34" s="10" t="s">
+        <v>185</v>
+      </c>
+      <c r="F34" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G34" s="10" t="s">
         <v>146</v>
       </c>
-      <c r="G34" s="12" t="s">
+      <c r="H34" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H34" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I34" s="14"/>
-      <c r="J34" s="14" t="s">
+      <c r="I34" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="35" spans="1:10" ht="43.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A35" s="9">
         <v>310</v>
       </c>
@@ -2218,26 +2300,27 @@
       <c r="D35" s="15" t="s">
         <v>126</v>
       </c>
-      <c r="E35" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F35" s="15" t="s">
+      <c r="E35" s="15"/>
+      <c r="F35" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G35" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G35" s="17" t="s">
+      <c r="H35" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="H35" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I35" s="14" t="s">
+      <c r="I35" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J35" s="14" t="s">
         <v>135</v>
       </c>
-      <c r="J35" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K35" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A36" s="9">
         <v>320</v>
       </c>
@@ -2248,26 +2331,27 @@
       <c r="D36" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="E36" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F36" s="15" t="s">
+      <c r="E36" s="15"/>
+      <c r="F36" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G36" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="H36" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="H36" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I36" s="14" t="s">
+      <c r="I36" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J36" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="J36" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K36" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9">
         <v>330</v>
       </c>
@@ -2278,26 +2362,27 @@
       <c r="D37" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="E37" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F37" s="15" t="s">
+      <c r="E37" s="15"/>
+      <c r="F37" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G37" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="G37" s="17" t="s">
+      <c r="H37" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="H37" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I37" s="14" t="s">
+      <c r="I37" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J37" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="J37" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K37" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9">
         <v>340</v>
       </c>
@@ -2308,26 +2393,27 @@
       <c r="D38" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="E38" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F38" s="15" t="s">
+      <c r="E38" s="15"/>
+      <c r="F38" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G38" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="G38" s="17" t="s">
+      <c r="H38" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="H38" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I38" s="14" t="s">
+      <c r="I38" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J38" s="14" t="s">
         <v>136</v>
       </c>
-      <c r="J38" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+      <c r="K38" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="30" hidden="1" x14ac:dyDescent="0.25">
       <c r="A39" s="9">
         <v>350</v>
       </c>
@@ -2338,26 +2424,27 @@
       <c r="D39" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="E39" s="16" t="s">
-        <v>19</v>
-      </c>
-      <c r="F39" s="15" t="s">
+      <c r="E39" s="15"/>
+      <c r="F39" s="16" t="s">
+        <v>19</v>
+      </c>
+      <c r="G39" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="G39" s="17" t="s">
+      <c r="H39" s="17" t="s">
         <v>61</v>
       </c>
-      <c r="H39" s="13" t="s">
-        <v>18</v>
-      </c>
-      <c r="I39" s="14" t="s">
+      <c r="I39" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="J39" s="14" t="s">
         <v>137</v>
       </c>
-      <c r="J39" s="14" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="K39" s="14" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="18">
         <v>300</v>
       </c>
@@ -2370,24 +2457,27 @@
       <c r="D40" s="10" t="s">
         <v>125</v>
       </c>
-      <c r="E40" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="F40" s="10" t="s">
+      <c r="E40" s="10" t="s">
+        <v>184</v>
+      </c>
+      <c r="F40" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="G40" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="G40" s="12" t="s">
+      <c r="H40" s="12" t="s">
         <v>119</v>
       </c>
-      <c r="H40" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I40" s="14"/>
-      <c r="J40" s="14" t="s">
+      <c r="I40" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" s="14"/>
+      <c r="K40" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="41" spans="1:10" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="48.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="20">
         <v>380</v>
       </c>
@@ -2400,24 +2490,25 @@
       <c r="D41" s="10" t="s">
         <v>139</v>
       </c>
-      <c r="E41" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F41" s="10" t="s">
+      <c r="E41" s="10"/>
+      <c r="F41" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G41" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="G41" s="12" t="s">
+      <c r="H41" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H41" s="13"/>
-      <c r="I41" s="14" t="s">
+      <c r="I41" s="13"/>
+      <c r="J41" s="14" t="s">
         <v>162</v>
       </c>
-      <c r="J41" s="14" t="s">
+      <c r="K41" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="42" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="20">
         <v>370</v>
       </c>
@@ -2430,24 +2521,27 @@
       <c r="D42" s="10" t="s">
         <v>142</v>
       </c>
-      <c r="E42" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F42" s="10" t="s">
+      <c r="E42" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="F42" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="G42" s="12" t="s">
+      <c r="H42" s="12" t="s">
         <v>56</v>
       </c>
-      <c r="H42" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="I42" s="14"/>
-      <c r="J42" s="14" t="s">
+      <c r="I42" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="43" spans="1:10" ht="263.39999999999998" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="263.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20">
         <v>390</v>
       </c>
@@ -2460,59 +2554,62 @@
       <c r="D43" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="E43" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" s="10" t="s">
+      <c r="E43" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="F43" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G43" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="G43" s="12" t="s">
+      <c r="H43" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="H43" s="13"/>
-      <c r="I43" s="14"/>
-      <c r="J43" s="14" t="s">
+      <c r="I43" s="13"/>
+      <c r="J43" s="14"/>
+      <c r="K43" s="14" t="s">
         <v>152</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J43" xr:uid="{CD7B405C-B925-43EB-A348-6C5A23DE5406}">
-    <filterColumn colId="9">
+  <autoFilter ref="A1:K43" xr:uid="{CD7B405C-B925-43EB-A348-6C5A23DE5406}">
+    <filterColumn colId="10">
       <filters>
         <filter val="M"/>
       </filters>
     </filterColumn>
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:J43">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:K43">
       <sortCondition ref="B1:B43"/>
     </sortState>
   </autoFilter>
   <conditionalFormatting sqref="B2:B43">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="2" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E2:E1048576">
-    <cfRule type="containsText" dxfId="6" priority="7" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",E2)))</formula>
+  <conditionalFormatting sqref="F2:F1048576">
+    <cfRule type="containsText" dxfId="5" priority="7" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",F2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="8" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",E2)))</formula>
+    <cfRule type="containsText" dxfId="4" priority="8" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",F2)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H1:H1048576">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="N">
-      <formula>NOT(ISERROR(SEARCH("N",H1)))</formula>
+  <conditionalFormatting sqref="I1:I1048576">
+    <cfRule type="containsText" dxfId="3" priority="3" operator="containsText" text="N">
+      <formula>NOT(ISERROR(SEARCH("N",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H2:H43">
-    <cfRule type="containsText" dxfId="3" priority="1" operator="containsText" text="R">
-      <formula>NOT(ISERROR(SEARCH("R",H2)))</formula>
+  <conditionalFormatting sqref="I2:I43">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="R">
+      <formula>NOT(ISERROR(SEARCH("R",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="2" priority="4" operator="containsText" text="P">
-      <formula>NOT(ISERROR(SEARCH("P",H2)))</formula>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="P">
+      <formula>NOT(ISERROR(SEARCH("P",I2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="5" operator="containsText" text="Y">
-      <formula>NOT(ISERROR(SEARCH("Y",H2)))</formula>
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="Y">
+      <formula>NOT(ISERROR(SEARCH("Y",I2)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>